<commit_message>
chỉnh sửa file Plan của dự án
</commit_message>
<xml_diff>
--- a/Document/sale_project v2011.08.20.xlsx
+++ b/Document/sale_project v2011.08.20.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,14 +11,14 @@
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan!$A$9:$BC$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan!$A$9:$BC$68</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
   <si>
     <t>STT</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>Trang chủ</t>
+  </si>
+  <si>
+    <t>Giao diện các trang danh mục</t>
+  </si>
+  <si>
+    <t>Hung</t>
+  </si>
+  <si>
+    <t>TuND</t>
+  </si>
+  <si>
+    <t>MinhNN</t>
   </si>
 </sst>
 </file>
@@ -437,9 +449,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -451,11 +460,14 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="76">
     <dxf>
       <font>
         <color theme="0"/>
@@ -476,6 +488,33 @@
         <color theme="0"/>
       </font>
       <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
         <gradientFill>
           <stop position="0">
             <color rgb="FF0000CC"/>
@@ -518,33 +557,6 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
         <gradientFill>
           <stop position="0">
             <color rgb="FF0000CC"/>
@@ -560,6 +572,33 @@
         <color theme="0"/>
       </font>
       <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
         <gradientFill>
           <stop position="0">
             <color rgb="FF0000CC"/>
@@ -595,6 +634,273 @@
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
       </fill>
     </dxf>
     <dxf>
@@ -1270,20 +1576,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1534,13 +1840,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC67"/>
+  <dimension ref="A1:BC68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1555,73 +1861,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55">
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:55">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="23">
-        <f>SUMIF($D$9:$D$63,C2,$E$9:$E$63)</f>
-        <v>3</v>
-      </c>
-      <c r="E2" s="23"/>
+      <c r="D2" s="22">
+        <f>SUMIF($D$9:$D$64,C2,$E$9:$E$64)</f>
+        <v>5</v>
+      </c>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:55">
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="23">
-        <f t="shared" ref="D3:D7" si="0">SUMIF($D$9:$D$63,C3,$E$9:$E$63)</f>
-        <v>11</v>
-      </c>
-      <c r="E3" s="23"/>
+      <c r="D3" s="22">
+        <f t="shared" ref="D3:D7" si="0">SUMIF($D$9:$D$64,C3,$E$9:$E$64)</f>
+        <v>12</v>
+      </c>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:55">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E4" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:55">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="1:55">
+      <c r="C6" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="22">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:55">
+      <c r="C7" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="22">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:55">
-      <c r="C6" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="23">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:55">
-      <c r="C7" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="23">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:55" s="16" customFormat="1" ht="30">
       <c r="B8" s="15" t="s">
@@ -1860,11 +2166,11 @@
         <v>3</v>
       </c>
       <c r="F10" s="11">
-        <f>IFERROR( HLOOKUP("BE",I10:BC$67,$A$67-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("B",I10:BC$67,$A$67-$A10+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I10:BC$68,$A$68-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("B",I10:BC$68,$A$68-$A10+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G10" s="11">
-        <f>IFERROR( HLOOKUP("BE",I10:BC$67,$A$67-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("E",I10:BC$67,$A$67-$A10+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I10:BC$68,$A$68-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("E",I10:BC$68,$A$68-$A10+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H10" s="10"/>
@@ -1943,11 +2249,11 @@
         <v>3</v>
       </c>
       <c r="F11" s="11">
-        <f>IFERROR( HLOOKUP("BE",I11:BC$67,$A$67-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",I11:BC$67,$A$67-$A11+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I11:BC$68,$A$68-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",I11:BC$68,$A$68-$A11+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G11" s="11">
-        <f>IFERROR( HLOOKUP("BE",I11:BC$67,$A$67-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",I11:BC$67,$A$67-$A11+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I11:BC$68,$A$68-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",I11:BC$68,$A$68-$A11+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H11" s="10"/>
@@ -2016,11 +2322,11 @@
         <v>1</v>
       </c>
       <c r="F12" s="11">
-        <f>IFERROR( HLOOKUP("BE",I12:BC$67,$A$67-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("B",I12:BC$67,$A$67-$A12+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I12:BC$68,$A$68-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("B",I12:BC$68,$A$68-$A12+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G12" s="11">
-        <f>IFERROR( HLOOKUP("BE",I12:BC$67,$A$67-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("E",I12:BC$67,$A$67-$A12+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I12:BC$68,$A$68-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("E",I12:BC$68,$A$68-$A12+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H12" s="10"/>
@@ -2135,76 +2441,76 @@
       <c r="BB13" s="13"/>
       <c r="BC13" s="13"/>
     </row>
-    <row r="14" spans="1:55" s="29" customFormat="1">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25" t="s">
+    <row r="14" spans="1:55" s="28" customFormat="1">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="25">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26">
-        <f>IFERROR( HLOOKUP("BE",I14:BC$67,$A$67-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("B",I14:BC$67,$A$67-$A14+1,FALSE),0)</f>
+      <c r="E14" s="24">
+        <v>2</v>
+      </c>
+      <c r="F14" s="25">
+        <f>IFERROR( HLOOKUP("BE",I14:BC$68,$A$68-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("B",I14:BC$68,$A$68-$A14+1,FALSE),0)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="26">
-        <f>IFERROR( HLOOKUP("BE",I14:BC$67,$A$67-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("E",I14:BC$67,$A$67-$A14+1,FALSE),0)</f>
+      <c r="G14" s="25">
+        <f>IFERROR( HLOOKUP("BE",I14:BC$68,$A$68-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("E",I14:BC$68,$A$68-$A14+1,FALSE),0)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28" t="s">
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
-      <c r="Y14" s="28"/>
-      <c r="Z14" s="28"/>
-      <c r="AA14" s="28"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="28"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
-      <c r="AG14" s="28"/>
-      <c r="AH14" s="28"/>
-      <c r="AI14" s="28"/>
-      <c r="AJ14" s="28"/>
-      <c r="AK14" s="28"/>
-      <c r="AL14" s="28"/>
-      <c r="AM14" s="28"/>
-      <c r="AN14" s="28"/>
-      <c r="AO14" s="28"/>
-      <c r="AP14" s="28"/>
-      <c r="AQ14" s="28"/>
-      <c r="AR14" s="28"/>
-      <c r="AS14" s="28"/>
-      <c r="AT14" s="28"/>
-      <c r="AU14" s="28"/>
-      <c r="AV14" s="28"/>
-      <c r="AW14" s="28"/>
-      <c r="AX14" s="28"/>
-      <c r="AY14" s="28"/>
-      <c r="AZ14" s="28"/>
-      <c r="BA14" s="28"/>
-      <c r="BB14" s="28"/>
-      <c r="BC14" s="28"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
+      <c r="AH14" s="27"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
+      <c r="AK14" s="27"/>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="27"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+      <c r="AR14" s="27"/>
+      <c r="AS14" s="27"/>
+      <c r="AT14" s="27"/>
+      <c r="AU14" s="27"/>
+      <c r="AV14" s="27"/>
+      <c r="AW14" s="27"/>
+      <c r="AX14" s="27"/>
+      <c r="AY14" s="27"/>
+      <c r="AZ14" s="27"/>
+      <c r="BA14" s="27"/>
+      <c r="BB14" s="27"/>
+      <c r="BC14" s="27"/>
     </row>
     <row r="15" spans="1:55" s="14" customFormat="1">
       <c r="A15">
@@ -2282,22 +2588,32 @@
         <v>1</v>
       </c>
       <c r="F16" s="11">
-        <f>IFERROR( HLOOKUP("BE",I16:BC$67,$A$67-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("B",I16:BC$67,$A$67-$A16+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I16:BC$68,$A$68-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("B",I16:BC$68,$A$68-$A16+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G16" s="11">
-        <f>IFERROR( HLOOKUP("BE",I16:BC$67,$A$67-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("E",I16:BC$67,$A$67-$A16+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",I16:BC$68,$A$68-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("E",I16:BC$68,$A$68-$A16+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -2355,22 +2671,32 @@
         <v>1</v>
       </c>
       <c r="F17" s="11">
-        <f>IFERROR( HLOOKUP("BE",I17:BC$67,$A$67-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("B",I17:BC$67,$A$67-$A17+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I17:BC$68,$A$68-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("B",I17:BC$68,$A$68-$A17+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G17" s="11">
-        <f>IFERROR( HLOOKUP("BE",I17:BC$67,$A$67-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("E",I17:BC$67,$A$67-$A17+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",I17:BC$68,$A$68-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("E",I17:BC$68,$A$68-$A17+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -2422,28 +2748,38 @@
         <v>59</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="E18" s="10">
         <v>1</v>
       </c>
       <c r="F18" s="11">
-        <f>IFERROR( HLOOKUP("BE",I18:BC$67,$A$67-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",I18:BC$67,$A$67-$A18+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I18:BC$68,$A$68-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",I18:BC$68,$A$68-$A18+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G18" s="11">
-        <f>IFERROR( HLOOKUP("BE",I18:BC$67,$A$67-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",I18:BC$67,$A$67-$A18+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",I18:BC$68,$A$68-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",I18:BC$68,$A$68-$A18+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -2501,22 +2837,32 @@
         <v>1</v>
       </c>
       <c r="F19" s="11">
-        <f>IFERROR( HLOOKUP("BE",I19:BC$67,$A$67-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",I19:BC$67,$A$67-$A19+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",I19:BC$68,$A$68-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",I19:BC$68,$A$68-$A19+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G19" s="11">
-        <f>IFERROR( HLOOKUP("BE",I19:BC$67,$A$67-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",I19:BC$67,$A$67-$A19+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",I19:BC$68,$A$68-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",I19:BC$68,$A$68-$A19+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="J19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -2574,22 +2920,32 @@
         <v>1</v>
       </c>
       <c r="F20" s="11">
-        <f>IFERROR( HLOOKUP("BE",I20:BC$67,$A$67-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",I20:BC$67,$A$67-$A20+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",I20:BC$68,$A$68-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",I20:BC$68,$A$68-$A20+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G20" s="11">
-        <f>IFERROR( HLOOKUP("BE",I20:BC$67,$A$67-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",I20:BC$67,$A$67-$A20+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",I20:BC$68,$A$68-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",I20:BC$68,$A$68-$A20+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H20" s="10"/>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="J20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -2647,20 +3003,32 @@
         <v>1</v>
       </c>
       <c r="F21" s="11">
-        <f>IFERROR( HLOOKUP("BE",I21:BC$67,$A$67-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",I21:BC$67,$A$67-$A21+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I21:BC$68,$A$68-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",I21:BC$68,$A$68-$A21+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G21" s="11">
-        <f>IFERROR( HLOOKUP("BE",I21:BC$67,$A$67-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",I21:BC$67,$A$67-$A21+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I21:BC$68,$A$68-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",I21:BC$68,$A$68-$A21+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H21" s="10"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -2712,26 +3080,38 @@
         <v>70</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E22" s="10">
         <v>1</v>
       </c>
       <c r="F22" s="11">
-        <f>IFERROR( HLOOKUP("BE",I22:BC$67,$A$67-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",I22:BC$67,$A$67-$A22+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I22:BC$68,$A$68-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",I22:BC$68,$A$68-$A22+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G22" s="11">
-        <f>IFERROR( HLOOKUP("BE",I22:BC$67,$A$67-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",I22:BC$67,$A$67-$A22+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I22:BC$68,$A$68-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",I22:BC$68,$A$68-$A22+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H22" s="10"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -2783,26 +3163,38 @@
         <v>71</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E23" s="10">
         <v>1</v>
       </c>
       <c r="F23" s="11">
-        <f>IFERROR( HLOOKUP("BE",I23:BC$67,$A$67-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("B",I23:BC$67,$A$67-$A23+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I23:BC$68,$A$68-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("B",I23:BC$68,$A$68-$A23+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G23" s="11">
-        <f>IFERROR( HLOOKUP("BE",I23:BC$67,$A$67-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("E",I23:BC$67,$A$67-$A23+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I23:BC$68,$A$68-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("E",I23:BC$68,$A$68-$A23+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H23" s="10"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -2845,141 +3237,139 @@
       <c r="BB23" s="1"/>
       <c r="BC23" s="1"/>
     </row>
-    <row r="24" spans="1:55" s="14" customFormat="1">
+    <row r="24" spans="1:55">
       <c r="A24">
         <v>14</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
-      <c r="AD24" s="13"/>
-      <c r="AE24" s="13"/>
-      <c r="AF24" s="13"/>
-      <c r="AG24" s="13"/>
-      <c r="AH24" s="13"/>
-      <c r="AI24" s="13"/>
-      <c r="AJ24" s="13"/>
-      <c r="AK24" s="13"/>
-      <c r="AL24" s="13"/>
-      <c r="AM24" s="13"/>
-      <c r="AN24" s="13"/>
-      <c r="AO24" s="13"/>
-      <c r="AP24" s="13"/>
-      <c r="AQ24" s="13"/>
-      <c r="AR24" s="13"/>
-      <c r="AS24" s="13"/>
-      <c r="AT24" s="13"/>
-      <c r="AU24" s="13"/>
-      <c r="AV24" s="13"/>
-      <c r="AW24" s="13"/>
-      <c r="AX24" s="13"/>
-      <c r="AY24" s="13"/>
-      <c r="AZ24" s="13"/>
-      <c r="BA24" s="13"/>
-      <c r="BB24" s="13"/>
-      <c r="BC24" s="13"/>
-    </row>
-    <row r="25" spans="1:55">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11">
+        <f>IFERROR( HLOOKUP("BE",I24:BC$68,$A$68-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",I24:BC$68,$A$68-$A24+1,FALSE),0)</f>
+        <v>40773</v>
+      </c>
+      <c r="G24" s="11">
+        <f>IFERROR( HLOOKUP("BE",I24:BC$68,$A$68-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",I24:BC$68,$A$68-$A24+1,FALSE),0)</f>
+        <v>40773</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="1"/>
+      <c r="BB24" s="1"/>
+      <c r="BC24" s="1"/>
+    </row>
+    <row r="25" spans="1:55" s="14" customFormat="1">
       <c r="A25">
         <v>15</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="10">
-        <v>3</v>
-      </c>
-      <c r="F25" s="11">
-        <f>IFERROR( HLOOKUP("BE",I25:BC$67,$A$67-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("B",I25:BC$67,$A$67-$A25+1,FALSE),0)</f>
-        <v>40776</v>
-      </c>
-      <c r="G25" s="11">
-        <f>IFERROR( HLOOKUP("BE",I25:BC$67,$A$67-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("E",I25:BC$67,$A$67-$A25+1,FALSE),0)</f>
-        <v>40777</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="1"/>
-      <c r="AJ25" s="1"/>
-      <c r="AK25" s="1"/>
-      <c r="AL25" s="1"/>
-      <c r="AM25" s="1"/>
-      <c r="AN25" s="1"/>
-      <c r="AO25" s="1"/>
-      <c r="AP25" s="1"/>
-      <c r="AQ25" s="1"/>
-      <c r="AR25" s="1"/>
-      <c r="AS25" s="1"/>
-      <c r="AT25" s="1"/>
-      <c r="AU25" s="1"/>
-      <c r="AV25" s="1"/>
-      <c r="AW25" s="1"/>
-      <c r="AX25" s="1"/>
-      <c r="AY25" s="1"/>
-      <c r="AZ25" s="1"/>
-      <c r="BA25" s="1"/>
-      <c r="BB25" s="1"/>
-      <c r="BC25" s="1"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="13"/>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="13"/>
+      <c r="AH25" s="13"/>
+      <c r="AI25" s="13"/>
+      <c r="AJ25" s="13"/>
+      <c r="AK25" s="13"/>
+      <c r="AL25" s="13"/>
+      <c r="AM25" s="13"/>
+      <c r="AN25" s="13"/>
+      <c r="AO25" s="13"/>
+      <c r="AP25" s="13"/>
+      <c r="AQ25" s="13"/>
+      <c r="AR25" s="13"/>
+      <c r="AS25" s="13"/>
+      <c r="AT25" s="13"/>
+      <c r="AU25" s="13"/>
+      <c r="AV25" s="13"/>
+      <c r="AW25" s="13"/>
+      <c r="AX25" s="13"/>
+      <c r="AY25" s="13"/>
+      <c r="AZ25" s="13"/>
+      <c r="BA25" s="13"/>
+      <c r="BB25" s="13"/>
+      <c r="BC25" s="13"/>
     </row>
     <row r="26" spans="1:55">
       <c r="A26">
@@ -2987,20 +3377,20 @@
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="E26" s="10">
         <v>3</v>
       </c>
       <c r="F26" s="11">
-        <f>IFERROR( HLOOKUP("BE",I26:BC$67,$A$67-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",I26:BC$67,$A$67-$A26+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I26:BC$68,$A$68-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",I26:BC$68,$A$68-$A26+1,FALSE),0)</f>
         <v>40776</v>
       </c>
       <c r="G26" s="11">
-        <f>IFERROR( HLOOKUP("BE",I26:BC$67,$A$67-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",I26:BC$67,$A$67-$A26+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I26:BC$68,$A$68-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",I26:BC$68,$A$68-$A26+1,FALSE),0)</f>
         <v>40777</v>
       </c>
       <c r="H26" s="10"/>
@@ -3062,20 +3452,20 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E27" s="10">
         <v>3</v>
       </c>
       <c r="F27" s="11">
-        <f>IFERROR( HLOOKUP("BE",I27:BC$67,$A$67-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",I27:BC$67,$A$67-$A27+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I27:BC$68,$A$68-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",I27:BC$68,$A$68-$A27+1,FALSE),0)</f>
         <v>40776</v>
       </c>
       <c r="G27" s="11">
-        <f>IFERROR( HLOOKUP("BE",I27:BC$67,$A$67-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",I27:BC$67,$A$67-$A27+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I27:BC$68,$A$68-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",I27:BC$68,$A$68-$A27+1,FALSE),0)</f>
         <v>40777</v>
       </c>
       <c r="H27" s="10"/>
@@ -3136,23 +3526,13 @@
         <v>18</v>
       </c>
       <c r="B28" s="10"/>
-      <c r="C28" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="10">
-        <v>3</v>
-      </c>
-      <c r="F28" s="11">
-        <f>IFERROR( HLOOKUP("BE",I28:BC$67,$A$67-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("B",I28:BC$67,$A$67-$A28+1,FALSE),0)</f>
-        <v>40776</v>
-      </c>
-      <c r="G28" s="11">
-        <f>IFERROR( HLOOKUP("BE",I28:BC$67,$A$67-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("E",I28:BC$67,$A$67-$A28+1,FALSE),0)</f>
-        <v>40777</v>
-      </c>
+      <c r="C28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="10"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3160,12 +3540,8 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -3211,21 +3587,21 @@
         <v>19</v>
       </c>
       <c r="B29" s="10"/>
-      <c r="C29" s="19" t="s">
-        <v>45</v>
+      <c r="C29" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E29" s="10">
         <v>3</v>
       </c>
       <c r="F29" s="11">
-        <f>IFERROR( HLOOKUP("BE",I29:BC$67,$A$67-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",I29:BC$67,$A$67-$A29+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I29:BC$68,$A$68-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",I29:BC$68,$A$68-$A29+1,FALSE),0)</f>
         <v>40776</v>
       </c>
       <c r="G29" s="11">
-        <f>IFERROR( HLOOKUP("BE",I29:BC$67,$A$67-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",I29:BC$67,$A$67-$A29+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I29:BC$68,$A$68-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",I29:BC$68,$A$68-$A29+1,FALSE),0)</f>
         <v>40777</v>
       </c>
       <c r="H29" s="10"/>
@@ -3286,22 +3662,22 @@
         <v>20</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="10" t="s">
-        <v>35</v>
+      <c r="C30" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="E30" s="10">
         <v>3</v>
       </c>
       <c r="F30" s="11">
-        <f>IFERROR( HLOOKUP("BE",I30:BC$67,$A$67-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",I30:BC$67,$A$67-$A30+1,FALSE),0)</f>
-        <v>40778</v>
+        <f>IFERROR( HLOOKUP("BE",I30:BC$68,$A$68-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",I30:BC$68,$A$68-$A30+1,FALSE),0)</f>
+        <v>40776</v>
       </c>
       <c r="G30" s="11">
-        <f>IFERROR( HLOOKUP("BE",I30:BC$67,$A$67-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",I30:BC$67,$A$67-$A30+1,FALSE),0)</f>
-        <v>40779</v>
+        <f>IFERROR( HLOOKUP("BE",I30:BC$68,$A$68-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",I30:BC$68,$A$68-$A30+1,FALSE),0)</f>
+        <v>40777</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="1"/>
@@ -3310,14 +3686,14 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -3361,23 +3737,13 @@
         <v>21</v>
       </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="10">
-        <v>3</v>
-      </c>
-      <c r="F31" s="11">
-        <f>IFERROR( HLOOKUP("BE",I31:BC$67,$A$67-$A31+1,FALSE),0)+ IFERROR( HLOOKUP("B",I31:BC$67,$A$67-$A31+1,FALSE),0)</f>
-        <v>40778</v>
-      </c>
-      <c r="G31" s="11">
-        <f>IFERROR( HLOOKUP("BE",I31:BC$67,$A$67-$A31+1,FALSE),0)+ IFERROR( HLOOKUP("E",I31:BC$67,$A$67-$A31+1,FALSE),0)</f>
-        <v>40779</v>
-      </c>
+      <c r="C31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
       <c r="H31" s="10"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -3387,12 +3753,8 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -3436,21 +3798,21 @@
         <v>22</v>
       </c>
       <c r="B32" s="10"/>
-      <c r="C32" s="19" t="s">
-        <v>47</v>
+      <c r="C32" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E32" s="10">
         <v>3</v>
       </c>
       <c r="F32" s="11">
-        <f>IFERROR( HLOOKUP("BE",I32:BC$67,$A$67-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",I32:BC$67,$A$67-$A32+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I32:BC$68,$A$68-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",I32:BC$68,$A$68-$A32+1,FALSE),0)</f>
         <v>40778</v>
       </c>
       <c r="G32" s="11">
-        <f>IFERROR( HLOOKUP("BE",I32:BC$67,$A$67-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",I32:BC$67,$A$67-$A32+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I32:BC$68,$A$68-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",I32:BC$68,$A$68-$A32+1,FALSE),0)</f>
         <v>40779</v>
       </c>
       <c r="H32" s="10"/>
@@ -3511,21 +3873,21 @@
         <v>23</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="10" t="s">
-        <v>48</v>
+      <c r="C33" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" s="10">
         <v>3</v>
       </c>
       <c r="F33" s="11">
-        <f>IFERROR( HLOOKUP("BE",I33:BC$67,$A$67-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",I33:BC$67,$A$67-$A33+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I33:BC$68,$A$68-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",I33:BC$68,$A$68-$A33+1,FALSE),0)</f>
         <v>40778</v>
       </c>
       <c r="G33" s="11">
-        <f>IFERROR( HLOOKUP("BE",I33:BC$67,$A$67-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",I33:BC$67,$A$67-$A33+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I33:BC$68,$A$68-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",I33:BC$68,$A$68-$A33+1,FALSE),0)</f>
         <v>40779</v>
       </c>
       <c r="H33" s="10"/>
@@ -3587,20 +3949,20 @@
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E34" s="10">
         <v>3</v>
       </c>
       <c r="F34" s="11">
-        <f>IFERROR( HLOOKUP("BE",I34:BC$67,$A$67-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("B",I34:BC$67,$A$67-$A34+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I34:BC$68,$A$68-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("B",I34:BC$68,$A$68-$A34+1,FALSE),0)</f>
         <v>40778</v>
       </c>
       <c r="G34" s="11">
-        <f>IFERROR( HLOOKUP("BE",I34:BC$67,$A$67-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("E",I34:BC$67,$A$67-$A34+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I34:BC$68,$A$68-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("E",I34:BC$68,$A$68-$A34+1,FALSE),0)</f>
         <v>40779</v>
       </c>
       <c r="H34" s="10"/>
@@ -3656,154 +4018,164 @@
       <c r="BB34" s="1"/>
       <c r="BC34" s="1"/>
     </row>
-    <row r="35" spans="1:55" s="14" customFormat="1">
+    <row r="35" spans="1:55">
       <c r="A35">
         <v>25</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13"/>
-      <c r="W35" s="13"/>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="13"/>
-      <c r="AB35" s="13"/>
-      <c r="AC35" s="13"/>
-      <c r="AD35" s="13"/>
-      <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="13"/>
-      <c r="AH35" s="13"/>
-      <c r="AI35" s="13"/>
-      <c r="AJ35" s="13"/>
-      <c r="AK35" s="13"/>
-      <c r="AL35" s="13"/>
-      <c r="AM35" s="13"/>
-      <c r="AN35" s="13"/>
-      <c r="AO35" s="13"/>
-      <c r="AP35" s="13"/>
-      <c r="AQ35" s="13"/>
-      <c r="AR35" s="13"/>
-      <c r="AS35" s="13"/>
-      <c r="AT35" s="13"/>
-      <c r="AU35" s="13"/>
-      <c r="AV35" s="13"/>
-      <c r="AW35" s="13"/>
-      <c r="AX35" s="13"/>
-      <c r="AY35" s="13"/>
-      <c r="AZ35" s="13"/>
-      <c r="BA35" s="13"/>
-      <c r="BB35" s="13"/>
-      <c r="BC35" s="13"/>
-    </row>
-    <row r="36" spans="1:55">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="10">
+        <v>3</v>
+      </c>
+      <c r="F35" s="11">
+        <f>IFERROR( HLOOKUP("BE",I35:BC$68,$A$68-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",I35:BC$68,$A$68-$A35+1,FALSE),0)</f>
+        <v>40778</v>
+      </c>
+      <c r="G35" s="11">
+        <f>IFERROR( HLOOKUP("BE",I35:BC$68,$A$68-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",I35:BC$68,$A$68-$A35+1,FALSE),0)</f>
+        <v>40779</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
+      <c r="AK35" s="1"/>
+      <c r="AL35" s="1"/>
+      <c r="AM35" s="1"/>
+      <c r="AN35" s="1"/>
+      <c r="AO35" s="1"/>
+      <c r="AP35" s="1"/>
+      <c r="AQ35" s="1"/>
+      <c r="AR35" s="1"/>
+      <c r="AS35" s="1"/>
+      <c r="AT35" s="1"/>
+      <c r="AU35" s="1"/>
+      <c r="AV35" s="1"/>
+      <c r="AW35" s="1"/>
+      <c r="AX35" s="1"/>
+      <c r="AY35" s="1"/>
+      <c r="AZ35" s="1"/>
+      <c r="BA35" s="1"/>
+      <c r="BB35" s="1"/>
+      <c r="BC35" s="1"/>
+    </row>
+    <row r="36" spans="1:55" s="14" customFormat="1">
       <c r="A36">
         <v>26</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="10">
-        <v>3</v>
-      </c>
-      <c r="F36" s="11">
-        <f>IFERROR( HLOOKUP("BE",I36:BC$67,$A$67-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("B",I36:BC$67,$A$67-$A36+1,FALSE),0)</f>
-        <v>40780</v>
-      </c>
-      <c r="G36" s="11">
-        <f>IFERROR( HLOOKUP("BE",I36:BC$67,$A$67-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("E",I36:BC$67,$A$67-$A36+1,FALSE),0)</f>
-        <v>40781</v>
-      </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
-      <c r="Z36" s="1"/>
-      <c r="AA36" s="1"/>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="1"/>
-      <c r="AD36" s="1"/>
-      <c r="AE36" s="1"/>
-      <c r="AF36" s="1"/>
-      <c r="AG36" s="1"/>
-      <c r="AH36" s="1"/>
-      <c r="AI36" s="1"/>
-      <c r="AJ36" s="1"/>
-      <c r="AK36" s="1"/>
-      <c r="AL36" s="1"/>
-      <c r="AM36" s="1"/>
-      <c r="AN36" s="1"/>
-      <c r="AO36" s="1"/>
-      <c r="AP36" s="1"/>
-      <c r="AQ36" s="1"/>
-      <c r="AR36" s="1"/>
-      <c r="AS36" s="1"/>
-      <c r="AT36" s="1"/>
-      <c r="AU36" s="1"/>
-      <c r="AV36" s="1"/>
-      <c r="AW36" s="1"/>
-      <c r="AX36" s="1"/>
-      <c r="AY36" s="1"/>
-      <c r="AZ36" s="1"/>
-      <c r="BA36" s="1"/>
-      <c r="BB36" s="1"/>
-      <c r="BC36" s="1"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
+      <c r="AB36" s="13"/>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="13"/>
+      <c r="AF36" s="13"/>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="13"/>
+      <c r="AI36" s="13"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="13"/>
+      <c r="AL36" s="13"/>
+      <c r="AM36" s="13"/>
+      <c r="AN36" s="13"/>
+      <c r="AO36" s="13"/>
+      <c r="AP36" s="13"/>
+      <c r="AQ36" s="13"/>
+      <c r="AR36" s="13"/>
+      <c r="AS36" s="13"/>
+      <c r="AT36" s="13"/>
+      <c r="AU36" s="13"/>
+      <c r="AV36" s="13"/>
+      <c r="AW36" s="13"/>
+      <c r="AX36" s="13"/>
+      <c r="AY36" s="13"/>
+      <c r="AZ36" s="13"/>
+      <c r="BA36" s="13"/>
+      <c r="BB36" s="13"/>
+      <c r="BC36" s="13"/>
     </row>
     <row r="37" spans="1:55">
       <c r="A37">
         <v>27</v>
       </c>
       <c r="B37" s="10"/>
-      <c r="C37" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="C37" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="10">
+        <v>3</v>
+      </c>
+      <c r="F37" s="11">
+        <f>IFERROR( HLOOKUP("BE",I37:BC$68,$A$68-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("B",I37:BC$68,$A$68-$A37+1,FALSE),0)</f>
+        <v>40780</v>
+      </c>
+      <c r="G37" s="11">
+        <f>IFERROR( HLOOKUP("BE",I37:BC$68,$A$68-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("E",I37:BC$68,$A$68-$A37+1,FALSE),0)</f>
+        <v>40781</v>
+      </c>
       <c r="H37" s="10"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -3815,8 +4187,12 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
+      <c r="S37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
@@ -3858,23 +4234,13 @@
         <v>28</v>
       </c>
       <c r="B38" s="10"/>
-      <c r="C38" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="10">
-        <v>3</v>
-      </c>
-      <c r="F38" s="11">
-        <f>IFERROR( HLOOKUP("BE",I38:BC$67,$A$67-$A38+1,FALSE),0)+ IFERROR( HLOOKUP("B",I38:BC$67,$A$67-$A38+1,FALSE),0)</f>
-        <v>40780</v>
-      </c>
-      <c r="G38" s="11">
-        <f>IFERROR( HLOOKUP("BE",I38:BC$67,$A$67-$A38+1,FALSE),0)+ IFERROR( HLOOKUP("E",I38:BC$67,$A$67-$A38+1,FALSE),0)</f>
-        <v>40781</v>
-      </c>
+      <c r="C38" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
       <c r="H38" s="10"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -3886,12 +4252,8 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T38" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
@@ -3933,21 +4295,21 @@
         <v>29</v>
       </c>
       <c r="B39" s="10"/>
-      <c r="C39" s="10" t="s">
-        <v>51</v>
+      <c r="C39" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E39" s="10">
         <v>3</v>
       </c>
       <c r="F39" s="11">
-        <f>IFERROR( HLOOKUP("BE",I39:BC$67,$A$67-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("B",I39:BC$67,$A$67-$A39+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I39:BC$68,$A$68-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("B",I39:BC$68,$A$68-$A39+1,FALSE),0)</f>
         <v>40780</v>
       </c>
       <c r="G39" s="11">
-        <f>IFERROR( HLOOKUP("BE",I39:BC$67,$A$67-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("E",I39:BC$67,$A$67-$A39+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I39:BC$68,$A$68-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("E",I39:BC$68,$A$68-$A39+1,FALSE),0)</f>
         <v>40781</v>
       </c>
       <c r="H39" s="10"/>
@@ -4009,20 +4371,20 @@
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E40" s="10">
         <v>3</v>
       </c>
       <c r="F40" s="11">
-        <f>IFERROR( HLOOKUP("BE",I40:BC$67,$A$67-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("B",I40:BC$67,$A$67-$A40+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I40:BC$68,$A$68-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("B",I40:BC$68,$A$68-$A40+1,FALSE),0)</f>
         <v>40780</v>
       </c>
       <c r="G40" s="11">
-        <f>IFERROR( HLOOKUP("BE",I40:BC$67,$A$67-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("E",I40:BC$67,$A$67-$A40+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I40:BC$68,$A$68-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("E",I40:BC$68,$A$68-$A40+1,FALSE),0)</f>
         <v>40781</v>
       </c>
       <c r="H40" s="10"/>
@@ -4083,13 +4445,23 @@
         <v>31</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="C41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="10">
+        <v>3</v>
+      </c>
+      <c r="F41" s="11">
+        <f>IFERROR( HLOOKUP("BE",I41:BC$68,$A$68-$A41+1,FALSE),0)+ IFERROR( HLOOKUP("B",I41:BC$68,$A$68-$A41+1,FALSE),0)</f>
+        <v>40780</v>
+      </c>
+      <c r="G41" s="11">
+        <f>IFERROR( HLOOKUP("BE",I41:BC$68,$A$68-$A41+1,FALSE),0)+ IFERROR( HLOOKUP("E",I41:BC$68,$A$68-$A41+1,FALSE),0)</f>
+        <v>40781</v>
+      </c>
       <c r="H41" s="10"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -4101,8 +4473,12 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
+      <c r="S41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
@@ -4145,22 +4521,12 @@
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E42" s="10">
-        <v>3</v>
-      </c>
-      <c r="F42" s="11">
-        <f>IFERROR( HLOOKUP("BE",I42:BC$67,$A$67-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("B",I42:BC$67,$A$67-$A42+1,FALSE),0)</f>
-        <v>40782</v>
-      </c>
-      <c r="G42" s="11">
-        <f>IFERROR( HLOOKUP("BE",I42:BC$67,$A$67-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("E",I42:BC$67,$A$67-$A42+1,FALSE),0)</f>
-        <v>40783</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
       <c r="H42" s="10"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -4174,12 +4540,8 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
-      <c r="U42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
@@ -4219,21 +4581,21 @@
         <v>33</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="21" t="s">
-        <v>55</v>
+      <c r="C43" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E43" s="10">
         <v>3</v>
       </c>
       <c r="F43" s="11">
-        <f>IFERROR( HLOOKUP("BE",I43:BC$67,$A$67-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("B",I43:BC$67,$A$67-$A43+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I43:BC$68,$A$68-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("B",I43:BC$68,$A$68-$A43+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G43" s="11">
-        <f>IFERROR( HLOOKUP("BE",I43:BC$67,$A$67-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("E",I43:BC$67,$A$67-$A43+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I43:BC$68,$A$68-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("E",I43:BC$68,$A$68-$A43+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H43" s="10"/>
@@ -4294,21 +4656,21 @@
         <v>34</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="21" t="s">
-        <v>56</v>
+      <c r="C44" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" s="10">
         <v>3</v>
       </c>
       <c r="F44" s="11">
-        <f>IFERROR( HLOOKUP("BE",I44:BC$67,$A$67-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("B",I44:BC$67,$A$67-$A44+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I44:BC$68,$A$68-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("B",I44:BC$68,$A$68-$A44+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G44" s="11">
-        <f>IFERROR( HLOOKUP("BE",I44:BC$67,$A$67-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("E",I44:BC$67,$A$67-$A44+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I44:BC$68,$A$68-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("E",I44:BC$68,$A$68-$A44+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H44" s="10"/>
@@ -4369,21 +4731,21 @@
         <v>35</v>
       </c>
       <c r="B45" s="10"/>
-      <c r="C45" s="21" t="s">
-        <v>57</v>
+      <c r="C45" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E45" s="10">
         <v>3</v>
       </c>
       <c r="F45" s="11">
-        <f>IFERROR( HLOOKUP("BE",I45:BC$67,$A$67-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("B",I45:BC$67,$A$67-$A45+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I45:BC$68,$A$68-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("B",I45:BC$68,$A$68-$A45+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G45" s="11">
-        <f>IFERROR( HLOOKUP("BE",I45:BC$67,$A$67-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("E",I45:BC$67,$A$67-$A45+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I45:BC$68,$A$68-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("E",I45:BC$68,$A$68-$A45+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H45" s="10"/>
@@ -4439,133 +4801,141 @@
       <c r="BB45" s="1"/>
       <c r="BC45" s="1"/>
     </row>
-    <row r="46" spans="1:55" s="14" customFormat="1">
+    <row r="46" spans="1:55">
       <c r="A46">
         <v>36</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="13"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="13"/>
-      <c r="V46" s="13"/>
-      <c r="W46" s="13"/>
-      <c r="X46" s="13"/>
-      <c r="Y46" s="13"/>
-      <c r="Z46" s="13"/>
-      <c r="AA46" s="13"/>
-      <c r="AB46" s="13"/>
-      <c r="AC46" s="13"/>
-      <c r="AD46" s="13"/>
-      <c r="AE46" s="13"/>
-      <c r="AF46" s="13"/>
-      <c r="AG46" s="13"/>
-      <c r="AH46" s="13"/>
-      <c r="AI46" s="13"/>
-      <c r="AJ46" s="13"/>
-      <c r="AK46" s="13"/>
-      <c r="AL46" s="13"/>
-      <c r="AM46" s="13"/>
-      <c r="AN46" s="13"/>
-      <c r="AO46" s="13"/>
-      <c r="AP46" s="13"/>
-      <c r="AQ46" s="13"/>
-      <c r="AR46" s="13"/>
-      <c r="AS46" s="13"/>
-      <c r="AT46" s="13"/>
-      <c r="AU46" s="13"/>
-      <c r="AV46" s="13"/>
-      <c r="AW46" s="13"/>
-      <c r="AX46" s="13"/>
-      <c r="AY46" s="13"/>
-      <c r="AZ46" s="13"/>
-      <c r="BA46" s="13"/>
-      <c r="BB46" s="13"/>
-      <c r="BC46" s="13"/>
-    </row>
-    <row r="47" spans="1:55">
+      <c r="B46" s="10"/>
+      <c r="C46" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="10">
+        <v>3</v>
+      </c>
+      <c r="F46" s="11">
+        <f>IFERROR( HLOOKUP("BE",I46:BC$68,$A$68-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("B",I46:BC$68,$A$68-$A46+1,FALSE),0)</f>
+        <v>40782</v>
+      </c>
+      <c r="G46" s="11">
+        <f>IFERROR( HLOOKUP("BE",I46:BC$68,$A$68-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("E",I46:BC$68,$A$68-$A46+1,FALSE),0)</f>
+        <v>40783</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+      <c r="AF46" s="1"/>
+      <c r="AG46" s="1"/>
+      <c r="AH46" s="1"/>
+      <c r="AI46" s="1"/>
+      <c r="AJ46" s="1"/>
+      <c r="AK46" s="1"/>
+      <c r="AL46" s="1"/>
+      <c r="AM46" s="1"/>
+      <c r="AN46" s="1"/>
+      <c r="AO46" s="1"/>
+      <c r="AP46" s="1"/>
+      <c r="AQ46" s="1"/>
+      <c r="AR46" s="1"/>
+      <c r="AS46" s="1"/>
+      <c r="AT46" s="1"/>
+      <c r="AU46" s="1"/>
+      <c r="AV46" s="1"/>
+      <c r="AW46" s="1"/>
+      <c r="AX46" s="1"/>
+      <c r="AY46" s="1"/>
+      <c r="AZ46" s="1"/>
+      <c r="BA46" s="1"/>
+      <c r="BB46" s="1"/>
+      <c r="BC46" s="1"/>
+    </row>
+    <row r="47" spans="1:55" s="14" customFormat="1">
       <c r="A47">
         <v>37</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="11">
-        <f>IFERROR( HLOOKUP("BE",I47:BC$67,$A$67-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("B",I47:BC$67,$A$67-$A47+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="11">
-        <f>IFERROR( HLOOKUP("BE",I47:BC$67,$A$67-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("E",I47:BC$67,$A$67-$A47+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="10"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
-      <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
-      <c r="AA47" s="1"/>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="1"/>
-      <c r="AD47" s="1"/>
-      <c r="AE47" s="1"/>
-      <c r="AF47" s="1"/>
-      <c r="AG47" s="1"/>
-      <c r="AH47" s="1"/>
-      <c r="AI47" s="1"/>
-      <c r="AJ47" s="1"/>
-      <c r="AK47" s="1"/>
-      <c r="AL47" s="1"/>
-      <c r="AM47" s="1"/>
-      <c r="AN47" s="1"/>
-      <c r="AO47" s="1"/>
-      <c r="AP47" s="1"/>
-      <c r="AQ47" s="1"/>
-      <c r="AR47" s="1"/>
-      <c r="AS47" s="1"/>
-      <c r="AT47" s="1"/>
-      <c r="AU47" s="1"/>
-      <c r="AV47" s="1"/>
-      <c r="AW47" s="1"/>
-      <c r="AX47" s="1"/>
-      <c r="AY47" s="1"/>
-      <c r="AZ47" s="1"/>
-      <c r="BA47" s="1"/>
-      <c r="BB47" s="1"/>
-      <c r="BC47" s="1"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="13"/>
+      <c r="AC47" s="13"/>
+      <c r="AD47" s="13"/>
+      <c r="AE47" s="13"/>
+      <c r="AF47" s="13"/>
+      <c r="AG47" s="13"/>
+      <c r="AH47" s="13"/>
+      <c r="AI47" s="13"/>
+      <c r="AJ47" s="13"/>
+      <c r="AK47" s="13"/>
+      <c r="AL47" s="13"/>
+      <c r="AM47" s="13"/>
+      <c r="AN47" s="13"/>
+      <c r="AO47" s="13"/>
+      <c r="AP47" s="13"/>
+      <c r="AQ47" s="13"/>
+      <c r="AR47" s="13"/>
+      <c r="AS47" s="13"/>
+      <c r="AT47" s="13"/>
+      <c r="AU47" s="13"/>
+      <c r="AV47" s="13"/>
+      <c r="AW47" s="13"/>
+      <c r="AX47" s="13"/>
+      <c r="AY47" s="13"/>
+      <c r="AZ47" s="13"/>
+      <c r="BA47" s="13"/>
+      <c r="BB47" s="13"/>
+      <c r="BC47" s="13"/>
     </row>
     <row r="48" spans="1:55">
       <c r="A48">
@@ -4573,21 +4943,27 @@
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="10">
+        <v>2</v>
+      </c>
       <c r="F48" s="11">
-        <f>IFERROR( HLOOKUP("BE",I48:BC$67,$A$67-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("B",I48:BC$67,$A$67-$A48+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I48:BC$68,$A$68-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("B",I48:BC$68,$A$68-$A48+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="G48" s="11">
-        <f>IFERROR( HLOOKUP("BE",I48:BC$67,$A$67-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("E",I48:BC$67,$A$67-$A48+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I48:BC$68,$A$68-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("E",I48:BC$68,$A$68-$A48+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
+      <c r="J48" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -4639,24 +5015,40 @@
         <v>39</v>
       </c>
       <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
+      <c r="C49" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
       <c r="F49" s="11">
-        <f>IFERROR( HLOOKUP("BE",I49:BC$67,$A$67-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("B",I49:BC$67,$A$67-$A49+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I49:BC$68,$A$68-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("B",I49:BC$68,$A$68-$A49+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="G49" s="11">
-        <f>IFERROR( HLOOKUP("BE",I49:BC$67,$A$67-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("E",I49:BC$67,$A$67-$A49+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I49:BC$68,$A$68-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("E",I49:BC$68,$A$68-$A49+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="J49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -4708,11 +5100,11 @@
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="11">
-        <f>IFERROR( HLOOKUP("BE",I50:BC$67,$A$67-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("B",I50:BC$67,$A$67-$A50+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I50:BC$68,$A$68-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("B",I50:BC$68,$A$68-$A50+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G50" s="11">
-        <f>IFERROR( HLOOKUP("BE",I50:BC$67,$A$67-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("E",I50:BC$67,$A$67-$A50+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I50:BC$68,$A$68-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("E",I50:BC$68,$A$68-$A50+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H50" s="10"/>
@@ -4773,11 +5165,11 @@
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="11">
-        <f>IFERROR( HLOOKUP("BE",I51:BC$67,$A$67-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("B",I51:BC$67,$A$67-$A51+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I51:BC$68,$A$68-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("B",I51:BC$68,$A$68-$A51+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G51" s="11">
-        <f>IFERROR( HLOOKUP("BE",I51:BC$67,$A$67-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("E",I51:BC$67,$A$67-$A51+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I51:BC$68,$A$68-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("E",I51:BC$68,$A$68-$A51+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H51" s="10"/>
@@ -4838,11 +5230,11 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="11">
-        <f>IFERROR( HLOOKUP("BE",I52:BC$67,$A$67-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("B",I52:BC$67,$A$67-$A52+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I52:BC$68,$A$68-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("B",I52:BC$68,$A$68-$A52+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G52" s="11">
-        <f>IFERROR( HLOOKUP("BE",I52:BC$67,$A$67-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("E",I52:BC$67,$A$67-$A52+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I52:BC$68,$A$68-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("E",I52:BC$68,$A$68-$A52+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H52" s="10"/>
@@ -4903,11 +5295,11 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="11">
-        <f>IFERROR( HLOOKUP("BE",I53:BC$67,$A$67-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("B",I53:BC$67,$A$67-$A53+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I53:BC$68,$A$68-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("B",I53:BC$68,$A$68-$A53+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G53" s="11">
-        <f>IFERROR( HLOOKUP("BE",I53:BC$67,$A$67-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("E",I53:BC$67,$A$67-$A53+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I53:BC$68,$A$68-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("E",I53:BC$68,$A$68-$A53+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H53" s="10"/>
@@ -4968,11 +5360,11 @@
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="11">
-        <f>IFERROR( HLOOKUP("BE",I54:BC$67,$A$67-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("B",I54:BC$67,$A$67-$A54+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I54:BC$68,$A$68-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("B",I54:BC$68,$A$68-$A54+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G54" s="11">
-        <f>IFERROR( HLOOKUP("BE",I54:BC$67,$A$67-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("E",I54:BC$67,$A$67-$A54+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I54:BC$68,$A$68-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("E",I54:BC$68,$A$68-$A54+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H54" s="10"/>
@@ -5033,11 +5425,11 @@
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="11">
-        <f>IFERROR( HLOOKUP("BE",I55:BC$67,$A$67-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("B",I55:BC$67,$A$67-$A55+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I55:BC$68,$A$68-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("B",I55:BC$68,$A$68-$A55+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G55" s="11">
-        <f>IFERROR( HLOOKUP("BE",I55:BC$67,$A$67-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("E",I55:BC$67,$A$67-$A55+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I55:BC$68,$A$68-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("E",I55:BC$68,$A$68-$A55+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H55" s="10"/>
@@ -5098,11 +5490,11 @@
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
       <c r="F56" s="11">
-        <f>IFERROR( HLOOKUP("BE",I56:BC$67,$A$67-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("B",I56:BC$67,$A$67-$A56+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I56:BC$68,$A$68-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("B",I56:BC$68,$A$68-$A56+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G56" s="11">
-        <f>IFERROR( HLOOKUP("BE",I56:BC$67,$A$67-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("E",I56:BC$67,$A$67-$A56+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I56:BC$68,$A$68-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("E",I56:BC$68,$A$68-$A56+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H56" s="10"/>
@@ -5163,11 +5555,11 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="11">
-        <f>IFERROR( HLOOKUP("BE",I57:BC$67,$A$67-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("B",I57:BC$67,$A$67-$A57+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I57:BC$68,$A$68-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("B",I57:BC$68,$A$68-$A57+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G57" s="11">
-        <f>IFERROR( HLOOKUP("BE",I57:BC$67,$A$67-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("E",I57:BC$67,$A$67-$A57+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I57:BC$68,$A$68-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("E",I57:BC$68,$A$68-$A57+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H57" s="10"/>
@@ -5228,11 +5620,11 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="11">
-        <f>IFERROR( HLOOKUP("BE",I58:BC$67,$A$67-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("B",I58:BC$67,$A$67-$A58+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I58:BC$68,$A$68-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("B",I58:BC$68,$A$68-$A58+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G58" s="11">
-        <f>IFERROR( HLOOKUP("BE",I58:BC$67,$A$67-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("E",I58:BC$67,$A$67-$A58+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I58:BC$68,$A$68-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("E",I58:BC$68,$A$68-$A58+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H58" s="10"/>
@@ -5293,11 +5685,11 @@
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="11">
-        <f>IFERROR( HLOOKUP("BE",I59:BC$67,$A$67-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",I59:BC$67,$A$67-$A59+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I59:BC$68,$A$68-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",I59:BC$68,$A$68-$A59+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G59" s="11">
-        <f>IFERROR( HLOOKUP("BE",I59:BC$67,$A$67-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",I59:BC$67,$A$67-$A59+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I59:BC$68,$A$68-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",I59:BC$68,$A$68-$A59+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H59" s="10"/>
@@ -5358,11 +5750,11 @@
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="11">
-        <f>IFERROR( HLOOKUP("BE",I60:BC$67,$A$67-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("B",I60:BC$67,$A$67-$A60+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I60:BC$68,$A$68-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("B",I60:BC$68,$A$68-$A60+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G60" s="11">
-        <f>IFERROR( HLOOKUP("BE",I60:BC$67,$A$67-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("E",I60:BC$67,$A$67-$A60+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I60:BC$68,$A$68-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("E",I60:BC$68,$A$68-$A60+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H60" s="10"/>
@@ -5423,11 +5815,11 @@
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
       <c r="F61" s="11">
-        <f>IFERROR( HLOOKUP("BE",I61:BC$67,$A$67-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("B",I61:BC$67,$A$67-$A61+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I61:BC$68,$A$68-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("B",I61:BC$68,$A$68-$A61+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G61" s="11">
-        <f>IFERROR( HLOOKUP("BE",I61:BC$67,$A$67-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("E",I61:BC$67,$A$67-$A61+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I61:BC$68,$A$68-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("E",I61:BC$68,$A$68-$A61+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H61" s="10"/>
@@ -5488,11 +5880,11 @@
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
       <c r="F62" s="11">
-        <f>IFERROR( HLOOKUP("BE",I62:BC$67,$A$67-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",I62:BC$67,$A$67-$A62+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I62:BC$68,$A$68-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",I62:BC$68,$A$68-$A62+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G62" s="11">
-        <f>IFERROR( HLOOKUP("BE",I62:BC$67,$A$67-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",I62:BC$67,$A$67-$A62+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I62:BC$68,$A$68-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",I62:BC$68,$A$68-$A62+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H62" s="10"/>
@@ -5553,11 +5945,11 @@
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="11">
-        <f>IFERROR( HLOOKUP("BE",I63:BC$67,$A$67-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",I63:BC$67,$A$67-$A63+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I63:BC$68,$A$68-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",I63:BC$68,$A$68-$A63+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G63" s="11">
-        <f>IFERROR( HLOOKUP("BE",I63:BC$67,$A$67-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",I63:BC$67,$A$67-$A63+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I63:BC$68,$A$68-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",I63:BC$68,$A$68-$A63+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H63" s="10"/>
@@ -5613,6 +6005,66 @@
       <c r="A64">
         <v>54</v>
       </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="11">
+        <f>IFERROR( HLOOKUP("BE",I64:BC$68,$A$68-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("B",I64:BC$68,$A$68-$A64+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="11">
+        <f>IFERROR( HLOOKUP("BE",I64:BC$68,$A$68-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("E",I64:BC$68,$A$68-$A64+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H64" s="10"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="1"/>
+      <c r="AE64" s="1"/>
+      <c r="AF64" s="1"/>
+      <c r="AG64" s="1"/>
+      <c r="AH64" s="1"/>
+      <c r="AI64" s="1"/>
+      <c r="AJ64" s="1"/>
+      <c r="AK64" s="1"/>
+      <c r="AL64" s="1"/>
+      <c r="AM64" s="1"/>
+      <c r="AN64" s="1"/>
+      <c r="AO64" s="1"/>
+      <c r="AP64" s="1"/>
+      <c r="AQ64" s="1"/>
+      <c r="AR64" s="1"/>
+      <c r="AS64" s="1"/>
+      <c r="AT64" s="1"/>
+      <c r="AU64" s="1"/>
+      <c r="AV64" s="1"/>
+      <c r="AW64" s="1"/>
+      <c r="AX64" s="1"/>
+      <c r="AY64" s="1"/>
+      <c r="AZ64" s="1"/>
+      <c r="BA64" s="1"/>
+      <c r="BB64" s="1"/>
+      <c r="BC64" s="1"/>
     </row>
     <row r="65" spans="1:55">
       <c r="A65">
@@ -5624,253 +6076,258 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:55" s="17" customFormat="1">
+    <row r="67" spans="1:55">
       <c r="A67">
         <v>57</v>
       </c>
-      <c r="C67" s="17" t="s">
+    </row>
+    <row r="68" spans="1:55" s="17" customFormat="1">
+      <c r="A68">
+        <v>58</v>
+      </c>
+      <c r="C68" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="I67" s="12">
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="I68" s="12">
         <f>I8</f>
         <v>40770</v>
       </c>
-      <c r="J67" s="12">
-        <f t="shared" ref="J67:BC67" si="1">J8</f>
+      <c r="J68" s="12">
+        <f t="shared" ref="J68:BC68" si="1">J8</f>
         <v>40771</v>
       </c>
-      <c r="K67" s="12">
+      <c r="K68" s="12">
         <f t="shared" si="1"/>
         <v>40772</v>
       </c>
-      <c r="L67" s="12">
+      <c r="L68" s="12">
         <f t="shared" si="1"/>
         <v>40773</v>
       </c>
-      <c r="M67" s="12">
+      <c r="M68" s="12">
         <f t="shared" si="1"/>
         <v>40774</v>
       </c>
-      <c r="N67" s="12">
+      <c r="N68" s="12">
         <f t="shared" si="1"/>
         <v>40775</v>
       </c>
-      <c r="O67" s="12">
+      <c r="O68" s="12">
         <f t="shared" si="1"/>
         <v>40776</v>
       </c>
-      <c r="P67" s="12">
+      <c r="P68" s="12">
         <f t="shared" si="1"/>
         <v>40777</v>
       </c>
-      <c r="Q67" s="12">
+      <c r="Q68" s="12">
         <f t="shared" si="1"/>
         <v>40778</v>
       </c>
-      <c r="R67" s="12">
+      <c r="R68" s="12">
         <f t="shared" si="1"/>
         <v>40779</v>
       </c>
-      <c r="S67" s="12">
+      <c r="S68" s="12">
         <f t="shared" si="1"/>
         <v>40780</v>
       </c>
-      <c r="T67" s="12">
+      <c r="T68" s="12">
         <f t="shared" si="1"/>
         <v>40781</v>
       </c>
-      <c r="U67" s="12">
+      <c r="U68" s="12">
         <f t="shared" si="1"/>
         <v>40782</v>
       </c>
-      <c r="V67" s="12">
+      <c r="V68" s="12">
         <f t="shared" si="1"/>
         <v>40783</v>
       </c>
-      <c r="W67" s="12">
+      <c r="W68" s="12">
         <f t="shared" si="1"/>
         <v>40784</v>
       </c>
-      <c r="X67" s="12">
+      <c r="X68" s="12">
         <f t="shared" si="1"/>
         <v>40785</v>
       </c>
-      <c r="Y67" s="12">
+      <c r="Y68" s="12">
         <f t="shared" si="1"/>
         <v>40786</v>
       </c>
-      <c r="Z67" s="12">
+      <c r="Z68" s="12">
         <f t="shared" si="1"/>
         <v>40787</v>
       </c>
-      <c r="AA67" s="12">
+      <c r="AA68" s="12">
         <f t="shared" si="1"/>
         <v>40788</v>
       </c>
-      <c r="AB67" s="12">
+      <c r="AB68" s="12">
         <f t="shared" si="1"/>
         <v>40789</v>
       </c>
-      <c r="AC67" s="12">
+      <c r="AC68" s="12">
         <f t="shared" si="1"/>
         <v>40790</v>
       </c>
-      <c r="AD67" s="12">
+      <c r="AD68" s="12">
         <f t="shared" si="1"/>
         <v>40791</v>
       </c>
-      <c r="AE67" s="12">
+      <c r="AE68" s="12">
         <f t="shared" si="1"/>
         <v>40792</v>
       </c>
-      <c r="AF67" s="12">
+      <c r="AF68" s="12">
         <f t="shared" si="1"/>
         <v>40793</v>
       </c>
-      <c r="AG67" s="12">
+      <c r="AG68" s="12">
         <f t="shared" si="1"/>
         <v>40794</v>
       </c>
-      <c r="AH67" s="12">
+      <c r="AH68" s="12">
         <f t="shared" si="1"/>
         <v>40795</v>
       </c>
-      <c r="AI67" s="12">
+      <c r="AI68" s="12">
         <f t="shared" si="1"/>
         <v>40796</v>
       </c>
-      <c r="AJ67" s="12">
+      <c r="AJ68" s="12">
         <f t="shared" si="1"/>
         <v>40797</v>
       </c>
-      <c r="AK67" s="12">
+      <c r="AK68" s="12">
         <f t="shared" si="1"/>
         <v>40798</v>
       </c>
-      <c r="AL67" s="12">
+      <c r="AL68" s="12">
         <f t="shared" si="1"/>
         <v>40799</v>
       </c>
-      <c r="AM67" s="12">
+      <c r="AM68" s="12">
         <f t="shared" si="1"/>
         <v>40800</v>
       </c>
-      <c r="AN67" s="12">
+      <c r="AN68" s="12">
         <f t="shared" si="1"/>
         <v>40801</v>
       </c>
-      <c r="AO67" s="12">
+      <c r="AO68" s="12">
         <f t="shared" si="1"/>
         <v>40802</v>
       </c>
-      <c r="AP67" s="12">
+      <c r="AP68" s="12">
         <f t="shared" si="1"/>
         <v>40803</v>
       </c>
-      <c r="AQ67" s="12">
+      <c r="AQ68" s="12">
         <f t="shared" si="1"/>
         <v>40804</v>
       </c>
-      <c r="AR67" s="12">
+      <c r="AR68" s="12">
         <f t="shared" si="1"/>
         <v>40805</v>
       </c>
-      <c r="AS67" s="12">
+      <c r="AS68" s="12">
         <f t="shared" si="1"/>
         <v>40806</v>
       </c>
-      <c r="AT67" s="12">
+      <c r="AT68" s="12">
         <f t="shared" si="1"/>
         <v>40807</v>
       </c>
-      <c r="AU67" s="12">
+      <c r="AU68" s="12">
         <f t="shared" si="1"/>
         <v>40808</v>
       </c>
-      <c r="AV67" s="12">
+      <c r="AV68" s="12">
         <f t="shared" si="1"/>
         <v>40809</v>
       </c>
-      <c r="AW67" s="12">
+      <c r="AW68" s="12">
         <f t="shared" si="1"/>
         <v>40810</v>
       </c>
-      <c r="AX67" s="12">
+      <c r="AX68" s="12">
         <f t="shared" si="1"/>
         <v>40811</v>
       </c>
-      <c r="AY67" s="12">
+      <c r="AY68" s="12">
         <f t="shared" si="1"/>
         <v>40812</v>
       </c>
-      <c r="AZ67" s="12">
+      <c r="AZ68" s="12">
         <f t="shared" si="1"/>
         <v>40813</v>
       </c>
-      <c r="BA67" s="12">
+      <c r="BA68" s="12">
         <f t="shared" si="1"/>
         <v>40814</v>
       </c>
-      <c r="BB67" s="12">
+      <c r="BB68" s="12">
         <f t="shared" si="1"/>
         <v>40815</v>
       </c>
-      <c r="BC67" s="12">
+      <c r="BC68" s="12">
         <f t="shared" si="1"/>
         <v>40816</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A9:BC67">
+  <autoFilter ref="A9:BC68">
     <filterColumn colId="4"/>
   </autoFilter>
-  <conditionalFormatting sqref="I47:AV64 I16:BC23 I47:BC63 I10:BC12 I25:BC34 I36:BC45">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+  <conditionalFormatting sqref="I48:AV65 I10:BC12 I26:BC35 I37:BC46 I16:BC24 I48:BC64">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16:BC23 I47:BC63 I10:BC12 I25:BC34 I36:BC45">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+  <conditionalFormatting sqref="I10:BC12 I26:BC35 I37:BC46 I16:BC24 I48:BC64">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:BC14">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:BC14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Chỉnh sửa lại plan
</commit_message>
<xml_diff>
--- a/Document/sale_project v2011.08.20.xlsx
+++ b/Document/sale_project v2011.08.20.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan!$A$9:$BC$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan!$A$9:$BC$70</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t>STT</t>
   </si>
@@ -230,12 +230,6 @@
     <t>Uy</t>
   </si>
   <si>
-    <t>Quản lý nhóm khách hàng</t>
-  </si>
-  <si>
-    <t>Quản lý khách hàng</t>
-  </si>
-  <si>
     <t>Cập nhật giá bán sản phẩm</t>
   </si>
   <si>
@@ -273,6 +267,18 @@
   </si>
   <si>
     <t>MinhNN</t>
+  </si>
+  <si>
+    <t>Quản lý khách hàng master</t>
+  </si>
+  <si>
+    <t>Quản lý khách hàng detail</t>
+  </si>
+  <si>
+    <t>Quản lý nhóm khách hàng detail</t>
+  </si>
+  <si>
+    <t>Quản lý nhóm khách hàng master</t>
   </si>
 </sst>
 </file>
@@ -467,679 +473,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF0000CC"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1840,13 +1174,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC68"/>
+  <dimension ref="A1:BC70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="8" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N49" sqref="N49"/>
+      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1862,10 +1196,10 @@
   <sheetData>
     <row r="1" spans="1:55">
       <c r="C1" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E1" s="22"/>
     </row>
@@ -1874,8 +1208,8 @@
         <v>26</v>
       </c>
       <c r="D2" s="22">
-        <f>SUMIF($D$9:$D$64,C2,$E$9:$E$64)</f>
-        <v>5</v>
+        <f>SUMIF($D$9:$D$66,C2,$E$9:$E$66)</f>
+        <v>6</v>
       </c>
       <c r="E2" s="22"/>
     </row>
@@ -1884,14 +1218,14 @@
         <v>31</v>
       </c>
       <c r="D3" s="22">
-        <f t="shared" ref="D3:D7" si="0">SUMIF($D$9:$D$64,C3,$E$9:$E$64)</f>
+        <f t="shared" ref="D3:D7" si="0">SUMIF($D$9:$D$66,C3,$E$9:$E$66)</f>
         <v>12</v>
       </c>
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:55">
       <c r="C4" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="22">
         <f t="shared" si="0"/>
@@ -1901,7 +1235,7 @@
     </row>
     <row r="5" spans="1:55">
       <c r="C5" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="22">
         <f t="shared" si="0"/>
@@ -1911,11 +1245,11 @@
     </row>
     <row r="6" spans="1:55">
       <c r="C6" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="22">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14.6</v>
       </c>
       <c r="E6" s="22"/>
     </row>
@@ -1925,7 +1259,7 @@
       </c>
       <c r="D7" s="22">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12.6</v>
       </c>
       <c r="E7" s="22"/>
     </row>
@@ -1940,7 +1274,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>25</v>
@@ -2166,11 +1500,11 @@
         <v>3</v>
       </c>
       <c r="F10" s="11">
-        <f>IFERROR( HLOOKUP("BE",I10:BC$68,$A$68-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("B",I10:BC$68,$A$68-$A10+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I10:BC$70,$A$70-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("B",I10:BC$70,$A$70-$A10+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G10" s="11">
-        <f>IFERROR( HLOOKUP("BE",I10:BC$68,$A$68-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("E",I10:BC$68,$A$68-$A10+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I10:BC$70,$A$70-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("E",I10:BC$70,$A$70-$A10+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H10" s="10"/>
@@ -2249,11 +1583,11 @@
         <v>3</v>
       </c>
       <c r="F11" s="11">
-        <f>IFERROR( HLOOKUP("BE",I11:BC$68,$A$68-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",I11:BC$68,$A$68-$A11+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I11:BC$70,$A$70-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",I11:BC$70,$A$70-$A11+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G11" s="11">
-        <f>IFERROR( HLOOKUP("BE",I11:BC$68,$A$68-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",I11:BC$68,$A$68-$A11+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I11:BC$70,$A$70-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",I11:BC$70,$A$70-$A11+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H11" s="10"/>
@@ -2322,11 +1656,11 @@
         <v>1</v>
       </c>
       <c r="F12" s="11">
-        <f>IFERROR( HLOOKUP("BE",I12:BC$68,$A$68-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("B",I12:BC$68,$A$68-$A12+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I12:BC$70,$A$70-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("B",I12:BC$70,$A$70-$A12+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G12" s="11">
-        <f>IFERROR( HLOOKUP("BE",I12:BC$68,$A$68-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("E",I12:BC$68,$A$68-$A12+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I12:BC$70,$A$70-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("E",I12:BC$70,$A$70-$A12+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H12" s="10"/>
@@ -2445,7 +1779,7 @@
       <c r="A14" s="23"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>69</v>
@@ -2454,11 +1788,11 @@
         <v>2</v>
       </c>
       <c r="F14" s="25">
-        <f>IFERROR( HLOOKUP("BE",I14:BC$68,$A$68-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("B",I14:BC$68,$A$68-$A14+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I14:BC$70,$A$70-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("B",I14:BC$70,$A$70-$A14+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G14" s="25">
-        <f>IFERROR( HLOOKUP("BE",I14:BC$68,$A$68-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("E",I14:BC$68,$A$68-$A14+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I14:BC$70,$A$70-$A14+1,FALSE),0)+ IFERROR( HLOOKUP("E",I14:BC$70,$A$70-$A14+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H14" s="26"/>
@@ -2588,11 +1922,11 @@
         <v>1</v>
       </c>
       <c r="F16" s="11">
-        <f>IFERROR( HLOOKUP("BE",I16:BC$68,$A$68-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("B",I16:BC$68,$A$68-$A16+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I16:BC$70,$A$70-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("B",I16:BC$70,$A$70-$A16+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G16" s="11">
-        <f>IFERROR( HLOOKUP("BE",I16:BC$68,$A$68-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("E",I16:BC$68,$A$68-$A16+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I16:BC$70,$A$70-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("E",I16:BC$70,$A$70-$A16+1,FALSE),0)</f>
         <v>40775</v>
       </c>
       <c r="H16" s="10"/>
@@ -2662,20 +1996,20 @@
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
       </c>
       <c r="F17" s="11">
-        <f>IFERROR( HLOOKUP("BE",I17:BC$68,$A$68-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("B",I17:BC$68,$A$68-$A17+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I17:BC$70,$A$70-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("B",I17:BC$70,$A$70-$A17+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G17" s="11">
-        <f>IFERROR( HLOOKUP("BE",I17:BC$68,$A$68-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("E",I17:BC$68,$A$68-$A17+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I17:BC$70,$A$70-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("E",I17:BC$70,$A$70-$A17+1,FALSE),0)</f>
         <v>40775</v>
       </c>
       <c r="H17" s="10"/>
@@ -2754,11 +2088,11 @@
         <v>1</v>
       </c>
       <c r="F18" s="11">
-        <f>IFERROR( HLOOKUP("BE",I18:BC$68,$A$68-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",I18:BC$68,$A$68-$A18+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I18:BC$70,$A$70-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",I18:BC$70,$A$70-$A18+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G18" s="11">
-        <f>IFERROR( HLOOKUP("BE",I18:BC$68,$A$68-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",I18:BC$68,$A$68-$A18+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I18:BC$70,$A$70-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",I18:BC$70,$A$70-$A18+1,FALSE),0)</f>
         <v>40775</v>
       </c>
       <c r="H18" s="10"/>
@@ -2831,38 +2165,28 @@
         <v>60</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="E19" s="10">
         <v>1</v>
       </c>
       <c r="F19" s="11">
-        <f>IFERROR( HLOOKUP("BE",I19:BC$68,$A$68-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",I19:BC$68,$A$68-$A19+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I19:BC$70,$A$70-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",I19:BC$70,$A$70-$A19+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G19" s="11">
-        <f>IFERROR( HLOOKUP("BE",I19:BC$68,$A$68-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",I19:BC$68,$A$68-$A19+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",I19:BC$70,$A$70-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",I19:BC$70,$A$70-$A19+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -2914,17 +2238,17 @@
         <v>61</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E20" s="10">
         <v>1</v>
       </c>
       <c r="F20" s="11">
-        <f>IFERROR( HLOOKUP("BE",I20:BC$68,$A$68-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",I20:BC$68,$A$68-$A20+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I20:BC$70,$A$70-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",I20:BC$70,$A$70-$A20+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G20" s="11">
-        <f>IFERROR( HLOOKUP("BE",I20:BC$68,$A$68-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",I20:BC$68,$A$68-$A20+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I20:BC$70,$A$70-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",I20:BC$70,$A$70-$A20+1,FALSE),0)</f>
         <v>40775</v>
       </c>
       <c r="H20" s="10"/>
@@ -3003,11 +2327,11 @@
         <v>1</v>
       </c>
       <c r="F21" s="11">
-        <f>IFERROR( HLOOKUP("BE",I21:BC$68,$A$68-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",I21:BC$68,$A$68-$A21+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I21:BC$70,$A$70-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",I21:BC$70,$A$70-$A21+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G21" s="11">
-        <f>IFERROR( HLOOKUP("BE",I21:BC$68,$A$68-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",I21:BC$68,$A$68-$A21+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I21:BC$70,$A$70-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",I21:BC$70,$A$70-$A21+1,FALSE),0)</f>
         <v>40775</v>
       </c>
       <c r="H21" s="10"/>
@@ -3077,41 +2401,31 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E22" s="10">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F22" s="11">
-        <f>IFERROR( HLOOKUP("BE",I22:BC$68,$A$68-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",I22:BC$68,$A$68-$A22+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",I22:BC$70,$A$70-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",I22:BC$70,$A$70-$A22+1,FALSE),0)</f>
+        <v>40774</v>
       </c>
       <c r="G22" s="11">
-        <f>IFERROR( HLOOKUP("BE",I22:BC$68,$A$68-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",I22:BC$68,$A$68-$A22+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",I22:BC$70,$A$70-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",I22:BC$70,$A$70-$A22+1,FALSE),0)</f>
+        <v>40774</v>
       </c>
       <c r="H22" s="10"/>
-      <c r="I22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -3160,20 +2474,20 @@
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E23" s="10">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F23" s="11">
-        <f>IFERROR( HLOOKUP("BE",I23:BC$68,$A$68-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("B",I23:BC$68,$A$68-$A23+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I23:BC$70,$A$70-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("B",I23:BC$70,$A$70-$A23+1,FALSE),0)</f>
         <v>40770</v>
       </c>
       <c r="G23" s="11">
-        <f>IFERROR( HLOOKUP("BE",I23:BC$68,$A$68-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("E",I23:BC$68,$A$68-$A23+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I23:BC$70,$A$70-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("E",I23:BC$70,$A$70-$A23+1,FALSE),0)</f>
         <v>40775</v>
       </c>
       <c r="H23" s="10"/>
@@ -3243,30 +2557,30 @@
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E24" s="10">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F24" s="11">
-        <f>IFERROR( HLOOKUP("BE",I24:BC$68,$A$68-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",I24:BC$68,$A$68-$A24+1,FALSE),0)</f>
-        <v>40773</v>
+        <f>IFERROR( HLOOKUP("BE",I24:BC$70,$A$70-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",I24:BC$70,$A$70-$A24+1,FALSE),0)</f>
+        <v>40774</v>
       </c>
       <c r="G24" s="11">
-        <f>IFERROR( HLOOKUP("BE",I24:BC$68,$A$68-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",I24:BC$68,$A$68-$A24+1,FALSE),0)</f>
-        <v>40773</v>
+        <f>IFERROR( HLOOKUP("BE",I24:BC$70,$A$70-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",I24:BC$70,$A$70-$A24+1,FALSE),0)</f>
+        <v>40774</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1" t="s">
+      <c r="L24" s="1"/>
+      <c r="M24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -3310,66 +2624,88 @@
       <c r="BB24" s="1"/>
       <c r="BC24" s="1"/>
     </row>
-    <row r="25" spans="1:55" s="14" customFormat="1">
+    <row r="25" spans="1:55">
       <c r="A25">
         <v>15</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="13"/>
-      <c r="AD25" s="13"/>
-      <c r="AE25" s="13"/>
-      <c r="AF25" s="13"/>
-      <c r="AG25" s="13"/>
-      <c r="AH25" s="13"/>
-      <c r="AI25" s="13"/>
-      <c r="AJ25" s="13"/>
-      <c r="AK25" s="13"/>
-      <c r="AL25" s="13"/>
-      <c r="AM25" s="13"/>
-      <c r="AN25" s="13"/>
-      <c r="AO25" s="13"/>
-      <c r="AP25" s="13"/>
-      <c r="AQ25" s="13"/>
-      <c r="AR25" s="13"/>
-      <c r="AS25" s="13"/>
-      <c r="AT25" s="13"/>
-      <c r="AU25" s="13"/>
-      <c r="AV25" s="13"/>
-      <c r="AW25" s="13"/>
-      <c r="AX25" s="13"/>
-      <c r="AY25" s="13"/>
-      <c r="AZ25" s="13"/>
-      <c r="BA25" s="13"/>
-      <c r="BB25" s="13"/>
-      <c r="BC25" s="13"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="F25" s="11">
+        <f>IFERROR( HLOOKUP("BE",I25:BC$70,$A$70-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("B",I25:BC$70,$A$70-$A25+1,FALSE),0)</f>
+        <v>40770</v>
+      </c>
+      <c r="G25" s="11">
+        <f>IFERROR( HLOOKUP("BE",I25:BC$70,$A$70-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("E",I25:BC$70,$A$70-$A25+1,FALSE),0)</f>
+        <v>40775</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="1"/>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1"/>
+      <c r="BA25" s="1"/>
+      <c r="BB25" s="1"/>
+      <c r="BC25" s="1"/>
     </row>
     <row r="26" spans="1:55">
       <c r="A26">
@@ -3377,35 +2713,33 @@
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="E26" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F26" s="11">
-        <f>IFERROR( HLOOKUP("BE",I26:BC$68,$A$68-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",I26:BC$68,$A$68-$A26+1,FALSE),0)</f>
-        <v>40776</v>
+        <f>IFERROR( HLOOKUP("BE",I26:BC$70,$A$70-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",I26:BC$70,$A$70-$A26+1,FALSE),0)</f>
+        <v>40773</v>
       </c>
       <c r="G26" s="11">
-        <f>IFERROR( HLOOKUP("BE",I26:BC$68,$A$68-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",I26:BC$68,$A$68-$A26+1,FALSE),0)</f>
-        <v>40777</v>
+        <f>IFERROR( HLOOKUP("BE",I26:BC$70,$A$70-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",I26:BC$70,$A$70-$A26+1,FALSE),0)</f>
+        <v>40773</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -3446,80 +2780,66 @@
       <c r="BB26" s="1"/>
       <c r="BC26" s="1"/>
     </row>
-    <row r="27" spans="1:55">
+    <row r="27" spans="1:55" s="14" customFormat="1">
       <c r="A27">
         <v>17</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="10">
-        <v>3</v>
-      </c>
-      <c r="F27" s="11">
-        <f>IFERROR( HLOOKUP("BE",I27:BC$68,$A$68-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",I27:BC$68,$A$68-$A27+1,FALSE),0)</f>
-        <v>40776</v>
-      </c>
-      <c r="G27" s="11">
-        <f>IFERROR( HLOOKUP("BE",I27:BC$68,$A$68-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",I27:BC$68,$A$68-$A27+1,FALSE),0)</f>
-        <v>40777</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
-      <c r="AG27" s="1"/>
-      <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
-      <c r="AJ27" s="1"/>
-      <c r="AK27" s="1"/>
-      <c r="AL27" s="1"/>
-      <c r="AM27" s="1"/>
-      <c r="AN27" s="1"/>
-      <c r="AO27" s="1"/>
-      <c r="AP27" s="1"/>
-      <c r="AQ27" s="1"/>
-      <c r="AR27" s="1"/>
-      <c r="AS27" s="1"/>
-      <c r="AT27" s="1"/>
-      <c r="AU27" s="1"/>
-      <c r="AV27" s="1"/>
-      <c r="AW27" s="1"/>
-      <c r="AX27" s="1"/>
-      <c r="AY27" s="1"/>
-      <c r="AZ27" s="1"/>
-      <c r="BA27" s="1"/>
-      <c r="BB27" s="1"/>
-      <c r="BC27" s="1"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="13"/>
+      <c r="AC27" s="13"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="13"/>
+      <c r="AH27" s="13"/>
+      <c r="AI27" s="13"/>
+      <c r="AJ27" s="13"/>
+      <c r="AK27" s="13"/>
+      <c r="AL27" s="13"/>
+      <c r="AM27" s="13"/>
+      <c r="AN27" s="13"/>
+      <c r="AO27" s="13"/>
+      <c r="AP27" s="13"/>
+      <c r="AQ27" s="13"/>
+      <c r="AR27" s="13"/>
+      <c r="AS27" s="13"/>
+      <c r="AT27" s="13"/>
+      <c r="AU27" s="13"/>
+      <c r="AV27" s="13"/>
+      <c r="AW27" s="13"/>
+      <c r="AX27" s="13"/>
+      <c r="AY27" s="13"/>
+      <c r="AZ27" s="13"/>
+      <c r="BA27" s="13"/>
+      <c r="BB27" s="13"/>
+      <c r="BC27" s="13"/>
     </row>
     <row r="28" spans="1:55">
       <c r="A28">
@@ -3527,12 +2847,22 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="10">
+        <v>3</v>
+      </c>
+      <c r="F28" s="11">
+        <f>IFERROR( HLOOKUP("BE",I28:BC$70,$A$70-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("B",I28:BC$70,$A$70-$A28+1,FALSE),0)</f>
+        <v>40776</v>
+      </c>
+      <c r="G28" s="11">
+        <f>IFERROR( HLOOKUP("BE",I28:BC$70,$A$70-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("E",I28:BC$70,$A$70-$A28+1,FALSE),0)</f>
+        <v>40777</v>
+      </c>
       <c r="H28" s="10"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3540,8 +2870,12 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="O28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -3587,21 +2921,21 @@
         <v>19</v>
       </c>
       <c r="B29" s="10"/>
-      <c r="C29" s="18" t="s">
-        <v>44</v>
+      <c r="C29" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="10">
         <v>3</v>
       </c>
       <c r="F29" s="11">
-        <f>IFERROR( HLOOKUP("BE",I29:BC$68,$A$68-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",I29:BC$68,$A$68-$A29+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I29:BC$70,$A$70-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",I29:BC$70,$A$70-$A29+1,FALSE),0)</f>
         <v>40776</v>
       </c>
       <c r="G29" s="11">
-        <f>IFERROR( HLOOKUP("BE",I29:BC$68,$A$68-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",I29:BC$68,$A$68-$A29+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I29:BC$70,$A$70-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",I29:BC$70,$A$70-$A29+1,FALSE),0)</f>
         <v>40777</v>
       </c>
       <c r="H29" s="10"/>
@@ -3662,23 +2996,13 @@
         <v>20</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="10">
-        <v>3</v>
-      </c>
-      <c r="F30" s="11">
-        <f>IFERROR( HLOOKUP("BE",I30:BC$68,$A$68-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",I30:BC$68,$A$68-$A30+1,FALSE),0)</f>
-        <v>40776</v>
-      </c>
-      <c r="G30" s="11">
-        <f>IFERROR( HLOOKUP("BE",I30:BC$68,$A$68-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",I30:BC$68,$A$68-$A30+1,FALSE),0)</f>
-        <v>40777</v>
-      </c>
+      <c r="C30" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="10"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3686,12 +3010,8 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
@@ -3737,13 +3057,23 @@
         <v>21</v>
       </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="C31" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="10">
+        <v>3</v>
+      </c>
+      <c r="F31" s="11">
+        <f>IFERROR( HLOOKUP("BE",I31:BC$70,$A$70-$A31+1,FALSE),0)+ IFERROR( HLOOKUP("B",I31:BC$70,$A$70-$A31+1,FALSE),0)</f>
+        <v>40776</v>
+      </c>
+      <c r="G31" s="11">
+        <f>IFERROR( HLOOKUP("BE",I31:BC$70,$A$70-$A31+1,FALSE),0)+ IFERROR( HLOOKUP("E",I31:BC$70,$A$70-$A31+1,FALSE),0)</f>
+        <v>40777</v>
+      </c>
       <c r="H31" s="10"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -3751,8 +3081,12 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
+      <c r="O31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -3799,21 +3133,21 @@
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E32" s="10">
         <v>3</v>
       </c>
       <c r="F32" s="11">
-        <f>IFERROR( HLOOKUP("BE",I32:BC$68,$A$68-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",I32:BC$68,$A$68-$A32+1,FALSE),0)</f>
-        <v>40778</v>
+        <f>IFERROR( HLOOKUP("BE",I32:BC$70,$A$70-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",I32:BC$70,$A$70-$A32+1,FALSE),0)</f>
+        <v>40776</v>
       </c>
       <c r="G32" s="11">
-        <f>IFERROR( HLOOKUP("BE",I32:BC$68,$A$68-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",I32:BC$68,$A$68-$A32+1,FALSE),0)</f>
-        <v>40779</v>
+        <f>IFERROR( HLOOKUP("BE",I32:BC$70,$A$70-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",I32:BC$70,$A$70-$A32+1,FALSE),0)</f>
+        <v>40777</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="1"/>
@@ -3822,14 +3156,14 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -3873,23 +3207,13 @@
         <v>23</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="10">
-        <v>3</v>
-      </c>
-      <c r="F33" s="11">
-        <f>IFERROR( HLOOKUP("BE",I33:BC$68,$A$68-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",I33:BC$68,$A$68-$A33+1,FALSE),0)</f>
-        <v>40778</v>
-      </c>
-      <c r="G33" s="11">
-        <f>IFERROR( HLOOKUP("BE",I33:BC$68,$A$68-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",I33:BC$68,$A$68-$A33+1,FALSE),0)</f>
-        <v>40779</v>
-      </c>
+      <c r="C33" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="10"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -3899,12 +3223,8 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -3948,21 +3268,21 @@
         <v>24</v>
       </c>
       <c r="B34" s="10"/>
-      <c r="C34" s="10" t="s">
-        <v>48</v>
+      <c r="C34" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="10">
         <v>3</v>
       </c>
       <c r="F34" s="11">
-        <f>IFERROR( HLOOKUP("BE",I34:BC$68,$A$68-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("B",I34:BC$68,$A$68-$A34+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I34:BC$70,$A$70-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("B",I34:BC$70,$A$70-$A34+1,FALSE),0)</f>
         <v>40778</v>
       </c>
       <c r="G34" s="11">
-        <f>IFERROR( HLOOKUP("BE",I34:BC$68,$A$68-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("E",I34:BC$68,$A$68-$A34+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I34:BC$70,$A$70-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("E",I34:BC$70,$A$70-$A34+1,FALSE),0)</f>
         <v>40779</v>
       </c>
       <c r="H34" s="10"/>
@@ -4023,21 +3343,21 @@
         <v>25</v>
       </c>
       <c r="B35" s="10"/>
-      <c r="C35" s="10" t="s">
-        <v>43</v>
+      <c r="C35" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E35" s="10">
         <v>3</v>
       </c>
       <c r="F35" s="11">
-        <f>IFERROR( HLOOKUP("BE",I35:BC$68,$A$68-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",I35:BC$68,$A$68-$A35+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I35:BC$70,$A$70-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",I35:BC$70,$A$70-$A35+1,FALSE),0)</f>
         <v>40778</v>
       </c>
       <c r="G35" s="11">
-        <f>IFERROR( HLOOKUP("BE",I35:BC$68,$A$68-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",I35:BC$68,$A$68-$A35+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I35:BC$70,$A$70-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",I35:BC$70,$A$70-$A35+1,FALSE),0)</f>
         <v>40779</v>
       </c>
       <c r="H35" s="10"/>
@@ -4093,66 +3413,80 @@
       <c r="BB35" s="1"/>
       <c r="BC35" s="1"/>
     </row>
-    <row r="36" spans="1:55" s="14" customFormat="1">
+    <row r="36" spans="1:55">
       <c r="A36">
         <v>26</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
-      <c r="AB36" s="13"/>
-      <c r="AC36" s="13"/>
-      <c r="AD36" s="13"/>
-      <c r="AE36" s="13"/>
-      <c r="AF36" s="13"/>
-      <c r="AG36" s="13"/>
-      <c r="AH36" s="13"/>
-      <c r="AI36" s="13"/>
-      <c r="AJ36" s="13"/>
-      <c r="AK36" s="13"/>
-      <c r="AL36" s="13"/>
-      <c r="AM36" s="13"/>
-      <c r="AN36" s="13"/>
-      <c r="AO36" s="13"/>
-      <c r="AP36" s="13"/>
-      <c r="AQ36" s="13"/>
-      <c r="AR36" s="13"/>
-      <c r="AS36" s="13"/>
-      <c r="AT36" s="13"/>
-      <c r="AU36" s="13"/>
-      <c r="AV36" s="13"/>
-      <c r="AW36" s="13"/>
-      <c r="AX36" s="13"/>
-      <c r="AY36" s="13"/>
-      <c r="AZ36" s="13"/>
-      <c r="BA36" s="13"/>
-      <c r="BB36" s="13"/>
-      <c r="BC36" s="13"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="10">
+        <v>3</v>
+      </c>
+      <c r="F36" s="11">
+        <f>IFERROR( HLOOKUP("BE",I36:BC$70,$A$70-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("B",I36:BC$70,$A$70-$A36+1,FALSE),0)</f>
+        <v>40778</v>
+      </c>
+      <c r="G36" s="11">
+        <f>IFERROR( HLOOKUP("BE",I36:BC$70,$A$70-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("E",I36:BC$70,$A$70-$A36+1,FALSE),0)</f>
+        <v>40779</v>
+      </c>
+      <c r="H36" s="10"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+      <c r="AO36" s="1"/>
+      <c r="AP36" s="1"/>
+      <c r="AQ36" s="1"/>
+      <c r="AR36" s="1"/>
+      <c r="AS36" s="1"/>
+      <c r="AT36" s="1"/>
+      <c r="AU36" s="1"/>
+      <c r="AV36" s="1"/>
+      <c r="AW36" s="1"/>
+      <c r="AX36" s="1"/>
+      <c r="AY36" s="1"/>
+      <c r="AZ36" s="1"/>
+      <c r="BA36" s="1"/>
+      <c r="BB36" s="1"/>
+      <c r="BC36" s="1"/>
     </row>
     <row r="37" spans="1:55">
       <c r="A37">
@@ -4160,7 +3494,7 @@
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>31</v>
@@ -4169,12 +3503,12 @@
         <v>3</v>
       </c>
       <c r="F37" s="11">
-        <f>IFERROR( HLOOKUP("BE",I37:BC$68,$A$68-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("B",I37:BC$68,$A$68-$A37+1,FALSE),0)</f>
-        <v>40780</v>
+        <f>IFERROR( HLOOKUP("BE",I37:BC$70,$A$70-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("B",I37:BC$70,$A$70-$A37+1,FALSE),0)</f>
+        <v>40778</v>
       </c>
       <c r="G37" s="11">
-        <f>IFERROR( HLOOKUP("BE",I37:BC$68,$A$68-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("E",I37:BC$68,$A$68-$A37+1,FALSE),0)</f>
-        <v>40781</v>
+        <f>IFERROR( HLOOKUP("BE",I37:BC$70,$A$70-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("E",I37:BC$70,$A$70-$A37+1,FALSE),0)</f>
+        <v>40779</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="1"/>
@@ -4185,14 +3519,14 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
@@ -4229,87 +3563,87 @@
       <c r="BB37" s="1"/>
       <c r="BC37" s="1"/>
     </row>
-    <row r="38" spans="1:55">
+    <row r="38" spans="1:55" s="14" customFormat="1">
       <c r="A38">
         <v>28</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-      <c r="AG38" s="1"/>
-      <c r="AH38" s="1"/>
-      <c r="AI38" s="1"/>
-      <c r="AJ38" s="1"/>
-      <c r="AK38" s="1"/>
-      <c r="AL38" s="1"/>
-      <c r="AM38" s="1"/>
-      <c r="AN38" s="1"/>
-      <c r="AO38" s="1"/>
-      <c r="AP38" s="1"/>
-      <c r="AQ38" s="1"/>
-      <c r="AR38" s="1"/>
-      <c r="AS38" s="1"/>
-      <c r="AT38" s="1"/>
-      <c r="AU38" s="1"/>
-      <c r="AV38" s="1"/>
-      <c r="AW38" s="1"/>
-      <c r="AX38" s="1"/>
-      <c r="AY38" s="1"/>
-      <c r="AZ38" s="1"/>
-      <c r="BA38" s="1"/>
-      <c r="BB38" s="1"/>
-      <c r="BC38" s="1"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13"/>
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="13"/>
+      <c r="AF38" s="13"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="13"/>
+      <c r="AI38" s="13"/>
+      <c r="AJ38" s="13"/>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="13"/>
+      <c r="AM38" s="13"/>
+      <c r="AN38" s="13"/>
+      <c r="AO38" s="13"/>
+      <c r="AP38" s="13"/>
+      <c r="AQ38" s="13"/>
+      <c r="AR38" s="13"/>
+      <c r="AS38" s="13"/>
+      <c r="AT38" s="13"/>
+      <c r="AU38" s="13"/>
+      <c r="AV38" s="13"/>
+      <c r="AW38" s="13"/>
+      <c r="AX38" s="13"/>
+      <c r="AY38" s="13"/>
+      <c r="AZ38" s="13"/>
+      <c r="BA38" s="13"/>
+      <c r="BB38" s="13"/>
+      <c r="BC38" s="13"/>
     </row>
     <row r="39" spans="1:55">
       <c r="A39">
         <v>29</v>
       </c>
       <c r="B39" s="10"/>
-      <c r="C39" s="20" t="s">
-        <v>50</v>
+      <c r="C39" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="E39" s="10">
         <v>3</v>
       </c>
       <c r="F39" s="11">
-        <f>IFERROR( HLOOKUP("BE",I39:BC$68,$A$68-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("B",I39:BC$68,$A$68-$A39+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I39:BC$70,$A$70-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("B",I39:BC$70,$A$70-$A39+1,FALSE),0)</f>
         <v>40780</v>
       </c>
       <c r="G39" s="11">
-        <f>IFERROR( HLOOKUP("BE",I39:BC$68,$A$68-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("E",I39:BC$68,$A$68-$A39+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I39:BC$70,$A$70-$A39+1,FALSE),0)+ IFERROR( HLOOKUP("E",I39:BC$70,$A$70-$A39+1,FALSE),0)</f>
         <v>40781</v>
       </c>
       <c r="H39" s="10"/>
@@ -4370,23 +3704,13 @@
         <v>30</v>
       </c>
       <c r="B40" s="10"/>
-      <c r="C40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" s="10">
-        <v>3</v>
-      </c>
-      <c r="F40" s="11">
-        <f>IFERROR( HLOOKUP("BE",I40:BC$68,$A$68-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("B",I40:BC$68,$A$68-$A40+1,FALSE),0)</f>
-        <v>40780</v>
-      </c>
-      <c r="G40" s="11">
-        <f>IFERROR( HLOOKUP("BE",I40:BC$68,$A$68-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("E",I40:BC$68,$A$68-$A40+1,FALSE),0)</f>
-        <v>40781</v>
-      </c>
+      <c r="C40" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
       <c r="H40" s="10"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -4398,12 +3722,8 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T40" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
@@ -4445,21 +3765,21 @@
         <v>31</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="10" t="s">
-        <v>52</v>
+      <c r="C41" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E41" s="10">
         <v>3</v>
       </c>
       <c r="F41" s="11">
-        <f>IFERROR( HLOOKUP("BE",I41:BC$68,$A$68-$A41+1,FALSE),0)+ IFERROR( HLOOKUP("B",I41:BC$68,$A$68-$A41+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I41:BC$70,$A$70-$A41+1,FALSE),0)+ IFERROR( HLOOKUP("B",I41:BC$70,$A$70-$A41+1,FALSE),0)</f>
         <v>40780</v>
       </c>
       <c r="G41" s="11">
-        <f>IFERROR( HLOOKUP("BE",I41:BC$68,$A$68-$A41+1,FALSE),0)+ IFERROR( HLOOKUP("E",I41:BC$68,$A$68-$A41+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I41:BC$70,$A$70-$A41+1,FALSE),0)+ IFERROR( HLOOKUP("E",I41:BC$70,$A$70-$A41+1,FALSE),0)</f>
         <v>40781</v>
       </c>
       <c r="H41" s="10"/>
@@ -4520,13 +3840,23 @@
         <v>32</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+      <c r="C42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="10">
+        <v>3</v>
+      </c>
+      <c r="F42" s="11">
+        <f>IFERROR( HLOOKUP("BE",I42:BC$70,$A$70-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("B",I42:BC$70,$A$70-$A42+1,FALSE),0)</f>
+        <v>40780</v>
+      </c>
+      <c r="G42" s="11">
+        <f>IFERROR( HLOOKUP("BE",I42:BC$70,$A$70-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("E",I42:BC$70,$A$70-$A42+1,FALSE),0)</f>
+        <v>40781</v>
+      </c>
       <c r="H42" s="10"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -4538,8 +3868,12 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
+      <c r="S42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
@@ -4581,22 +3915,22 @@
         <v>33</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="20" t="s">
-        <v>54</v>
+      <c r="C43" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E43" s="10">
         <v>3</v>
       </c>
       <c r="F43" s="11">
-        <f>IFERROR( HLOOKUP("BE",I43:BC$68,$A$68-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("B",I43:BC$68,$A$68-$A43+1,FALSE),0)</f>
-        <v>40782</v>
+        <f>IFERROR( HLOOKUP("BE",I43:BC$70,$A$70-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("B",I43:BC$70,$A$70-$A43+1,FALSE),0)</f>
+        <v>40780</v>
       </c>
       <c r="G43" s="11">
-        <f>IFERROR( HLOOKUP("BE",I43:BC$68,$A$68-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("E",I43:BC$68,$A$68-$A43+1,FALSE),0)</f>
-        <v>40783</v>
+        <f>IFERROR( HLOOKUP("BE",I43:BC$70,$A$70-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("E",I43:BC$70,$A$70-$A43+1,FALSE),0)</f>
+        <v>40781</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="1"/>
@@ -4609,14 +3943,14 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1" t="s">
+      <c r="S43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -4656,23 +3990,13 @@
         <v>34</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="10">
-        <v>3</v>
-      </c>
-      <c r="F44" s="11">
-        <f>IFERROR( HLOOKUP("BE",I44:BC$68,$A$68-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("B",I44:BC$68,$A$68-$A44+1,FALSE),0)</f>
-        <v>40782</v>
-      </c>
-      <c r="G44" s="11">
-        <f>IFERROR( HLOOKUP("BE",I44:BC$68,$A$68-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("E",I44:BC$68,$A$68-$A44+1,FALSE),0)</f>
-        <v>40783</v>
-      </c>
+      <c r="C44" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
       <c r="H44" s="10"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -4686,12 +4010,8 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
-      <c r="U44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -4732,20 +4052,20 @@
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E45" s="10">
         <v>3</v>
       </c>
       <c r="F45" s="11">
-        <f>IFERROR( HLOOKUP("BE",I45:BC$68,$A$68-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("B",I45:BC$68,$A$68-$A45+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I45:BC$70,$A$70-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("B",I45:BC$70,$A$70-$A45+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G45" s="11">
-        <f>IFERROR( HLOOKUP("BE",I45:BC$68,$A$68-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("E",I45:BC$68,$A$68-$A45+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I45:BC$70,$A$70-$A45+1,FALSE),0)+ IFERROR( HLOOKUP("E",I45:BC$70,$A$70-$A45+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H45" s="10"/>
@@ -4807,20 +4127,20 @@
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E46" s="10">
         <v>3</v>
       </c>
       <c r="F46" s="11">
-        <f>IFERROR( HLOOKUP("BE",I46:BC$68,$A$68-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("B",I46:BC$68,$A$68-$A46+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I46:BC$70,$A$70-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("B",I46:BC$70,$A$70-$A46+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G46" s="11">
-        <f>IFERROR( HLOOKUP("BE",I46:BC$68,$A$68-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("E",I46:BC$68,$A$68-$A46+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I46:BC$70,$A$70-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("E",I46:BC$70,$A$70-$A46+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H46" s="10"/>
@@ -4876,94 +4196,106 @@
       <c r="BB46" s="1"/>
       <c r="BC46" s="1"/>
     </row>
-    <row r="47" spans="1:55" s="14" customFormat="1">
+    <row r="47" spans="1:55">
       <c r="A47">
         <v>37</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="13"/>
-      <c r="S47" s="13"/>
-      <c r="T47" s="13"/>
-      <c r="U47" s="13"/>
-      <c r="V47" s="13"/>
-      <c r="W47" s="13"/>
-      <c r="X47" s="13"/>
-      <c r="Y47" s="13"/>
-      <c r="Z47" s="13"/>
-      <c r="AA47" s="13"/>
-      <c r="AB47" s="13"/>
-      <c r="AC47" s="13"/>
-      <c r="AD47" s="13"/>
-      <c r="AE47" s="13"/>
-      <c r="AF47" s="13"/>
-      <c r="AG47" s="13"/>
-      <c r="AH47" s="13"/>
-      <c r="AI47" s="13"/>
-      <c r="AJ47" s="13"/>
-      <c r="AK47" s="13"/>
-      <c r="AL47" s="13"/>
-      <c r="AM47" s="13"/>
-      <c r="AN47" s="13"/>
-      <c r="AO47" s="13"/>
-      <c r="AP47" s="13"/>
-      <c r="AQ47" s="13"/>
-      <c r="AR47" s="13"/>
-      <c r="AS47" s="13"/>
-      <c r="AT47" s="13"/>
-      <c r="AU47" s="13"/>
-      <c r="AV47" s="13"/>
-      <c r="AW47" s="13"/>
-      <c r="AX47" s="13"/>
-      <c r="AY47" s="13"/>
-      <c r="AZ47" s="13"/>
-      <c r="BA47" s="13"/>
-      <c r="BB47" s="13"/>
-      <c r="BC47" s="13"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="10">
+        <v>3</v>
+      </c>
+      <c r="F47" s="11">
+        <f>IFERROR( HLOOKUP("BE",I47:BC$70,$A$70-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("B",I47:BC$70,$A$70-$A47+1,FALSE),0)</f>
+        <v>40782</v>
+      </c>
+      <c r="G47" s="11">
+        <f>IFERROR( HLOOKUP("BE",I47:BC$70,$A$70-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("E",I47:BC$70,$A$70-$A47+1,FALSE),0)</f>
+        <v>40783</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="1"/>
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="1"/>
+      <c r="AI47" s="1"/>
+      <c r="AJ47" s="1"/>
+      <c r="AK47" s="1"/>
+      <c r="AL47" s="1"/>
+      <c r="AM47" s="1"/>
+      <c r="AN47" s="1"/>
+      <c r="AO47" s="1"/>
+      <c r="AP47" s="1"/>
+      <c r="AQ47" s="1"/>
+      <c r="AR47" s="1"/>
+      <c r="AS47" s="1"/>
+      <c r="AT47" s="1"/>
+      <c r="AU47" s="1"/>
+      <c r="AV47" s="1"/>
+      <c r="AW47" s="1"/>
+      <c r="AX47" s="1"/>
+      <c r="AY47" s="1"/>
+      <c r="AZ47" s="1"/>
+      <c r="BA47" s="1"/>
+      <c r="BB47" s="1"/>
+      <c r="BC47" s="1"/>
     </row>
     <row r="48" spans="1:55">
       <c r="A48">
         <v>38</v>
       </c>
       <c r="B48" s="10"/>
-      <c r="C48" s="10" t="s">
-        <v>64</v>
+      <c r="C48" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E48" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" s="11">
-        <f>IFERROR( HLOOKUP("BE",I48:BC$68,$A$68-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("B",I48:BC$68,$A$68-$A48+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",I48:BC$70,$A$70-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("B",I48:BC$70,$A$70-$A48+1,FALSE),0)</f>
+        <v>40782</v>
       </c>
       <c r="G48" s="11">
-        <f>IFERROR( HLOOKUP("BE",I48:BC$68,$A$68-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("E",I48:BC$68,$A$68-$A48+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",I48:BC$70,$A$70-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("E",I48:BC$70,$A$70-$A48+1,FALSE),0)</f>
+        <v>40783</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -4974,8 +4306,12 @@
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
+      <c r="U48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
@@ -5010,106 +4346,94 @@
       <c r="BB48" s="1"/>
       <c r="BC48" s="1"/>
     </row>
-    <row r="49" spans="1:55">
+    <row r="49" spans="1:55" s="14" customFormat="1">
       <c r="A49">
         <v>39</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="10">
-        <v>1</v>
-      </c>
-      <c r="F49" s="11">
-        <f>IFERROR( HLOOKUP("BE",I49:BC$68,$A$68-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("B",I49:BC$68,$A$68-$A49+1,FALSE),0)</f>
-        <v>40771</v>
-      </c>
-      <c r="G49" s="11">
-        <f>IFERROR( HLOOKUP("BE",I49:BC$68,$A$68-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("E",I49:BC$68,$A$68-$A49+1,FALSE),0)</f>
-        <v>40775</v>
-      </c>
-      <c r="H49" s="10"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-      <c r="AF49" s="1"/>
-      <c r="AG49" s="1"/>
-      <c r="AH49" s="1"/>
-      <c r="AI49" s="1"/>
-      <c r="AJ49" s="1"/>
-      <c r="AK49" s="1"/>
-      <c r="AL49" s="1"/>
-      <c r="AM49" s="1"/>
-      <c r="AN49" s="1"/>
-      <c r="AO49" s="1"/>
-      <c r="AP49" s="1"/>
-      <c r="AQ49" s="1"/>
-      <c r="AR49" s="1"/>
-      <c r="AS49" s="1"/>
-      <c r="AT49" s="1"/>
-      <c r="AU49" s="1"/>
-      <c r="AV49" s="1"/>
-      <c r="AW49" s="1"/>
-      <c r="AX49" s="1"/>
-      <c r="AY49" s="1"/>
-      <c r="AZ49" s="1"/>
-      <c r="BA49" s="1"/>
-      <c r="BB49" s="1"/>
-      <c r="BC49" s="1"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="13"/>
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="13"/>
+      <c r="AF49" s="13"/>
+      <c r="AG49" s="13"/>
+      <c r="AH49" s="13"/>
+      <c r="AI49" s="13"/>
+      <c r="AJ49" s="13"/>
+      <c r="AK49" s="13"/>
+      <c r="AL49" s="13"/>
+      <c r="AM49" s="13"/>
+      <c r="AN49" s="13"/>
+      <c r="AO49" s="13"/>
+      <c r="AP49" s="13"/>
+      <c r="AQ49" s="13"/>
+      <c r="AR49" s="13"/>
+      <c r="AS49" s="13"/>
+      <c r="AT49" s="13"/>
+      <c r="AU49" s="13"/>
+      <c r="AV49" s="13"/>
+      <c r="AW49" s="13"/>
+      <c r="AX49" s="13"/>
+      <c r="AY49" s="13"/>
+      <c r="AZ49" s="13"/>
+      <c r="BA49" s="13"/>
+      <c r="BB49" s="13"/>
+      <c r="BC49" s="13"/>
     </row>
     <row r="50" spans="1:55">
       <c r="A50">
         <v>40</v>
       </c>
       <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="C50" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="10">
+        <v>2</v>
+      </c>
       <c r="F50" s="11">
-        <f>IFERROR( HLOOKUP("BE",I50:BC$68,$A$68-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("B",I50:BC$68,$A$68-$A50+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I50:BC$70,$A$70-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("B",I50:BC$70,$A$70-$A50+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="G50" s="11">
-        <f>IFERROR( HLOOKUP("BE",I50:BC$68,$A$68-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("E",I50:BC$68,$A$68-$A50+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I50:BC$70,$A$70-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("E",I50:BC$70,$A$70-$A50+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -5161,24 +4485,40 @@
         <v>41</v>
       </c>
       <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="C51" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" s="10">
+        <v>1</v>
+      </c>
       <c r="F51" s="11">
-        <f>IFERROR( HLOOKUP("BE",I51:BC$68,$A$68-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("B",I51:BC$68,$A$68-$A51+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I51:BC$70,$A$70-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("B",I51:BC$70,$A$70-$A51+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="G51" s="11">
-        <f>IFERROR( HLOOKUP("BE",I51:BC$68,$A$68-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("E",I51:BC$68,$A$68-$A51+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",I51:BC$70,$A$70-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("E",I51:BC$70,$A$70-$A51+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
+      <c r="J51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
@@ -5230,11 +4570,11 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="11">
-        <f>IFERROR( HLOOKUP("BE",I52:BC$68,$A$68-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("B",I52:BC$68,$A$68-$A52+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I52:BC$70,$A$70-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("B",I52:BC$70,$A$70-$A52+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G52" s="11">
-        <f>IFERROR( HLOOKUP("BE",I52:BC$68,$A$68-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("E",I52:BC$68,$A$68-$A52+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I52:BC$70,$A$70-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("E",I52:BC$70,$A$70-$A52+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H52" s="10"/>
@@ -5295,11 +4635,11 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="11">
-        <f>IFERROR( HLOOKUP("BE",I53:BC$68,$A$68-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("B",I53:BC$68,$A$68-$A53+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I53:BC$70,$A$70-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("B",I53:BC$70,$A$70-$A53+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G53" s="11">
-        <f>IFERROR( HLOOKUP("BE",I53:BC$68,$A$68-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("E",I53:BC$68,$A$68-$A53+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I53:BC$70,$A$70-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("E",I53:BC$70,$A$70-$A53+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H53" s="10"/>
@@ -5360,11 +4700,11 @@
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="11">
-        <f>IFERROR( HLOOKUP("BE",I54:BC$68,$A$68-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("B",I54:BC$68,$A$68-$A54+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I54:BC$70,$A$70-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("B",I54:BC$70,$A$70-$A54+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G54" s="11">
-        <f>IFERROR( HLOOKUP("BE",I54:BC$68,$A$68-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("E",I54:BC$68,$A$68-$A54+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I54:BC$70,$A$70-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("E",I54:BC$70,$A$70-$A54+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H54" s="10"/>
@@ -5425,11 +4765,11 @@
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="11">
-        <f>IFERROR( HLOOKUP("BE",I55:BC$68,$A$68-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("B",I55:BC$68,$A$68-$A55+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I55:BC$70,$A$70-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("B",I55:BC$70,$A$70-$A55+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G55" s="11">
-        <f>IFERROR( HLOOKUP("BE",I55:BC$68,$A$68-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("E",I55:BC$68,$A$68-$A55+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I55:BC$70,$A$70-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("E",I55:BC$70,$A$70-$A55+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H55" s="10"/>
@@ -5490,11 +4830,11 @@
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
       <c r="F56" s="11">
-        <f>IFERROR( HLOOKUP("BE",I56:BC$68,$A$68-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("B",I56:BC$68,$A$68-$A56+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I56:BC$70,$A$70-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("B",I56:BC$70,$A$70-$A56+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G56" s="11">
-        <f>IFERROR( HLOOKUP("BE",I56:BC$68,$A$68-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("E",I56:BC$68,$A$68-$A56+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I56:BC$70,$A$70-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("E",I56:BC$70,$A$70-$A56+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H56" s="10"/>
@@ -5555,11 +4895,11 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="11">
-        <f>IFERROR( HLOOKUP("BE",I57:BC$68,$A$68-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("B",I57:BC$68,$A$68-$A57+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I57:BC$70,$A$70-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("B",I57:BC$70,$A$70-$A57+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G57" s="11">
-        <f>IFERROR( HLOOKUP("BE",I57:BC$68,$A$68-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("E",I57:BC$68,$A$68-$A57+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I57:BC$70,$A$70-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("E",I57:BC$70,$A$70-$A57+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H57" s="10"/>
@@ -5620,11 +4960,11 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="11">
-        <f>IFERROR( HLOOKUP("BE",I58:BC$68,$A$68-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("B",I58:BC$68,$A$68-$A58+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I58:BC$70,$A$70-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("B",I58:BC$70,$A$70-$A58+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G58" s="11">
-        <f>IFERROR( HLOOKUP("BE",I58:BC$68,$A$68-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("E",I58:BC$68,$A$68-$A58+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I58:BC$70,$A$70-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("E",I58:BC$70,$A$70-$A58+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H58" s="10"/>
@@ -5685,11 +5025,11 @@
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="11">
-        <f>IFERROR( HLOOKUP("BE",I59:BC$68,$A$68-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",I59:BC$68,$A$68-$A59+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I59:BC$70,$A$70-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",I59:BC$70,$A$70-$A59+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G59" s="11">
-        <f>IFERROR( HLOOKUP("BE",I59:BC$68,$A$68-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",I59:BC$68,$A$68-$A59+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I59:BC$70,$A$70-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",I59:BC$70,$A$70-$A59+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H59" s="10"/>
@@ -5750,11 +5090,11 @@
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="11">
-        <f>IFERROR( HLOOKUP("BE",I60:BC$68,$A$68-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("B",I60:BC$68,$A$68-$A60+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I60:BC$70,$A$70-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("B",I60:BC$70,$A$70-$A60+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G60" s="11">
-        <f>IFERROR( HLOOKUP("BE",I60:BC$68,$A$68-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("E",I60:BC$68,$A$68-$A60+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I60:BC$70,$A$70-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("E",I60:BC$70,$A$70-$A60+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H60" s="10"/>
@@ -5815,11 +5155,11 @@
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
       <c r="F61" s="11">
-        <f>IFERROR( HLOOKUP("BE",I61:BC$68,$A$68-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("B",I61:BC$68,$A$68-$A61+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I61:BC$70,$A$70-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("B",I61:BC$70,$A$70-$A61+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G61" s="11">
-        <f>IFERROR( HLOOKUP("BE",I61:BC$68,$A$68-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("E",I61:BC$68,$A$68-$A61+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I61:BC$70,$A$70-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("E",I61:BC$70,$A$70-$A61+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H61" s="10"/>
@@ -5880,11 +5220,11 @@
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
       <c r="F62" s="11">
-        <f>IFERROR( HLOOKUP("BE",I62:BC$68,$A$68-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",I62:BC$68,$A$68-$A62+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I62:BC$70,$A$70-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",I62:BC$70,$A$70-$A62+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G62" s="11">
-        <f>IFERROR( HLOOKUP("BE",I62:BC$68,$A$68-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",I62:BC$68,$A$68-$A62+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I62:BC$70,$A$70-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",I62:BC$70,$A$70-$A62+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H62" s="10"/>
@@ -5945,11 +5285,11 @@
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="11">
-        <f>IFERROR( HLOOKUP("BE",I63:BC$68,$A$68-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",I63:BC$68,$A$68-$A63+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I63:BC$70,$A$70-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",I63:BC$70,$A$70-$A63+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G63" s="11">
-        <f>IFERROR( HLOOKUP("BE",I63:BC$68,$A$68-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",I63:BC$68,$A$68-$A63+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I63:BC$70,$A$70-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",I63:BC$70,$A$70-$A63+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H63" s="10"/>
@@ -6010,11 +5350,11 @@
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="11">
-        <f>IFERROR( HLOOKUP("BE",I64:BC$68,$A$68-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("B",I64:BC$68,$A$68-$A64+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I64:BC$70,$A$70-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("B",I64:BC$70,$A$70-$A64+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G64" s="11">
-        <f>IFERROR( HLOOKUP("BE",I64:BC$68,$A$68-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("E",I64:BC$68,$A$68-$A64+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",I64:BC$70,$A$70-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("E",I64:BC$70,$A$70-$A64+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H64" s="10"/>
@@ -6070,264 +5410,394 @@
       <c r="A65">
         <v>55</v>
       </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="11">
+        <f>IFERROR( HLOOKUP("BE",I65:BC$70,$A$70-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("B",I65:BC$70,$A$70-$A65+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G65" s="11">
+        <f>IFERROR( HLOOKUP("BE",I65:BC$70,$A$70-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("E",I65:BC$70,$A$70-$A65+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="10"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+      <c r="AD65" s="1"/>
+      <c r="AE65" s="1"/>
+      <c r="AF65" s="1"/>
+      <c r="AG65" s="1"/>
+      <c r="AH65" s="1"/>
+      <c r="AI65" s="1"/>
+      <c r="AJ65" s="1"/>
+      <c r="AK65" s="1"/>
+      <c r="AL65" s="1"/>
+      <c r="AM65" s="1"/>
+      <c r="AN65" s="1"/>
+      <c r="AO65" s="1"/>
+      <c r="AP65" s="1"/>
+      <c r="AQ65" s="1"/>
+      <c r="AR65" s="1"/>
+      <c r="AS65" s="1"/>
+      <c r="AT65" s="1"/>
+      <c r="AU65" s="1"/>
+      <c r="AV65" s="1"/>
+      <c r="AW65" s="1"/>
+      <c r="AX65" s="1"/>
+      <c r="AY65" s="1"/>
+      <c r="AZ65" s="1"/>
+      <c r="BA65" s="1"/>
+      <c r="BB65" s="1"/>
+      <c r="BC65" s="1"/>
     </row>
     <row r="66" spans="1:55">
       <c r="A66">
         <v>56</v>
       </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="11">
+        <f>IFERROR( HLOOKUP("BE",I66:BC$70,$A$70-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("B",I66:BC$70,$A$70-$A66+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="11">
+        <f>IFERROR( HLOOKUP("BE",I66:BC$70,$A$70-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("E",I66:BC$70,$A$70-$A66+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="10"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+      <c r="AF66" s="1"/>
+      <c r="AG66" s="1"/>
+      <c r="AH66" s="1"/>
+      <c r="AI66" s="1"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+      <c r="AL66" s="1"/>
+      <c r="AM66" s="1"/>
+      <c r="AN66" s="1"/>
+      <c r="AO66" s="1"/>
+      <c r="AP66" s="1"/>
+      <c r="AQ66" s="1"/>
+      <c r="AR66" s="1"/>
+      <c r="AS66" s="1"/>
+      <c r="AT66" s="1"/>
+      <c r="AU66" s="1"/>
+      <c r="AV66" s="1"/>
+      <c r="AW66" s="1"/>
+      <c r="AX66" s="1"/>
+      <c r="AY66" s="1"/>
+      <c r="AZ66" s="1"/>
+      <c r="BA66" s="1"/>
+      <c r="BB66" s="1"/>
+      <c r="BC66" s="1"/>
     </row>
     <row r="67" spans="1:55">
       <c r="A67">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:55" s="17" customFormat="1">
+    <row r="68" spans="1:55">
       <c r="A68">
         <v>58</v>
       </c>
-      <c r="C68" s="17" t="s">
+    </row>
+    <row r="69" spans="1:55">
+      <c r="A69">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:55" s="17" customFormat="1">
+      <c r="A70">
+        <v>60</v>
+      </c>
+      <c r="C70" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="I68" s="12">
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="I70" s="12">
         <f>I8</f>
         <v>40770</v>
       </c>
-      <c r="J68" s="12">
-        <f t="shared" ref="J68:BC68" si="1">J8</f>
+      <c r="J70" s="12">
+        <f t="shared" ref="J70:BC70" si="1">J8</f>
         <v>40771</v>
       </c>
-      <c r="K68" s="12">
+      <c r="K70" s="12">
         <f t="shared" si="1"/>
         <v>40772</v>
       </c>
-      <c r="L68" s="12">
+      <c r="L70" s="12">
         <f t="shared" si="1"/>
         <v>40773</v>
       </c>
-      <c r="M68" s="12">
+      <c r="M70" s="12">
         <f t="shared" si="1"/>
         <v>40774</v>
       </c>
-      <c r="N68" s="12">
+      <c r="N70" s="12">
         <f t="shared" si="1"/>
         <v>40775</v>
       </c>
-      <c r="O68" s="12">
+      <c r="O70" s="12">
         <f t="shared" si="1"/>
         <v>40776</v>
       </c>
-      <c r="P68" s="12">
+      <c r="P70" s="12">
         <f t="shared" si="1"/>
         <v>40777</v>
       </c>
-      <c r="Q68" s="12">
+      <c r="Q70" s="12">
         <f t="shared" si="1"/>
         <v>40778</v>
       </c>
-      <c r="R68" s="12">
+      <c r="R70" s="12">
         <f t="shared" si="1"/>
         <v>40779</v>
       </c>
-      <c r="S68" s="12">
+      <c r="S70" s="12">
         <f t="shared" si="1"/>
         <v>40780</v>
       </c>
-      <c r="T68" s="12">
+      <c r="T70" s="12">
         <f t="shared" si="1"/>
         <v>40781</v>
       </c>
-      <c r="U68" s="12">
+      <c r="U70" s="12">
         <f t="shared" si="1"/>
         <v>40782</v>
       </c>
-      <c r="V68" s="12">
+      <c r="V70" s="12">
         <f t="shared" si="1"/>
         <v>40783</v>
       </c>
-      <c r="W68" s="12">
+      <c r="W70" s="12">
         <f t="shared" si="1"/>
         <v>40784</v>
       </c>
-      <c r="X68" s="12">
+      <c r="X70" s="12">
         <f t="shared" si="1"/>
         <v>40785</v>
       </c>
-      <c r="Y68" s="12">
+      <c r="Y70" s="12">
         <f t="shared" si="1"/>
         <v>40786</v>
       </c>
-      <c r="Z68" s="12">
+      <c r="Z70" s="12">
         <f t="shared" si="1"/>
         <v>40787</v>
       </c>
-      <c r="AA68" s="12">
+      <c r="AA70" s="12">
         <f t="shared" si="1"/>
         <v>40788</v>
       </c>
-      <c r="AB68" s="12">
+      <c r="AB70" s="12">
         <f t="shared" si="1"/>
         <v>40789</v>
       </c>
-      <c r="AC68" s="12">
+      <c r="AC70" s="12">
         <f t="shared" si="1"/>
         <v>40790</v>
       </c>
-      <c r="AD68" s="12">
+      <c r="AD70" s="12">
         <f t="shared" si="1"/>
         <v>40791</v>
       </c>
-      <c r="AE68" s="12">
+      <c r="AE70" s="12">
         <f t="shared" si="1"/>
         <v>40792</v>
       </c>
-      <c r="AF68" s="12">
+      <c r="AF70" s="12">
         <f t="shared" si="1"/>
         <v>40793</v>
       </c>
-      <c r="AG68" s="12">
+      <c r="AG70" s="12">
         <f t="shared" si="1"/>
         <v>40794</v>
       </c>
-      <c r="AH68" s="12">
+      <c r="AH70" s="12">
         <f t="shared" si="1"/>
         <v>40795</v>
       </c>
-      <c r="AI68" s="12">
+      <c r="AI70" s="12">
         <f t="shared" si="1"/>
         <v>40796</v>
       </c>
-      <c r="AJ68" s="12">
+      <c r="AJ70" s="12">
         <f t="shared" si="1"/>
         <v>40797</v>
       </c>
-      <c r="AK68" s="12">
+      <c r="AK70" s="12">
         <f t="shared" si="1"/>
         <v>40798</v>
       </c>
-      <c r="AL68" s="12">
+      <c r="AL70" s="12">
         <f t="shared" si="1"/>
         <v>40799</v>
       </c>
-      <c r="AM68" s="12">
+      <c r="AM70" s="12">
         <f t="shared" si="1"/>
         <v>40800</v>
       </c>
-      <c r="AN68" s="12">
+      <c r="AN70" s="12">
         <f t="shared" si="1"/>
         <v>40801</v>
       </c>
-      <c r="AO68" s="12">
+      <c r="AO70" s="12">
         <f t="shared" si="1"/>
         <v>40802</v>
       </c>
-      <c r="AP68" s="12">
+      <c r="AP70" s="12">
         <f t="shared" si="1"/>
         <v>40803</v>
       </c>
-      <c r="AQ68" s="12">
+      <c r="AQ70" s="12">
         <f t="shared" si="1"/>
         <v>40804</v>
       </c>
-      <c r="AR68" s="12">
+      <c r="AR70" s="12">
         <f t="shared" si="1"/>
         <v>40805</v>
       </c>
-      <c r="AS68" s="12">
+      <c r="AS70" s="12">
         <f t="shared" si="1"/>
         <v>40806</v>
       </c>
-      <c r="AT68" s="12">
+      <c r="AT70" s="12">
         <f t="shared" si="1"/>
         <v>40807</v>
       </c>
-      <c r="AU68" s="12">
+      <c r="AU70" s="12">
         <f t="shared" si="1"/>
         <v>40808</v>
       </c>
-      <c r="AV68" s="12">
+      <c r="AV70" s="12">
         <f t="shared" si="1"/>
         <v>40809</v>
       </c>
-      <c r="AW68" s="12">
+      <c r="AW70" s="12">
         <f t="shared" si="1"/>
         <v>40810</v>
       </c>
-      <c r="AX68" s="12">
+      <c r="AX70" s="12">
         <f t="shared" si="1"/>
         <v>40811</v>
       </c>
-      <c r="AY68" s="12">
+      <c r="AY70" s="12">
         <f t="shared" si="1"/>
         <v>40812</v>
       </c>
-      <c r="AZ68" s="12">
+      <c r="AZ70" s="12">
         <f t="shared" si="1"/>
         <v>40813</v>
       </c>
-      <c r="BA68" s="12">
+      <c r="BA70" s="12">
         <f t="shared" si="1"/>
         <v>40814</v>
       </c>
-      <c r="BB68" s="12">
+      <c r="BB70" s="12">
         <f t="shared" si="1"/>
         <v>40815</v>
       </c>
-      <c r="BC68" s="12">
+      <c r="BC70" s="12">
         <f t="shared" si="1"/>
         <v>40816</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A9:BC68">
+  <autoFilter ref="A9:BC70">
     <filterColumn colId="4"/>
   </autoFilter>
-  <conditionalFormatting sqref="I48:AV65 I10:BC12 I26:BC35 I37:BC46 I16:BC24 I48:BC64">
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+  <conditionalFormatting sqref="I50:AV67 I10:BC12 I28:BC37 I39:BC48 I16:BC26 I50:BC66">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BC12 I26:BC35 I37:BC46 I16:BC24 I48:BC64">
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+  <conditionalFormatting sqref="I10:BC12 I28:BC37 I39:BC48 I16:BC26 I50:BC66">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:BC14">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:BC14">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
chỉnh sửa file plan
</commit_message>
<xml_diff>
--- a/Document/sale_project v2011.08.20.xlsx
+++ b/Document/sale_project v2011.08.20.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="85">
   <si>
     <t>STT</t>
   </si>
@@ -261,12 +261,6 @@
   </si>
   <si>
     <t>Hung</t>
-  </si>
-  <si>
-    <t>TuND</t>
-  </si>
-  <si>
-    <t>MinhNN</t>
   </si>
   <si>
     <t>Quản lý khách hàng master</t>
@@ -1177,10 +1171,10 @@
   <dimension ref="A1:BC70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1239,7 +1233,7 @@
       </c>
       <c r="D5" s="22">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="22"/>
     </row>
@@ -1259,7 +1253,7 @@
       </c>
       <c r="D7" s="22">
         <f t="shared" si="0"/>
-        <v>12.6</v>
+        <v>12</v>
       </c>
       <c r="E7" s="22"/>
     </row>
@@ -2401,10 +2395,10 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E22" s="10">
         <v>0.4</v>
@@ -2474,10 +2468,10 @@
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E23" s="10">
         <v>0.6</v>
@@ -2557,7 +2551,7 @@
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>80</v>
@@ -2630,7 +2624,7 @@
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>72</v>
@@ -4416,7 +4410,7 @@
         <v>64</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="E50" s="10">
         <v>2</v>
@@ -4489,7 +4483,7 @@
         <v>65</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E51" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
sua tên form mọi người cứ theo đó mà đặt tên
</commit_message>
<xml_diff>
--- a/Document/sale_project v2011.08.20.xlsx
+++ b/Document/sale_project v2011.08.20.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan!$A$10:$BD$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan!$A$10:$BE$70</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="118">
   <si>
     <t>STT</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Báo cáo nhập, xuất, tồn kho</t>
   </si>
   <si>
-    <t>Nhập số dư đầu</t>
-  </si>
-  <si>
     <t>Báo cáo tổng hợp xuất nhập tồn</t>
   </si>
   <si>
@@ -300,6 +297,81 @@
   </si>
   <si>
     <t>Mẫu báo cáo dạng excel (nhập xuất tồn, …)</t>
+  </si>
+  <si>
+    <t>Số form</t>
+  </si>
+  <si>
+    <t>f701</t>
+  </si>
+  <si>
+    <t>f901</t>
+  </si>
+  <si>
+    <t>f301</t>
+  </si>
+  <si>
+    <t>f201</t>
+  </si>
+  <si>
+    <t>f801</t>
+  </si>
+  <si>
+    <t>f601</t>
+  </si>
+  <si>
+    <t>f501</t>
+  </si>
+  <si>
+    <t>f401</t>
+  </si>
+  <si>
+    <t>f321</t>
+  </si>
+  <si>
+    <t>f311</t>
+  </si>
+  <si>
+    <t>f331</t>
+  </si>
+  <si>
+    <t>f341</t>
+  </si>
+  <si>
+    <t>f351</t>
+  </si>
+  <si>
+    <t>f361</t>
+  </si>
+  <si>
+    <t>f371</t>
+  </si>
+  <si>
+    <t>f381</t>
+  </si>
+  <si>
+    <t>f911</t>
+  </si>
+  <si>
+    <t>f921</t>
+  </si>
+  <si>
+    <t>f931</t>
+  </si>
+  <si>
+    <t>f932</t>
+  </si>
+  <si>
+    <t>f941</t>
+  </si>
+  <si>
+    <t>f951</t>
+  </si>
+  <si>
+    <t>f961</t>
+  </si>
+  <si>
+    <t>f998, f999</t>
   </si>
 </sst>
 </file>
@@ -1129,13 +1201,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD71"/>
+  <dimension ref="A1:BE70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1146,63 +1218,63 @@
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10" style="9" customWidth="1"/>
-    <col min="10" max="56" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="57" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:57">
       <c r="C1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:56">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57">
       <c r="C2" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="22">
-        <f>SUMIF($D$10:$D$67,C2,$E$10:$E$67)</f>
+        <f t="shared" ref="D2:D7" si="0">SUMIF($D$10:$D$66,C2,$E$10:$E$66)</f>
         <v>6</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:56">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57">
       <c r="C3" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="22">
-        <f t="shared" ref="D3:D7" si="0">SUMIF($D$10:$D$67,C3,$E$10:$E$67)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57">
       <c r="C4" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="22">
         <f t="shared" si="0"/>
-        <v>10.4</v>
+        <v>7.4</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:56">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57">
       <c r="C5" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="22">
         <f t="shared" si="0"/>
@@ -1210,12 +1282,12 @@
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:56">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:57">
       <c r="C6" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="22">
         <f t="shared" si="0"/>
@@ -1223,9 +1295,9 @@
       </c>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:56">
+    <row r="7" spans="1:57">
       <c r="C7" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="22">
         <f t="shared" si="0"/>
@@ -1233,11 +1305,11 @@
       </c>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:56">
+    <row r="8" spans="1:57">
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:56" s="16" customFormat="1" ht="30">
+    <row r="9" spans="1:57" s="16" customFormat="1" ht="30">
       <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1320,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>25</v>
@@ -1257,154 +1329,157 @@
         <v>23</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="15">
         <v>40770</v>
       </c>
-      <c r="K9" s="15">
+      <c r="L9" s="15">
         <v>40771</v>
       </c>
-      <c r="L9" s="15">
+      <c r="M9" s="15">
         <v>40772</v>
       </c>
-      <c r="M9" s="15">
+      <c r="N9" s="15">
         <v>40773</v>
       </c>
-      <c r="N9" s="15">
+      <c r="O9" s="15">
         <v>40774</v>
       </c>
-      <c r="O9" s="15">
+      <c r="P9" s="15">
         <v>40775</v>
       </c>
-      <c r="P9" s="15">
+      <c r="Q9" s="15">
         <v>40776</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="R9" s="15">
         <v>40777</v>
       </c>
-      <c r="R9" s="15">
+      <c r="S9" s="15">
         <v>40778</v>
       </c>
-      <c r="S9" s="15">
+      <c r="T9" s="15">
         <v>40779</v>
       </c>
-      <c r="T9" s="15">
+      <c r="U9" s="15">
         <v>40780</v>
       </c>
-      <c r="U9" s="15">
+      <c r="V9" s="15">
         <v>40781</v>
       </c>
-      <c r="V9" s="15">
+      <c r="W9" s="15">
         <v>40782</v>
       </c>
-      <c r="W9" s="15">
+      <c r="X9" s="15">
         <v>40783</v>
       </c>
-      <c r="X9" s="15">
+      <c r="Y9" s="15">
         <v>40784</v>
       </c>
-      <c r="Y9" s="15">
+      <c r="Z9" s="15">
         <v>40785</v>
       </c>
-      <c r="Z9" s="15">
+      <c r="AA9" s="15">
         <v>40786</v>
       </c>
-      <c r="AA9" s="15">
+      <c r="AB9" s="15">
         <v>40787</v>
       </c>
-      <c r="AB9" s="15">
+      <c r="AC9" s="15">
         <v>40788</v>
       </c>
-      <c r="AC9" s="15">
+      <c r="AD9" s="15">
         <v>40789</v>
       </c>
-      <c r="AD9" s="15">
+      <c r="AE9" s="15">
         <v>40790</v>
       </c>
-      <c r="AE9" s="15">
+      <c r="AF9" s="15">
         <v>40791</v>
       </c>
-      <c r="AF9" s="15">
+      <c r="AG9" s="15">
         <v>40792</v>
       </c>
-      <c r="AG9" s="15">
+      <c r="AH9" s="15">
         <v>40793</v>
       </c>
-      <c r="AH9" s="15">
+      <c r="AI9" s="15">
         <v>40794</v>
       </c>
-      <c r="AI9" s="15">
+      <c r="AJ9" s="15">
         <v>40795</v>
       </c>
-      <c r="AJ9" s="15">
+      <c r="AK9" s="15">
         <v>40796</v>
       </c>
-      <c r="AK9" s="15">
+      <c r="AL9" s="15">
         <v>40797</v>
       </c>
-      <c r="AL9" s="15">
+      <c r="AM9" s="15">
         <v>40798</v>
       </c>
-      <c r="AM9" s="15">
+      <c r="AN9" s="15">
         <v>40799</v>
       </c>
-      <c r="AN9" s="15">
+      <c r="AO9" s="15">
         <v>40800</v>
       </c>
-      <c r="AO9" s="15">
+      <c r="AP9" s="15">
         <v>40801</v>
       </c>
-      <c r="AP9" s="15">
+      <c r="AQ9" s="15">
         <v>40802</v>
       </c>
-      <c r="AQ9" s="15">
+      <c r="AR9" s="15">
         <v>40803</v>
       </c>
-      <c r="AR9" s="15">
+      <c r="AS9" s="15">
         <v>40804</v>
       </c>
-      <c r="AS9" s="15">
+      <c r="AT9" s="15">
         <v>40805</v>
       </c>
-      <c r="AT9" s="15">
+      <c r="AU9" s="15">
         <v>40806</v>
       </c>
-      <c r="AU9" s="15">
+      <c r="AV9" s="15">
         <v>40807</v>
       </c>
-      <c r="AV9" s="15">
+      <c r="AW9" s="15">
         <v>40808</v>
       </c>
-      <c r="AW9" s="15">
+      <c r="AX9" s="15">
         <v>40809</v>
       </c>
-      <c r="AX9" s="15">
+      <c r="AY9" s="15">
         <v>40810</v>
       </c>
-      <c r="AY9" s="15">
+      <c r="AZ9" s="15">
         <v>40811</v>
       </c>
-      <c r="AZ9" s="15">
+      <c r="BA9" s="15">
         <v>40812</v>
       </c>
-      <c r="BA9" s="15">
+      <c r="BB9" s="15">
         <v>40813</v>
       </c>
-      <c r="BB9" s="15">
+      <c r="BC9" s="15">
         <v>40814</v>
       </c>
-      <c r="BC9" s="15">
+      <c r="BD9" s="15">
         <v>40815</v>
       </c>
-      <c r="BD9" s="15">
+      <c r="BE9" s="15">
         <v>40816</v>
       </c>
     </row>
-    <row r="10" spans="1:56" s="14" customFormat="1">
+    <row r="10" spans="1:57" s="14" customFormat="1">
       <c r="B10" s="13"/>
       <c r="C10" s="13" t="s">
         <v>27</v>
@@ -1462,8 +1537,9 @@
       <c r="BB10" s="13"/>
       <c r="BC10" s="13"/>
       <c r="BD10" s="13"/>
-    </row>
-    <row r="11" spans="1:56">
+      <c r="BE10" s="13"/>
+    </row>
+    <row r="11" spans="1:57">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1478,34 +1554,34 @@
         <v>3</v>
       </c>
       <c r="F11" s="11">
-        <f>IFERROR( HLOOKUP("BE",J11:BD$71,$A$71-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",J11:BD$71,$A$71-$A11+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",K11:BE$70,$A$70-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",K11:BE$70,$A$70-$A11+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G11" s="11">
-        <f>IFERROR( HLOOKUP("BE",J11:BD$71,$A$71-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",J11:BD$71,$A$71-$A11+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",K11:BE$70,$A$70-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",K11:BE$70,$A$70-$A11+1,FALSE),0)</f>
+        <v>40775</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="10"/>
+      <c r="K11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -1546,8 +1622,9 @@
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
       <c r="BD11" s="1"/>
-    </row>
-    <row r="12" spans="1:56">
+      <c r="BE11" s="1"/>
+    </row>
+    <row r="12" spans="1:57">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1556,25 +1633,25 @@
         <v>29</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="10">
         <v>3</v>
       </c>
       <c r="F12" s="11">
-        <f>IFERROR( HLOOKUP("BE",J12:BD$71,$A$71-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("B",J12:BD$71,$A$71-$A12+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",K12:BE$70,$A$70-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("B",K12:BE$70,$A$70-$A12+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="G12" s="11">
-        <f>IFERROR( HLOOKUP("BE",J12:BD$71,$A$71-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("E",J12:BD$71,$A$71-$A12+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",K12:BE$70,$A$70-$A12+1,FALSE),0)+ IFERROR( HLOOKUP("E",K12:BE$70,$A$70-$A12+1,FALSE),0)</f>
+        <v>40770</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="1"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1620,8 +1697,9 @@
       <c r="BB12" s="1"/>
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
-    </row>
-    <row r="13" spans="1:56">
+      <c r="BE12" s="1"/>
+    </row>
+    <row r="13" spans="1:57">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1636,20 +1714,20 @@
         <v>1</v>
       </c>
       <c r="F13" s="11">
-        <f>IFERROR( HLOOKUP("BE",J13:BD$71,$A$71-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("B",J13:BD$71,$A$71-$A13+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",K13:BE$70,$A$70-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("B",K13:BE$70,$A$70-$A13+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="G13" s="11">
-        <f>IFERROR( HLOOKUP("BE",J13:BD$71,$A$71-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("E",J13:BD$71,$A$71-$A13+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",K13:BE$70,$A$70-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("E",K13:BE$70,$A$70-$A13+1,FALSE),0)</f>
+        <v>40771</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="1"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1694,8 +1772,9 @@
       <c r="BB13" s="1"/>
       <c r="BC13" s="1"/>
       <c r="BD13" s="1"/>
-    </row>
-    <row r="14" spans="1:56" s="14" customFormat="1">
+      <c r="BE13" s="1"/>
+    </row>
+    <row r="14" spans="1:57" s="14" customFormat="1">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1756,37 +1835,38 @@
       <c r="BB14" s="13"/>
       <c r="BC14" s="13"/>
       <c r="BD14" s="13"/>
-    </row>
-    <row r="15" spans="1:56" s="28" customFormat="1">
+      <c r="BE14" s="13"/>
+    </row>
+    <row r="15" spans="1:57" s="28" customFormat="1">
       <c r="A15" s="23"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="24">
         <v>2</v>
       </c>
       <c r="F15" s="25">
-        <f>IFERROR( HLOOKUP("BE",J15:BD$71,$A$71-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("B",J15:BD$71,$A$71-$A15+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K15:BE$70,$A$70-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("B",K15:BE$70,$A$70-$A15+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G15" s="25">
-        <f>IFERROR( HLOOKUP("BE",J15:BD$71,$A$71-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("E",J15:BD$71,$A$71-$A15+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K15:BE$70,$A$70-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("E",K15:BE$70,$A$70-$A15+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="J15" s="26"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
-      <c r="N15" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="O15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27" t="s">
+        <v>66</v>
+      </c>
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
@@ -1828,8 +1908,9 @@
       <c r="BB15" s="27"/>
       <c r="BC15" s="27"/>
       <c r="BD15" s="27"/>
-    </row>
-    <row r="16" spans="1:56" s="14" customFormat="1">
+      <c r="BE15" s="27"/>
+    </row>
+    <row r="16" spans="1:57" s="14" customFormat="1">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1890,50 +1971,53 @@
       <c r="BB16" s="13"/>
       <c r="BC16" s="13"/>
       <c r="BD16" s="13"/>
-    </row>
-    <row r="17" spans="1:56">
+      <c r="BE16" s="13"/>
+    </row>
+    <row r="17" spans="1:57">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
       </c>
       <c r="F17" s="11">
-        <f>IFERROR( HLOOKUP("BE",J17:BD$71,$A$71-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("B",J17:BD$71,$A$71-$A17+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K17:BE$70,$A$70-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("B",K17:BE$70,$A$70-$A17+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G17" s="11">
-        <f>IFERROR( HLOOKUP("BE",J17:BD$71,$A$71-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("E",J17:BD$71,$A$71-$A17+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K17:BE$70,$A$70-$A17+1,FALSE),0)+ IFERROR( HLOOKUP("E",K17:BE$70,$A$70-$A17+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1974,50 +2058,53 @@
       <c r="BB17" s="1"/>
       <c r="BC17" s="1"/>
       <c r="BD17" s="1"/>
-    </row>
-    <row r="18" spans="1:56">
+      <c r="BE17" s="1"/>
+    </row>
+    <row r="18" spans="1:57">
       <c r="A18">
         <v>7</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" s="10">
         <v>1</v>
       </c>
       <c r="F18" s="11">
-        <f>IFERROR( HLOOKUP("BE",J18:BD$71,$A$71-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",J18:BD$71,$A$71-$A18+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K18:BE$70,$A$70-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",K18:BE$70,$A$70-$A18+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G18" s="11">
-        <f>IFERROR( HLOOKUP("BE",J18:BD$71,$A$71-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",J18:BD$71,$A$71-$A18+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K18:BE$70,$A$70-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",K18:BE$70,$A$70-$A18+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -2058,14 +2145,15 @@
       <c r="BB18" s="1"/>
       <c r="BC18" s="1"/>
       <c r="BD18" s="1"/>
-    </row>
-    <row r="19" spans="1:56">
+      <c r="BE18" s="1"/>
+    </row>
+    <row r="19" spans="1:57">
       <c r="A19">
         <v>8</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>31</v>
@@ -2074,37 +2162,39 @@
         <v>1</v>
       </c>
       <c r="F19" s="11">
-        <f>IFERROR( HLOOKUP("BE",J19:BD$71,$A$71-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",J19:BD$71,$A$71-$A19+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K19:BE$70,$A$70-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",K19:BE$70,$A$70-$A19+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G19" s="11">
-        <f>IFERROR( HLOOKUP("BE",J19:BD$71,$A$71-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",J19:BD$71,$A$71-$A19+1,FALSE),0)</f>
-        <v>40776</v>
+        <f>IFERROR( HLOOKUP("BE",K19:BE$70,$A$70-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",K19:BE$70,$A$70-$A19+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -2144,14 +2234,15 @@
       <c r="BB19" s="1"/>
       <c r="BC19" s="1"/>
       <c r="BD19" s="1"/>
-    </row>
-    <row r="20" spans="1:56">
+      <c r="BE19" s="1"/>
+    </row>
+    <row r="20" spans="1:57">
       <c r="A20">
         <v>9</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>26</v>
@@ -2160,19 +2251,21 @@
         <v>1</v>
       </c>
       <c r="F20" s="11">
-        <f>IFERROR( HLOOKUP("BE",J20:BD$71,$A$71-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",J20:BD$71,$A$71-$A20+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K20:BE$70,$A$70-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",K20:BE$70,$A$70-$A20+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G20" s="11">
-        <f>IFERROR( HLOOKUP("BE",J20:BD$71,$A$71-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",J20:BD$71,$A$71-$A20+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K20:BE$70,$A$70-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",K20:BE$70,$A$70-$A20+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="1"/>
+      <c r="J20" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -2218,50 +2311,53 @@
       <c r="BB20" s="1"/>
       <c r="BC20" s="1"/>
       <c r="BD20" s="1"/>
-    </row>
-    <row r="21" spans="1:56">
+      <c r="BE20" s="1"/>
+    </row>
+    <row r="21" spans="1:57">
       <c r="A21">
         <v>10</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="10">
         <v>1</v>
       </c>
       <c r="F21" s="11">
-        <f>IFERROR( HLOOKUP("BE",J21:BD$71,$A$71-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",J21:BD$71,$A$71-$A21+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K21:BE$70,$A$70-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",K21:BE$70,$A$70-$A21+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G21" s="11">
-        <f>IFERROR( HLOOKUP("BE",J21:BD$71,$A$71-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",J21:BD$71,$A$71-$A21+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K21:BE$70,$A$70-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",K21:BE$70,$A$70-$A21+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2302,14 +2398,15 @@
       <c r="BB21" s="1"/>
       <c r="BC21" s="1"/>
       <c r="BD21" s="1"/>
-    </row>
-    <row r="22" spans="1:56">
+      <c r="BE21" s="1"/>
+    </row>
+    <row r="22" spans="1:57">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>31</v>
@@ -2318,34 +2415,34 @@
         <v>1</v>
       </c>
       <c r="F22" s="11">
-        <f>IFERROR( HLOOKUP("BE",J22:BD$71,$A$71-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",J22:BD$71,$A$71-$A22+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K22:BE$70,$A$70-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",K22:BE$70,$A$70-$A22+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G22" s="11">
-        <f>IFERROR( HLOOKUP("BE",J22:BD$71,$A$71-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",J22:BD$71,$A$71-$A22+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K22:BE$70,$A$70-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",K22:BE$70,$A$70-$A22+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="10"/>
+      <c r="K22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2386,39 +2483,42 @@
       <c r="BB22" s="1"/>
       <c r="BC22" s="1"/>
       <c r="BD22" s="1"/>
-    </row>
-    <row r="23" spans="1:56">
+      <c r="BE22" s="1"/>
+    </row>
+    <row r="23" spans="1:57">
       <c r="A23">
         <v>12</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="10">
         <v>0.4</v>
       </c>
       <c r="F23" s="11">
-        <f>IFERROR( HLOOKUP("BE",J23:BD$71,$A$71-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("B",J23:BD$71,$A$71-$A23+1,FALSE),0)</f>
-        <v>40774</v>
+        <f>IFERROR( HLOOKUP("BE",K23:BE$70,$A$70-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("B",K23:BE$70,$A$70-$A23+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G23" s="11">
-        <f>IFERROR( HLOOKUP("BE",J23:BD$71,$A$71-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("E",J23:BD$71,$A$71-$A23+1,FALSE),0)</f>
-        <v>40774</v>
+        <f>IFERROR( HLOOKUP("BE",K23:BE$70,$A$70-$A23+1,FALSE),0)+ IFERROR( HLOOKUP("E",K23:BE$70,$A$70-$A23+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -2460,50 +2560,51 @@
       <c r="BB23" s="1"/>
       <c r="BC23" s="1"/>
       <c r="BD23" s="1"/>
-    </row>
-    <row r="24" spans="1:56">
+      <c r="BE23" s="1"/>
+    </row>
+    <row r="24" spans="1:57">
       <c r="A24">
         <v>13</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E24" s="10">
         <v>0.6</v>
       </c>
       <c r="F24" s="11">
-        <f>IFERROR( HLOOKUP("BE",J24:BD$71,$A$71-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",J24:BD$71,$A$71-$A24+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K24:BE$70,$A$70-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",K24:BE$70,$A$70-$A24+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G24" s="11">
-        <f>IFERROR( HLOOKUP("BE",J24:BD$71,$A$71-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",J24:BD$71,$A$71-$A24+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K24:BE$70,$A$70-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",K24:BE$70,$A$70-$A24+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="10"/>
+      <c r="K24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2544,39 +2645,42 @@
       <c r="BB24" s="1"/>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
-    </row>
-    <row r="25" spans="1:56">
+      <c r="BE24" s="1"/>
+    </row>
+    <row r="25" spans="1:57">
       <c r="A25">
         <v>14</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="10">
         <v>0.4</v>
       </c>
       <c r="F25" s="11">
-        <f>IFERROR( HLOOKUP("BE",J25:BD$71,$A$71-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("B",J25:BD$71,$A$71-$A25+1,FALSE),0)</f>
-        <v>40774</v>
+        <f>IFERROR( HLOOKUP("BE",K25:BE$70,$A$70-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("B",K25:BE$70,$A$70-$A25+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G25" s="11">
-        <f>IFERROR( HLOOKUP("BE",J25:BD$71,$A$71-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("E",J25:BD$71,$A$71-$A25+1,FALSE),0)</f>
-        <v>40774</v>
+        <f>IFERROR( HLOOKUP("BE",K25:BE$70,$A$70-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("E",K25:BE$70,$A$70-$A25+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -2618,50 +2722,51 @@
       <c r="BB25" s="1"/>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1"/>
-    </row>
-    <row r="26" spans="1:56">
+      <c r="BE25" s="1"/>
+    </row>
+    <row r="26" spans="1:57">
       <c r="A26">
         <v>15</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="10">
         <v>0.6</v>
       </c>
       <c r="F26" s="11">
-        <f>IFERROR( HLOOKUP("BE",J26:BD$71,$A$71-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",J26:BD$71,$A$71-$A26+1,FALSE),0)</f>
-        <v>40770</v>
+        <f>IFERROR( HLOOKUP("BE",K26:BE$70,$A$70-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",K26:BE$70,$A$70-$A26+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G26" s="11">
-        <f>IFERROR( HLOOKUP("BE",J26:BD$71,$A$71-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",J26:BD$71,$A$71-$A26+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K26:BE$70,$A$70-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",K26:BE$70,$A$70-$A26+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="10"/>
+      <c r="K26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2702,38 +2807,39 @@
       <c r="BB26" s="1"/>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
-    </row>
-    <row r="27" spans="1:56">
+      <c r="BE26" s="1"/>
+    </row>
+    <row r="27" spans="1:57">
       <c r="A27">
         <v>16</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
       </c>
       <c r="F27" s="11">
-        <f>IFERROR( HLOOKUP("BE",J27:BD$71,$A$71-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",J27:BD$71,$A$71-$A27+1,FALSE),0)</f>
-        <v>40773</v>
+        <f>IFERROR( HLOOKUP("BE",K27:BE$70,$A$70-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",K27:BE$70,$A$70-$A27+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G27" s="11">
-        <f>IFERROR( HLOOKUP("BE",J27:BD$71,$A$71-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",J27:BD$71,$A$71-$A27+1,FALSE),0)</f>
-        <v>40773</v>
+        <f>IFERROR( HLOOKUP("BE",K27:BE$70,$A$70-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",K27:BE$70,$A$70-$A27+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="10"/>
-      <c r="J27" s="1"/>
+      <c r="J27" s="10"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2776,8 +2882,9 @@
       <c r="BB27" s="1"/>
       <c r="BC27" s="1"/>
       <c r="BD27" s="1"/>
-    </row>
-    <row r="28" spans="1:56" s="14" customFormat="1">
+      <c r="BE27" s="1"/>
+    </row>
+    <row r="28" spans="1:57" s="14" customFormat="1">
       <c r="A28">
         <v>17</v>
       </c>
@@ -2838,8 +2945,9 @@
       <c r="BB28" s="13"/>
       <c r="BC28" s="13"/>
       <c r="BD28" s="13"/>
-    </row>
-    <row r="29" spans="1:56">
+      <c r="BE28" s="13"/>
+    </row>
+    <row r="29" spans="1:57">
       <c r="A29">
         <v>18</v>
       </c>
@@ -2854,28 +2962,30 @@
         <v>3</v>
       </c>
       <c r="F29" s="11">
-        <f>IFERROR( HLOOKUP("BE",J29:BD$71,$A$71-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",J29:BD$71,$A$71-$A29+1,FALSE),0)</f>
-        <v>40776</v>
+        <f>IFERROR( HLOOKUP("BE",K29:BE$70,$A$70-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",K29:BE$70,$A$70-$A29+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G29" s="11">
-        <f>IFERROR( HLOOKUP("BE",J29:BD$71,$A$71-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",J29:BD$71,$A$71-$A29+1,FALSE),0)</f>
-        <v>40777</v>
+        <f>IFERROR( HLOOKUP("BE",K29:BE$70,$A$70-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",K29:BE$70,$A$70-$A29+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="1"/>
+      <c r="J29" s="10" t="s">
+        <v>102</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="1" t="s">
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -2914,44 +3024,47 @@
       <c r="BB29" s="1"/>
       <c r="BC29" s="1"/>
       <c r="BD29" s="1"/>
-    </row>
-    <row r="30" spans="1:56">
+      <c r="BE29" s="1"/>
+    </row>
+    <row r="30" spans="1:57">
       <c r="A30">
         <v>19</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="10">
         <v>3</v>
       </c>
       <c r="F30" s="11">
-        <f>IFERROR( HLOOKUP("BE",J30:BD$71,$A$71-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",J30:BD$71,$A$71-$A30+1,FALSE),0)</f>
-        <v>40776</v>
+        <f>IFERROR( HLOOKUP("BE",K30:BE$70,$A$70-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",K30:BE$70,$A$70-$A30+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G30" s="11">
-        <f>IFERROR( HLOOKUP("BE",J30:BD$71,$A$71-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",J30:BD$71,$A$71-$A30+1,FALSE),0)</f>
-        <v>40777</v>
+        <f>IFERROR( HLOOKUP("BE",K30:BE$70,$A$70-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",K30:BE$70,$A$70-$A30+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="10"/>
-      <c r="J30" s="1"/>
+      <c r="J30" s="10" t="s">
+        <v>103</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="1" t="s">
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -2990,8 +3103,9 @@
       <c r="BB30" s="1"/>
       <c r="BC30" s="1"/>
       <c r="BD30" s="1"/>
-    </row>
-    <row r="31" spans="1:56">
+      <c r="BE30" s="1"/>
+    </row>
+    <row r="31" spans="1:57">
       <c r="A31">
         <v>20</v>
       </c>
@@ -3005,7 +3119,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="10"/>
-      <c r="J31" s="1"/>
+      <c r="J31" s="10"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -3052,8 +3166,9 @@
       <c r="BB31" s="1"/>
       <c r="BC31" s="1"/>
       <c r="BD31" s="1"/>
-    </row>
-    <row r="32" spans="1:56">
+      <c r="BE31" s="1"/>
+    </row>
+    <row r="32" spans="1:57">
       <c r="A32">
         <v>21</v>
       </c>
@@ -3062,34 +3177,36 @@
         <v>44</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E32" s="10">
         <v>3</v>
       </c>
       <c r="F32" s="11">
-        <f>IFERROR( HLOOKUP("BE",J32:BD$71,$A$71-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",J32:BD$71,$A$71-$A32+1,FALSE),0)</f>
-        <v>40776</v>
+        <f>IFERROR( HLOOKUP("BE",K32:BE$70,$A$70-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",K32:BE$70,$A$70-$A32+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G32" s="11">
-        <f>IFERROR( HLOOKUP("BE",J32:BD$71,$A$71-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",J32:BD$71,$A$71-$A32+1,FALSE),0)</f>
-        <v>40777</v>
+        <f>IFERROR( HLOOKUP("BE",K32:BE$70,$A$70-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",K32:BE$70,$A$70-$A32+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="10"/>
-      <c r="J32" s="1"/>
+      <c r="J32" s="10" t="s">
+        <v>104</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1" t="s">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -3128,8 +3245,9 @@
       <c r="BB32" s="1"/>
       <c r="BC32" s="1"/>
       <c r="BD32" s="1"/>
-    </row>
-    <row r="33" spans="1:56">
+      <c r="BE32" s="1"/>
+    </row>
+    <row r="33" spans="1:57">
       <c r="A33">
         <v>22</v>
       </c>
@@ -3138,34 +3256,36 @@
         <v>45</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="10">
         <v>3</v>
       </c>
       <c r="F33" s="11">
-        <f>IFERROR( HLOOKUP("BE",J33:BD$71,$A$71-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",J33:BD$71,$A$71-$A33+1,FALSE),0)</f>
-        <v>40776</v>
+        <f>IFERROR( HLOOKUP("BE",K33:BE$70,$A$70-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",K33:BE$70,$A$70-$A33+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G33" s="11">
-        <f>IFERROR( HLOOKUP("BE",J33:BD$71,$A$71-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",J33:BD$71,$A$71-$A33+1,FALSE),0)</f>
-        <v>40777</v>
+        <f>IFERROR( HLOOKUP("BE",K33:BE$70,$A$70-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",K33:BE$70,$A$70-$A33+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="10"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="1" t="s">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -3204,8 +3324,9 @@
       <c r="BB33" s="1"/>
       <c r="BC33" s="1"/>
       <c r="BD33" s="1"/>
-    </row>
-    <row r="34" spans="1:56">
+      <c r="BE33" s="1"/>
+    </row>
+    <row r="34" spans="1:57">
       <c r="A34">
         <v>23</v>
       </c>
@@ -3219,7 +3340,7 @@
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="10"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="10"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -3266,8 +3387,9 @@
       <c r="BB34" s="1"/>
       <c r="BC34" s="1"/>
       <c r="BD34" s="1"/>
-    </row>
-    <row r="35" spans="1:56">
+      <c r="BE34" s="1"/>
+    </row>
+    <row r="35" spans="1:57">
       <c r="A35">
         <v>24</v>
       </c>
@@ -3276,22 +3398,24 @@
         <v>46</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" s="10">
         <v>3</v>
       </c>
       <c r="F35" s="11">
-        <f>IFERROR( HLOOKUP("BE",J35:BD$71,$A$71-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",J35:BD$71,$A$71-$A35+1,FALSE),0)</f>
-        <v>40778</v>
+        <f>IFERROR( HLOOKUP("BE",K35:BE$70,$A$70-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",K35:BE$70,$A$70-$A35+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G35" s="11">
-        <f>IFERROR( HLOOKUP("BE",J35:BD$71,$A$71-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",J35:BD$71,$A$71-$A35+1,FALSE),0)</f>
-        <v>40779</v>
+        <f>IFERROR( HLOOKUP("BE",K35:BE$70,$A$70-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",K35:BE$70,$A$70-$A35+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="10"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3299,13 +3423,13 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1" t="s">
+      <c r="R35" s="1"/>
+      <c r="S35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
@@ -3342,8 +3466,9 @@
       <c r="BB35" s="1"/>
       <c r="BC35" s="1"/>
       <c r="BD35" s="1"/>
-    </row>
-    <row r="36" spans="1:56">
+      <c r="BE35" s="1"/>
+    </row>
+    <row r="36" spans="1:57">
       <c r="A36">
         <v>25</v>
       </c>
@@ -3352,22 +3477,24 @@
         <v>47</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E36" s="10">
         <v>3</v>
       </c>
       <c r="F36" s="11">
-        <f>IFERROR( HLOOKUP("BE",J36:BD$71,$A$71-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("B",J36:BD$71,$A$71-$A36+1,FALSE),0)</f>
-        <v>40778</v>
+        <f>IFERROR( HLOOKUP("BE",K36:BE$70,$A$70-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("B",K36:BE$70,$A$70-$A36+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G36" s="11">
-        <f>IFERROR( HLOOKUP("BE",J36:BD$71,$A$71-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("E",J36:BD$71,$A$71-$A36+1,FALSE),0)</f>
-        <v>40779</v>
+        <f>IFERROR( HLOOKUP("BE",K36:BE$70,$A$70-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("E",K36:BE$70,$A$70-$A36+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="10"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="10" t="s">
+        <v>107</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -3375,13 +3502,13 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="1" t="s">
+      <c r="R36" s="1"/>
+      <c r="S36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
@@ -3418,8 +3545,9 @@
       <c r="BB36" s="1"/>
       <c r="BC36" s="1"/>
       <c r="BD36" s="1"/>
-    </row>
-    <row r="37" spans="1:56">
+      <c r="BE36" s="1"/>
+    </row>
+    <row r="37" spans="1:57">
       <c r="A37">
         <v>26</v>
       </c>
@@ -3428,22 +3556,24 @@
         <v>48</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E37" s="10">
         <v>3</v>
       </c>
       <c r="F37" s="11">
-        <f>IFERROR( HLOOKUP("BE",J37:BD$71,$A$71-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("B",J37:BD$71,$A$71-$A37+1,FALSE),0)</f>
-        <v>40778</v>
+        <f>IFERROR( HLOOKUP("BE",K37:BE$70,$A$70-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("B",K37:BE$70,$A$70-$A37+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G37" s="11">
-        <f>IFERROR( HLOOKUP("BE",J37:BD$71,$A$71-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("E",J37:BD$71,$A$71-$A37+1,FALSE),0)</f>
-        <v>40779</v>
+        <f>IFERROR( HLOOKUP("BE",K37:BE$70,$A$70-$A37+1,FALSE),0)+ IFERROR( HLOOKUP("E",K37:BE$70,$A$70-$A37+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="1"/>
+      <c r="J37" s="10" t="s">
+        <v>108</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -3451,13 +3581,13 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="1" t="s">
+      <c r="R37" s="1"/>
+      <c r="S37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
@@ -3494,8 +3624,9 @@
       <c r="BB37" s="1"/>
       <c r="BC37" s="1"/>
       <c r="BD37" s="1"/>
-    </row>
-    <row r="38" spans="1:56">
+      <c r="BE37" s="1"/>
+    </row>
+    <row r="38" spans="1:57">
       <c r="A38">
         <v>27</v>
       </c>
@@ -3510,16 +3641,18 @@
         <v>3</v>
       </c>
       <c r="F38" s="11">
-        <f>IFERROR( HLOOKUP("BE",J38:BD$71,$A$71-$A38+1,FALSE),0)+ IFERROR( HLOOKUP("B",J38:BD$71,$A$71-$A38+1,FALSE),0)</f>
-        <v>40778</v>
+        <f>IFERROR( HLOOKUP("BE",K38:BE$70,$A$70-$A38+1,FALSE),0)+ IFERROR( HLOOKUP("B",K38:BE$70,$A$70-$A38+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G38" s="11">
-        <f>IFERROR( HLOOKUP("BE",J38:BD$71,$A$71-$A38+1,FALSE),0)+ IFERROR( HLOOKUP("E",J38:BD$71,$A$71-$A38+1,FALSE),0)</f>
-        <v>40779</v>
+        <f>IFERROR( HLOOKUP("BE",K38:BE$70,$A$70-$A38+1,FALSE),0)+ IFERROR( HLOOKUP("E",K38:BE$70,$A$70-$A38+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="10"/>
-      <c r="J38" s="1"/>
+      <c r="J38" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -3527,13 +3660,13 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1" t="s">
+      <c r="R38" s="1"/>
+      <c r="S38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
@@ -3570,8 +3703,9 @@
       <c r="BB38" s="1"/>
       <c r="BC38" s="1"/>
       <c r="BD38" s="1"/>
-    </row>
-    <row r="39" spans="1:56" s="14" customFormat="1">
+      <c r="BE38" s="1"/>
+    </row>
+    <row r="39" spans="1:57" s="14" customFormat="1">
       <c r="A39">
         <v>28</v>
       </c>
@@ -3632,8 +3766,9 @@
       <c r="BB39" s="13"/>
       <c r="BC39" s="13"/>
       <c r="BD39" s="13"/>
-    </row>
-    <row r="40" spans="1:56">
+      <c r="BE39" s="13"/>
+    </row>
+    <row r="40" spans="1:57">
       <c r="A40">
         <v>29</v>
       </c>
@@ -3648,16 +3783,18 @@
         <v>3</v>
       </c>
       <c r="F40" s="11">
-        <f>IFERROR( HLOOKUP("BE",J40:BD$71,$A$71-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("B",J40:BD$71,$A$71-$A40+1,FALSE),0)</f>
-        <v>40780</v>
+        <f>IFERROR( HLOOKUP("BE",K40:BE$70,$A$70-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("B",K40:BE$70,$A$70-$A40+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G40" s="11">
-        <f>IFERROR( HLOOKUP("BE",J40:BD$71,$A$71-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("E",J40:BD$71,$A$71-$A40+1,FALSE),0)</f>
-        <v>40781</v>
+        <f>IFERROR( HLOOKUP("BE",K40:BE$70,$A$70-$A40+1,FALSE),0)+ IFERROR( HLOOKUP("E",K40:BE$70,$A$70-$A40+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="10" t="s">
+        <v>110</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -3667,13 +3804,13 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
-      <c r="T40" s="1" t="s">
+      <c r="T40" s="1"/>
+      <c r="U40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="V40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
@@ -3708,8 +3845,9 @@
       <c r="BB40" s="1"/>
       <c r="BC40" s="1"/>
       <c r="BD40" s="1"/>
-    </row>
-    <row r="41" spans="1:56">
+      <c r="BE40" s="1"/>
+    </row>
+    <row r="41" spans="1:57">
       <c r="A41">
         <v>30</v>
       </c>
@@ -3723,7 +3861,7 @@
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
       <c r="I41" s="10"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="10"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -3770,8 +3908,9 @@
       <c r="BB41" s="1"/>
       <c r="BC41" s="1"/>
       <c r="BD41" s="1"/>
-    </row>
-    <row r="42" spans="1:56">
+      <c r="BE41" s="1"/>
+    </row>
+    <row r="42" spans="1:57">
       <c r="A42">
         <v>31</v>
       </c>
@@ -3780,22 +3919,24 @@
         <v>50</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E42" s="10">
         <v>3</v>
       </c>
       <c r="F42" s="11">
-        <f>IFERROR( HLOOKUP("BE",J42:BD$71,$A$71-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("B",J42:BD$71,$A$71-$A42+1,FALSE),0)</f>
-        <v>40780</v>
+        <f>IFERROR( HLOOKUP("BE",K42:BE$70,$A$70-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("B",K42:BE$70,$A$70-$A42+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G42" s="11">
-        <f>IFERROR( HLOOKUP("BE",J42:BD$71,$A$71-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("E",J42:BD$71,$A$71-$A42+1,FALSE),0)</f>
-        <v>40781</v>
+        <f>IFERROR( HLOOKUP("BE",K42:BE$70,$A$70-$A42+1,FALSE),0)+ IFERROR( HLOOKUP("E",K42:BE$70,$A$70-$A42+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="1"/>
+      <c r="J42" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -3805,13 +3946,13 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
-      <c r="T42" s="1" t="s">
+      <c r="T42" s="1"/>
+      <c r="U42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U42" s="1" t="s">
+      <c r="V42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
@@ -3846,8 +3987,9 @@
       <c r="BB42" s="1"/>
       <c r="BC42" s="1"/>
       <c r="BD42" s="1"/>
-    </row>
-    <row r="43" spans="1:56">
+      <c r="BE42" s="1"/>
+    </row>
+    <row r="43" spans="1:57">
       <c r="A43">
         <v>32</v>
       </c>
@@ -3856,22 +3998,24 @@
         <v>51</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="10">
         <v>3</v>
       </c>
       <c r="F43" s="11">
-        <f>IFERROR( HLOOKUP("BE",J43:BD$71,$A$71-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("B",J43:BD$71,$A$71-$A43+1,FALSE),0)</f>
-        <v>40780</v>
+        <f>IFERROR( HLOOKUP("BE",K43:BE$70,$A$70-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("B",K43:BE$70,$A$70-$A43+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G43" s="11">
-        <f>IFERROR( HLOOKUP("BE",J43:BD$71,$A$71-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("E",J43:BD$71,$A$71-$A43+1,FALSE),0)</f>
-        <v>40781</v>
+        <f>IFERROR( HLOOKUP("BE",K43:BE$70,$A$70-$A43+1,FALSE),0)+ IFERROR( HLOOKUP("E",K43:BE$70,$A$70-$A43+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="10"/>
-      <c r="J43" s="1"/>
+      <c r="J43" s="10" t="s">
+        <v>111</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -3881,13 +4025,13 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-      <c r="T43" s="1" t="s">
+      <c r="T43" s="1"/>
+      <c r="U43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U43" s="1" t="s">
+      <c r="V43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -3922,8 +4066,9 @@
       <c r="BB43" s="1"/>
       <c r="BC43" s="1"/>
       <c r="BD43" s="1"/>
-    </row>
-    <row r="44" spans="1:56">
+      <c r="BE43" s="1"/>
+    </row>
+    <row r="44" spans="1:57">
       <c r="A44">
         <v>33</v>
       </c>
@@ -3932,22 +4077,24 @@
         <v>52</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="10">
         <v>3</v>
       </c>
       <c r="F44" s="11">
-        <f>IFERROR( HLOOKUP("BE",J44:BD$71,$A$71-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("B",J44:BD$71,$A$71-$A44+1,FALSE),0)</f>
-        <v>40780</v>
+        <f>IFERROR( HLOOKUP("BE",K44:BE$70,$A$70-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("B",K44:BE$70,$A$70-$A44+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G44" s="11">
-        <f>IFERROR( HLOOKUP("BE",J44:BD$71,$A$71-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("E",J44:BD$71,$A$71-$A44+1,FALSE),0)</f>
-        <v>40781</v>
+        <f>IFERROR( HLOOKUP("BE",K44:BE$70,$A$70-$A44+1,FALSE),0)+ IFERROR( HLOOKUP("E",K44:BE$70,$A$70-$A44+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="10"/>
-      <c r="J44" s="1"/>
+      <c r="J44" s="10" t="s">
+        <v>112</v>
+      </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -3957,13 +4104,13 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="1" t="s">
+      <c r="T44" s="1"/>
+      <c r="U44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U44" s="1" t="s">
+      <c r="V44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -3998,8 +4145,9 @@
       <c r="BB44" s="1"/>
       <c r="BC44" s="1"/>
       <c r="BD44" s="1"/>
-    </row>
-    <row r="45" spans="1:56">
+      <c r="BE44" s="1"/>
+    </row>
+    <row r="45" spans="1:57">
       <c r="A45">
         <v>34</v>
       </c>
@@ -4013,7 +4161,7 @@
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="10"/>
-      <c r="J45" s="1"/>
+      <c r="J45" s="10"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -4060,32 +4208,35 @@
       <c r="BB45" s="1"/>
       <c r="BC45" s="1"/>
       <c r="BD45" s="1"/>
-    </row>
-    <row r="46" spans="1:56">
+      <c r="BE45" s="1"/>
+    </row>
+    <row r="46" spans="1:57">
       <c r="A46">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E46" s="10">
         <v>3</v>
       </c>
       <c r="F46" s="11">
-        <f>IFERROR( HLOOKUP("BE",J46:BD$71,$A$71-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("B",J46:BD$71,$A$71-$A46+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K46:BE$70,$A$70-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("B",K46:BE$70,$A$70-$A46+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G46" s="11">
-        <f>IFERROR( HLOOKUP("BE",J46:BD$71,$A$71-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("E",J46:BD$71,$A$71-$A46+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K46:BE$70,$A$70-$A46+1,FALSE),0)+ IFERROR( HLOOKUP("E",K46:BE$70,$A$70-$A46+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="10"/>
-      <c r="J46" s="1"/>
+      <c r="J46" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -4097,13 +4248,13 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
-      <c r="V46" s="1" t="s">
+      <c r="V46" s="1"/>
+      <c r="W46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W46" s="1" t="s">
+      <c r="X46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
@@ -4136,10 +4287,11 @@
       <c r="BB46" s="1"/>
       <c r="BC46" s="1"/>
       <c r="BD46" s="1"/>
-    </row>
-    <row r="47" spans="1:56">
+      <c r="BE46" s="1"/>
+    </row>
+    <row r="47" spans="1:57">
       <c r="A47">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="20" t="s">
@@ -4152,16 +4304,18 @@
         <v>3</v>
       </c>
       <c r="F47" s="11">
-        <f>IFERROR( HLOOKUP("BE",J47:BD$71,$A$71-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("B",J47:BD$71,$A$71-$A47+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K47:BE$70,$A$70-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("B",K47:BE$70,$A$70-$A47+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G47" s="11">
-        <f>IFERROR( HLOOKUP("BE",J47:BD$71,$A$71-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("E",J47:BD$71,$A$71-$A47+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K47:BE$70,$A$70-$A47+1,FALSE),0)+ IFERROR( HLOOKUP("E",K47:BE$70,$A$70-$A47+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="10"/>
-      <c r="J47" s="1"/>
+      <c r="J47" s="10" t="s">
+        <v>115</v>
+      </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -4173,13 +4327,13 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
-      <c r="V47" s="1" t="s">
+      <c r="V47" s="1"/>
+      <c r="W47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W47" s="1" t="s">
+      <c r="X47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
@@ -4212,32 +4366,35 @@
       <c r="BB47" s="1"/>
       <c r="BC47" s="1"/>
       <c r="BD47" s="1"/>
-    </row>
-    <row r="48" spans="1:56">
+      <c r="BE47" s="1"/>
+    </row>
+    <row r="48" spans="1:57">
       <c r="A48">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E48" s="10">
         <v>3</v>
       </c>
       <c r="F48" s="11">
-        <f>IFERROR( HLOOKUP("BE",J48:BD$71,$A$71-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("B",J48:BD$71,$A$71-$A48+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K48:BE$70,$A$70-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("B",K48:BE$70,$A$70-$A48+1,FALSE),0)</f>
         <v>40782</v>
       </c>
       <c r="G48" s="11">
-        <f>IFERROR( HLOOKUP("BE",J48:BD$71,$A$71-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("E",J48:BD$71,$A$71-$A48+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K48:BE$70,$A$70-$A48+1,FALSE),0)+ IFERROR( HLOOKUP("E",K48:BE$70,$A$70-$A48+1,FALSE),0)</f>
         <v>40783</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="10"/>
-      <c r="J48" s="1"/>
+      <c r="J48" s="10" t="s">
+        <v>116</v>
+      </c>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -4249,13 +4406,13 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
-      <c r="V48" s="1" t="s">
+      <c r="V48" s="1"/>
+      <c r="W48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W48" s="1" t="s">
+      <c r="X48" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
@@ -4288,180 +4445,193 @@
       <c r="BB48" s="1"/>
       <c r="BC48" s="1"/>
       <c r="BD48" s="1"/>
-    </row>
-    <row r="49" spans="1:56">
+      <c r="BE48" s="1"/>
+    </row>
+    <row r="49" spans="1:57" s="14" customFormat="1">
       <c r="A49">
-        <v>38</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="10">
-        <v>3</v>
-      </c>
-      <c r="F49" s="11">
-        <f>IFERROR( HLOOKUP("BE",J49:BD$71,$A$71-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("B",J49:BD$71,$A$71-$A49+1,FALSE),0)</f>
-        <v>40782</v>
-      </c>
-      <c r="G49" s="11">
-        <f>IFERROR( HLOOKUP("BE",J49:BD$71,$A$71-$A49+1,FALSE),0)+ IFERROR( HLOOKUP("E",J49:BD$71,$A$71-$A49+1,FALSE),0)</f>
-        <v>40783</v>
-      </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="13"/>
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="13"/>
+      <c r="AF49" s="13"/>
+      <c r="AG49" s="13"/>
+      <c r="AH49" s="13"/>
+      <c r="AI49" s="13"/>
+      <c r="AJ49" s="13"/>
+      <c r="AK49" s="13"/>
+      <c r="AL49" s="13"/>
+      <c r="AM49" s="13"/>
+      <c r="AN49" s="13"/>
+      <c r="AO49" s="13"/>
+      <c r="AP49" s="13"/>
+      <c r="AQ49" s="13"/>
+      <c r="AR49" s="13"/>
+      <c r="AS49" s="13"/>
+      <c r="AT49" s="13"/>
+      <c r="AU49" s="13"/>
+      <c r="AV49" s="13"/>
+      <c r="AW49" s="13"/>
+      <c r="AX49" s="13"/>
+      <c r="AY49" s="13"/>
+      <c r="AZ49" s="13"/>
+      <c r="BA49" s="13"/>
+      <c r="BB49" s="13"/>
+      <c r="BC49" s="13"/>
+      <c r="BD49" s="13"/>
+      <c r="BE49" s="13"/>
+    </row>
+    <row r="50" spans="1:57">
+      <c r="A50">
+        <v>40</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="10">
+        <v>2</v>
+      </c>
+      <c r="F50" s="11">
+        <f>IFERROR( HLOOKUP("BE",K50:BE$70,$A$70-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("B",K50:BE$70,$A$70-$A50+1,FALSE),0)</f>
+        <v>40771</v>
+      </c>
+      <c r="G50" s="11">
+        <f>IFERROR( HLOOKUP("BE",K50:BE$70,$A$70-$A50+1,FALSE),0)+ IFERROR( HLOOKUP("E",K50:BE$70,$A$70-$A50+1,FALSE),0)</f>
+        <v>40771</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="1"/>
+      <c r="AH50" s="1"/>
+      <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
+      <c r="AK50" s="1"/>
+      <c r="AL50" s="1"/>
+      <c r="AM50" s="1"/>
+      <c r="AN50" s="1"/>
+      <c r="AO50" s="1"/>
+      <c r="AP50" s="1"/>
+      <c r="AQ50" s="1"/>
+      <c r="AR50" s="1"/>
+      <c r="AS50" s="1"/>
+      <c r="AT50" s="1"/>
+      <c r="AU50" s="1"/>
+      <c r="AV50" s="1"/>
+      <c r="AW50" s="1"/>
+      <c r="AX50" s="1"/>
+      <c r="AY50" s="1"/>
+      <c r="AZ50" s="1"/>
+      <c r="BA50" s="1"/>
+      <c r="BB50" s="1"/>
+      <c r="BC50" s="1"/>
+      <c r="BD50" s="1"/>
+      <c r="BE50" s="1"/>
+    </row>
+    <row r="51" spans="1:57">
+      <c r="A51">
         <v>41</v>
-      </c>
-      <c r="W49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-      <c r="AF49" s="1"/>
-      <c r="AG49" s="1"/>
-      <c r="AH49" s="1"/>
-      <c r="AI49" s="1"/>
-      <c r="AJ49" s="1"/>
-      <c r="AK49" s="1"/>
-      <c r="AL49" s="1"/>
-      <c r="AM49" s="1"/>
-      <c r="AN49" s="1"/>
-      <c r="AO49" s="1"/>
-      <c r="AP49" s="1"/>
-      <c r="AQ49" s="1"/>
-      <c r="AR49" s="1"/>
-      <c r="AS49" s="1"/>
-      <c r="AT49" s="1"/>
-      <c r="AU49" s="1"/>
-      <c r="AV49" s="1"/>
-      <c r="AW49" s="1"/>
-      <c r="AX49" s="1"/>
-      <c r="AY49" s="1"/>
-      <c r="AZ49" s="1"/>
-      <c r="BA49" s="1"/>
-      <c r="BB49" s="1"/>
-      <c r="BC49" s="1"/>
-      <c r="BD49" s="1"/>
-    </row>
-    <row r="50" spans="1:56" s="14" customFormat="1">
-      <c r="A50">
-        <v>39</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="13"/>
-      <c r="S50" s="13"/>
-      <c r="T50" s="13"/>
-      <c r="U50" s="13"/>
-      <c r="V50" s="13"/>
-      <c r="W50" s="13"/>
-      <c r="X50" s="13"/>
-      <c r="Y50" s="13"/>
-      <c r="Z50" s="13"/>
-      <c r="AA50" s="13"/>
-      <c r="AB50" s="13"/>
-      <c r="AC50" s="13"/>
-      <c r="AD50" s="13"/>
-      <c r="AE50" s="13"/>
-      <c r="AF50" s="13"/>
-      <c r="AG50" s="13"/>
-      <c r="AH50" s="13"/>
-      <c r="AI50" s="13"/>
-      <c r="AJ50" s="13"/>
-      <c r="AK50" s="13"/>
-      <c r="AL50" s="13"/>
-      <c r="AM50" s="13"/>
-      <c r="AN50" s="13"/>
-      <c r="AO50" s="13"/>
-      <c r="AP50" s="13"/>
-      <c r="AQ50" s="13"/>
-      <c r="AR50" s="13"/>
-      <c r="AS50" s="13"/>
-      <c r="AT50" s="13"/>
-      <c r="AU50" s="13"/>
-      <c r="AV50" s="13"/>
-      <c r="AW50" s="13"/>
-      <c r="AX50" s="13"/>
-      <c r="AY50" s="13"/>
-      <c r="AZ50" s="13"/>
-      <c r="BA50" s="13"/>
-      <c r="BB50" s="13"/>
-      <c r="BC50" s="13"/>
-      <c r="BD50" s="13"/>
-    </row>
-    <row r="51" spans="1:56">
-      <c r="A51">
-        <v>40</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="E51" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" s="11">
-        <f>IFERROR( HLOOKUP("BE",J51:BD$71,$A$71-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("B",J51:BD$71,$A$71-$A51+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K51:BE$70,$A$70-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("B",K51:BE$70,$A$70-$A51+1,FALSE),0)</f>
         <v>40771</v>
       </c>
       <c r="G51" s="11">
-        <f>IFERROR( HLOOKUP("BE",J51:BD$71,$A$71-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("E",J51:BD$71,$A$71-$A51+1,FALSE),0)</f>
-        <v>40771</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>87</v>
-      </c>
+        <f>IFERROR( HLOOKUP("BE",K51:BE$70,$A$70-$A51+1,FALSE),0)+ IFERROR( HLOOKUP("E",K51:BE$70,$A$70-$A51+1,FALSE),0)</f>
+        <v>40775</v>
+      </c>
+      <c r="H51" s="11"/>
       <c r="I51" s="10"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="J51" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -4502,47 +4672,32 @@
       <c r="BB51" s="1"/>
       <c r="BC51" s="1"/>
       <c r="BD51" s="1"/>
-    </row>
-    <row r="52" spans="1:56">
+      <c r="BE51" s="1"/>
+    </row>
+    <row r="52" spans="1:57">
       <c r="A52">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" s="10">
-        <v>1</v>
-      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
       <c r="F52" s="11">
-        <f>IFERROR( HLOOKUP("BE",J52:BD$71,$A$71-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("B",J52:BD$71,$A$71-$A52+1,FALSE),0)</f>
-        <v>40771</v>
+        <f>IFERROR( HLOOKUP("BE",K52:BE$70,$A$70-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("B",K52:BE$70,$A$70-$A52+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="G52" s="11">
-        <f>IFERROR( HLOOKUP("BE",J52:BD$71,$A$71-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("E",J52:BD$71,$A$71-$A52+1,FALSE),0)</f>
-        <v>40775</v>
+        <f>IFERROR( HLOOKUP("BE",K52:BE$70,$A$70-$A52+1,FALSE),0)+ IFERROR( HLOOKUP("E",K52:BE$70,$A$70-$A52+1,FALSE),0)</f>
+        <v>0</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="10"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="J52" s="10"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
@@ -4584,26 +4739,27 @@
       <c r="BB52" s="1"/>
       <c r="BC52" s="1"/>
       <c r="BD52" s="1"/>
-    </row>
-    <row r="53" spans="1:56">
+      <c r="BE52" s="1"/>
+    </row>
+    <row r="53" spans="1:57">
       <c r="A53">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="11">
-        <f>IFERROR( HLOOKUP("BE",J53:BD$71,$A$71-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("B",J53:BD$71,$A$71-$A53+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K53:BE$70,$A$70-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("B",K53:BE$70,$A$70-$A53+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G53" s="11">
-        <f>IFERROR( HLOOKUP("BE",J53:BD$71,$A$71-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("E",J53:BD$71,$A$71-$A53+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K53:BE$70,$A$70-$A53+1,FALSE),0)+ IFERROR( HLOOKUP("E",K53:BE$70,$A$70-$A53+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="10"/>
-      <c r="J53" s="1"/>
+      <c r="J53" s="10"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -4650,26 +4806,27 @@
       <c r="BB53" s="1"/>
       <c r="BC53" s="1"/>
       <c r="BD53" s="1"/>
-    </row>
-    <row r="54" spans="1:56">
+      <c r="BE53" s="1"/>
+    </row>
+    <row r="54" spans="1:57">
       <c r="A54">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="11">
-        <f>IFERROR( HLOOKUP("BE",J54:BD$71,$A$71-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("B",J54:BD$71,$A$71-$A54+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K54:BE$70,$A$70-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("B",K54:BE$70,$A$70-$A54+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G54" s="11">
-        <f>IFERROR( HLOOKUP("BE",J54:BD$71,$A$71-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("E",J54:BD$71,$A$71-$A54+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K54:BE$70,$A$70-$A54+1,FALSE),0)+ IFERROR( HLOOKUP("E",K54:BE$70,$A$70-$A54+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H54" s="11"/>
       <c r="I54" s="10"/>
-      <c r="J54" s="1"/>
+      <c r="J54" s="10"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -4716,138 +4873,143 @@
       <c r="BB54" s="1"/>
       <c r="BC54" s="1"/>
       <c r="BD54" s="1"/>
-    </row>
-    <row r="55" spans="1:56">
+      <c r="BE54" s="1"/>
+    </row>
+    <row r="55" spans="1:57" s="14" customFormat="1">
       <c r="A55">
-        <v>44</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="11">
-        <f>IFERROR( HLOOKUP("BE",J55:BD$71,$A$71-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("B",J55:BD$71,$A$71-$A55+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="11">
-        <f>IFERROR( HLOOKUP("BE",J55:BD$71,$A$71-$A55+1,FALSE),0)+ IFERROR( HLOOKUP("E",J55:BD$71,$A$71-$A55+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="W55" s="1"/>
-      <c r="X55" s="1"/>
-      <c r="Y55" s="1"/>
-      <c r="Z55" s="1"/>
-      <c r="AA55" s="1"/>
-      <c r="AB55" s="1"/>
-      <c r="AC55" s="1"/>
-      <c r="AD55" s="1"/>
-      <c r="AE55" s="1"/>
-      <c r="AF55" s="1"/>
-      <c r="AG55" s="1"/>
-      <c r="AH55" s="1"/>
-      <c r="AI55" s="1"/>
-      <c r="AJ55" s="1"/>
-      <c r="AK55" s="1"/>
-      <c r="AL55" s="1"/>
-      <c r="AM55" s="1"/>
-      <c r="AN55" s="1"/>
-      <c r="AO55" s="1"/>
-      <c r="AP55" s="1"/>
-      <c r="AQ55" s="1"/>
-      <c r="AR55" s="1"/>
-      <c r="AS55" s="1"/>
-      <c r="AT55" s="1"/>
-      <c r="AU55" s="1"/>
-      <c r="AV55" s="1"/>
-      <c r="AW55" s="1"/>
-      <c r="AX55" s="1"/>
-      <c r="AY55" s="1"/>
-      <c r="AZ55" s="1"/>
-      <c r="BA55" s="1"/>
-      <c r="BB55" s="1"/>
-      <c r="BC55" s="1"/>
-      <c r="BD55" s="1"/>
-    </row>
-    <row r="56" spans="1:56" s="14" customFormat="1">
+        <v>39</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="13"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="13"/>
+      <c r="W55" s="13"/>
+      <c r="X55" s="13"/>
+      <c r="Y55" s="13"/>
+      <c r="Z55" s="13"/>
+      <c r="AA55" s="13"/>
+      <c r="AB55" s="13"/>
+      <c r="AC55" s="13"/>
+      <c r="AD55" s="13"/>
+      <c r="AE55" s="13"/>
+      <c r="AF55" s="13"/>
+      <c r="AG55" s="13"/>
+      <c r="AH55" s="13"/>
+      <c r="AI55" s="13"/>
+      <c r="AJ55" s="13"/>
+      <c r="AK55" s="13"/>
+      <c r="AL55" s="13"/>
+      <c r="AM55" s="13"/>
+      <c r="AN55" s="13"/>
+      <c r="AO55" s="13"/>
+      <c r="AP55" s="13"/>
+      <c r="AQ55" s="13"/>
+      <c r="AR55" s="13"/>
+      <c r="AS55" s="13"/>
+      <c r="AT55" s="13"/>
+      <c r="AU55" s="13"/>
+      <c r="AV55" s="13"/>
+      <c r="AW55" s="13"/>
+      <c r="AX55" s="13"/>
+      <c r="AY55" s="13"/>
+      <c r="AZ55" s="13"/>
+      <c r="BA55" s="13"/>
+      <c r="BB55" s="13"/>
+      <c r="BC55" s="13"/>
+      <c r="BD55" s="13"/>
+      <c r="BE55" s="13"/>
+    </row>
+    <row r="56" spans="1:57">
       <c r="A56">
-        <v>39</v>
-      </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="13"/>
-      <c r="S56" s="13"/>
-      <c r="T56" s="13"/>
-      <c r="U56" s="13"/>
-      <c r="V56" s="13"/>
-      <c r="W56" s="13"/>
-      <c r="X56" s="13"/>
-      <c r="Y56" s="13"/>
-      <c r="Z56" s="13"/>
-      <c r="AA56" s="13"/>
-      <c r="AB56" s="13"/>
-      <c r="AC56" s="13"/>
-      <c r="AD56" s="13"/>
-      <c r="AE56" s="13"/>
-      <c r="AF56" s="13"/>
-      <c r="AG56" s="13"/>
-      <c r="AH56" s="13"/>
-      <c r="AI56" s="13"/>
-      <c r="AJ56" s="13"/>
-      <c r="AK56" s="13"/>
-      <c r="AL56" s="13"/>
-      <c r="AM56" s="13"/>
-      <c r="AN56" s="13"/>
-      <c r="AO56" s="13"/>
-      <c r="AP56" s="13"/>
-      <c r="AQ56" s="13"/>
-      <c r="AR56" s="13"/>
-      <c r="AS56" s="13"/>
-      <c r="AT56" s="13"/>
-      <c r="AU56" s="13"/>
-      <c r="AV56" s="13"/>
-      <c r="AW56" s="13"/>
-      <c r="AX56" s="13"/>
-      <c r="AY56" s="13"/>
-      <c r="AZ56" s="13"/>
-      <c r="BA56" s="13"/>
-      <c r="BB56" s="13"/>
-      <c r="BC56" s="13"/>
-      <c r="BD56" s="13"/>
-    </row>
-    <row r="57" spans="1:56">
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="11">
+        <f>IFERROR( HLOOKUP("BE",K56:BE$70,$A$70-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("B",K56:BE$70,$A$70-$A56+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="11">
+        <f>IFERROR( HLOOKUP("BE",K56:BE$70,$A$70-$A56+1,FALSE),0)+ IFERROR( HLOOKUP("E",K56:BE$70,$A$70-$A56+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="11"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="1"/>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+      <c r="AL56" s="1"/>
+      <c r="AM56" s="1"/>
+      <c r="AN56" s="1"/>
+      <c r="AO56" s="1"/>
+      <c r="AP56" s="1"/>
+      <c r="AQ56" s="1"/>
+      <c r="AR56" s="1"/>
+      <c r="AS56" s="1"/>
+      <c r="AT56" s="1"/>
+      <c r="AU56" s="1"/>
+      <c r="AV56" s="1"/>
+      <c r="AW56" s="1"/>
+      <c r="AX56" s="1"/>
+      <c r="AY56" s="1"/>
+      <c r="AZ56" s="1"/>
+      <c r="BA56" s="1"/>
+      <c r="BB56" s="1"/>
+      <c r="BC56" s="1"/>
+      <c r="BD56" s="1"/>
+      <c r="BE56" s="1"/>
+    </row>
+    <row r="57" spans="1:57">
       <c r="A57">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
@@ -4856,16 +5018,16 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="11">
-        <f>IFERROR( HLOOKUP("BE",J57:BD$71,$A$71-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("B",J57:BD$71,$A$71-$A57+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K57:BE$70,$A$70-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("B",K57:BE$70,$A$70-$A57+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G57" s="11">
-        <f>IFERROR( HLOOKUP("BE",J57:BD$71,$A$71-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("E",J57:BD$71,$A$71-$A57+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K57:BE$70,$A$70-$A57+1,FALSE),0)+ IFERROR( HLOOKUP("E",K57:BE$70,$A$70-$A57+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H57" s="11"/>
       <c r="I57" s="10"/>
-      <c r="J57" s="1"/>
+      <c r="J57" s="10"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -4912,10 +5074,11 @@
       <c r="BB57" s="1"/>
       <c r="BC57" s="1"/>
       <c r="BD57" s="1"/>
-    </row>
-    <row r="58" spans="1:56">
+      <c r="BE57" s="1"/>
+    </row>
+    <row r="58" spans="1:57">
       <c r="A58">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
@@ -4924,16 +5087,16 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="11">
-        <f>IFERROR( HLOOKUP("BE",J58:BD$71,$A$71-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("B",J58:BD$71,$A$71-$A58+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K58:BE$70,$A$70-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("B",K58:BE$70,$A$70-$A58+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G58" s="11">
-        <f>IFERROR( HLOOKUP("BE",J58:BD$71,$A$71-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("E",J58:BD$71,$A$71-$A58+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K58:BE$70,$A$70-$A58+1,FALSE),0)+ IFERROR( HLOOKUP("E",K58:BE$70,$A$70-$A58+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H58" s="11"/>
       <c r="I58" s="10"/>
-      <c r="J58" s="1"/>
+      <c r="J58" s="10"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -4980,28 +5143,27 @@
       <c r="BB58" s="1"/>
       <c r="BC58" s="1"/>
       <c r="BD58" s="1"/>
-    </row>
-    <row r="59" spans="1:56">
+      <c r="BE58" s="1"/>
+    </row>
+    <row r="59" spans="1:57">
       <c r="A59">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B59" s="10"/>
-      <c r="C59" s="10" t="s">
-        <v>93</v>
-      </c>
+      <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="11">
-        <f>IFERROR( HLOOKUP("BE",J59:BD$71,$A$71-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",J59:BD$71,$A$71-$A59+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K59:BE$70,$A$70-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",K59:BE$70,$A$70-$A59+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G59" s="11">
-        <f>IFERROR( HLOOKUP("BE",J59:BD$71,$A$71-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",J59:BD$71,$A$71-$A59+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K59:BE$70,$A$70-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",K59:BE$70,$A$70-$A59+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H59" s="11"/>
       <c r="I59" s="10"/>
-      <c r="J59" s="1"/>
+      <c r="J59" s="10"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -5048,26 +5210,27 @@
       <c r="BB59" s="1"/>
       <c r="BC59" s="1"/>
       <c r="BD59" s="1"/>
-    </row>
-    <row r="60" spans="1:56">
+      <c r="BE59" s="1"/>
+    </row>
+    <row r="60" spans="1:57">
       <c r="A60">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="11">
-        <f>IFERROR( HLOOKUP("BE",J60:BD$71,$A$71-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("B",J60:BD$71,$A$71-$A60+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K60:BE$70,$A$70-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("B",K60:BE$70,$A$70-$A60+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G60" s="11">
-        <f>IFERROR( HLOOKUP("BE",J60:BD$71,$A$71-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("E",J60:BD$71,$A$71-$A60+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K60:BE$70,$A$70-$A60+1,FALSE),0)+ IFERROR( HLOOKUP("E",K60:BE$70,$A$70-$A60+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H60" s="11"/>
       <c r="I60" s="10"/>
-      <c r="J60" s="1"/>
+      <c r="J60" s="10"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -5114,26 +5277,27 @@
       <c r="BB60" s="1"/>
       <c r="BC60" s="1"/>
       <c r="BD60" s="1"/>
-    </row>
-    <row r="61" spans="1:56">
+      <c r="BE60" s="1"/>
+    </row>
+    <row r="61" spans="1:57">
       <c r="A61">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
       <c r="F61" s="11">
-        <f>IFERROR( HLOOKUP("BE",J61:BD$71,$A$71-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("B",J61:BD$71,$A$71-$A61+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K61:BE$70,$A$70-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("B",K61:BE$70,$A$70-$A61+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G61" s="11">
-        <f>IFERROR( HLOOKUP("BE",J61:BD$71,$A$71-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("E",J61:BD$71,$A$71-$A61+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K61:BE$70,$A$70-$A61+1,FALSE),0)+ IFERROR( HLOOKUP("E",K61:BE$70,$A$70-$A61+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H61" s="11"/>
       <c r="I61" s="10"/>
-      <c r="J61" s="1"/>
+      <c r="J61" s="10"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -5180,26 +5344,27 @@
       <c r="BB61" s="1"/>
       <c r="BC61" s="1"/>
       <c r="BD61" s="1"/>
-    </row>
-    <row r="62" spans="1:56">
+      <c r="BE61" s="1"/>
+    </row>
+    <row r="62" spans="1:57">
       <c r="A62">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
       <c r="F62" s="11">
-        <f>IFERROR( HLOOKUP("BE",J62:BD$71,$A$71-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",J62:BD$71,$A$71-$A62+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K62:BE$70,$A$70-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",K62:BE$70,$A$70-$A62+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G62" s="11">
-        <f>IFERROR( HLOOKUP("BE",J62:BD$71,$A$71-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",J62:BD$71,$A$71-$A62+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K62:BE$70,$A$70-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",K62:BE$70,$A$70-$A62+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H62" s="11"/>
       <c r="I62" s="10"/>
-      <c r="J62" s="1"/>
+      <c r="J62" s="10"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -5246,26 +5411,27 @@
       <c r="BB62" s="1"/>
       <c r="BC62" s="1"/>
       <c r="BD62" s="1"/>
-    </row>
-    <row r="63" spans="1:56">
+      <c r="BE62" s="1"/>
+    </row>
+    <row r="63" spans="1:57">
       <c r="A63">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="11">
-        <f>IFERROR( HLOOKUP("BE",J63:BD$71,$A$71-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",J63:BD$71,$A$71-$A63+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K63:BE$70,$A$70-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",K63:BE$70,$A$70-$A63+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G63" s="11">
-        <f>IFERROR( HLOOKUP("BE",J63:BD$71,$A$71-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",J63:BD$71,$A$71-$A63+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K63:BE$70,$A$70-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",K63:BE$70,$A$70-$A63+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H63" s="11"/>
       <c r="I63" s="10"/>
-      <c r="J63" s="1"/>
+      <c r="J63" s="10"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -5312,26 +5478,27 @@
       <c r="BB63" s="1"/>
       <c r="BC63" s="1"/>
       <c r="BD63" s="1"/>
-    </row>
-    <row r="64" spans="1:56">
+      <c r="BE63" s="1"/>
+    </row>
+    <row r="64" spans="1:57">
       <c r="A64">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="11">
-        <f>IFERROR( HLOOKUP("BE",J64:BD$71,$A$71-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("B",J64:BD$71,$A$71-$A64+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K64:BE$70,$A$70-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("B",K64:BE$70,$A$70-$A64+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G64" s="11">
-        <f>IFERROR( HLOOKUP("BE",J64:BD$71,$A$71-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("E",J64:BD$71,$A$71-$A64+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K64:BE$70,$A$70-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("E",K64:BE$70,$A$70-$A64+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H64" s="11"/>
       <c r="I64" s="10"/>
-      <c r="J64" s="1"/>
+      <c r="J64" s="10"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -5378,26 +5545,27 @@
       <c r="BB64" s="1"/>
       <c r="BC64" s="1"/>
       <c r="BD64" s="1"/>
-    </row>
-    <row r="65" spans="1:56">
+      <c r="BE64" s="1"/>
+    </row>
+    <row r="65" spans="1:57">
       <c r="A65">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="11">
-        <f>IFERROR( HLOOKUP("BE",J65:BD$71,$A$71-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("B",J65:BD$71,$A$71-$A65+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K65:BE$70,$A$70-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("B",K65:BE$70,$A$70-$A65+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G65" s="11">
-        <f>IFERROR( HLOOKUP("BE",J65:BD$71,$A$71-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("E",J65:BD$71,$A$71-$A65+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K65:BE$70,$A$70-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("E",K65:BE$70,$A$70-$A65+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H65" s="11"/>
       <c r="I65" s="10"/>
-      <c r="J65" s="1"/>
+      <c r="J65" s="10"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -5444,26 +5612,27 @@
       <c r="BB65" s="1"/>
       <c r="BC65" s="1"/>
       <c r="BD65" s="1"/>
-    </row>
-    <row r="66" spans="1:56">
+      <c r="BE65" s="1"/>
+    </row>
+    <row r="66" spans="1:57">
       <c r="A66">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
       <c r="E66" s="10"/>
       <c r="F66" s="11">
-        <f>IFERROR( HLOOKUP("BE",J66:BD$71,$A$71-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("B",J66:BD$71,$A$71-$A66+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K66:BE$70,$A$70-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("B",K66:BE$70,$A$70-$A66+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G66" s="11">
-        <f>IFERROR( HLOOKUP("BE",J66:BD$71,$A$71-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("E",J66:BD$71,$A$71-$A66+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",K66:BE$70,$A$70-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("E",K66:BE$70,$A$70-$A66+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H66" s="11"/>
       <c r="I66" s="10"/>
-      <c r="J66" s="1"/>
+      <c r="J66" s="10"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -5510,293 +5679,230 @@
       <c r="BB66" s="1"/>
       <c r="BC66" s="1"/>
       <c r="BD66" s="1"/>
-    </row>
-    <row r="67" spans="1:56">
+      <c r="BE66" s="1"/>
+    </row>
+    <row r="67" spans="1:57">
       <c r="A67">
-        <v>56</v>
-      </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="11">
-        <f>IFERROR( HLOOKUP("BE",J67:BD$71,$A$71-$A67+1,FALSE),0)+ IFERROR( HLOOKUP("B",J67:BD$71,$A$71-$A67+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G67" s="11">
-        <f>IFERROR( HLOOKUP("BE",J67:BD$71,$A$71-$A67+1,FALSE),0)+ IFERROR( HLOOKUP("E",J67:BD$71,$A$71-$A67+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="11"/>
-      <c r="I67" s="10"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-      <c r="AF67" s="1"/>
-      <c r="AG67" s="1"/>
-      <c r="AH67" s="1"/>
-      <c r="AI67" s="1"/>
-      <c r="AJ67" s="1"/>
-      <c r="AK67" s="1"/>
-      <c r="AL67" s="1"/>
-      <c r="AM67" s="1"/>
-      <c r="AN67" s="1"/>
-      <c r="AO67" s="1"/>
-      <c r="AP67" s="1"/>
-      <c r="AQ67" s="1"/>
-      <c r="AR67" s="1"/>
-      <c r="AS67" s="1"/>
-      <c r="AT67" s="1"/>
-      <c r="AU67" s="1"/>
-      <c r="AV67" s="1"/>
-      <c r="AW67" s="1"/>
-      <c r="AX67" s="1"/>
-      <c r="AY67" s="1"/>
-      <c r="AZ67" s="1"/>
-      <c r="BA67" s="1"/>
-      <c r="BB67" s="1"/>
-      <c r="BC67" s="1"/>
-      <c r="BD67" s="1"/>
-    </row>
-    <row r="68" spans="1:56">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:57">
       <c r="A68">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="1:56">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:57">
       <c r="A69">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:56">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:57" s="17" customFormat="1">
       <c r="A70">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="71" spans="1:56" s="17" customFormat="1">
-      <c r="A71">
         <v>60</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="C70" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="J71" s="12">
-        <f>J9</f>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="K70" s="12">
+        <f>K9</f>
         <v>40770</v>
       </c>
-      <c r="K71" s="12">
-        <f t="shared" ref="K71:BD71" si="1">K9</f>
+      <c r="L70" s="12">
+        <f t="shared" ref="L70:BE70" si="1">L9</f>
         <v>40771</v>
       </c>
-      <c r="L71" s="12">
+      <c r="M70" s="12">
         <f t="shared" si="1"/>
         <v>40772</v>
       </c>
-      <c r="M71" s="12">
+      <c r="N70" s="12">
         <f t="shared" si="1"/>
         <v>40773</v>
       </c>
-      <c r="N71" s="12">
+      <c r="O70" s="12">
         <f t="shared" si="1"/>
         <v>40774</v>
       </c>
-      <c r="O71" s="12">
+      <c r="P70" s="12">
         <f t="shared" si="1"/>
         <v>40775</v>
       </c>
-      <c r="P71" s="12">
+      <c r="Q70" s="12">
         <f t="shared" si="1"/>
         <v>40776</v>
       </c>
-      <c r="Q71" s="12">
+      <c r="R70" s="12">
         <f t="shared" si="1"/>
         <v>40777</v>
       </c>
-      <c r="R71" s="12">
+      <c r="S70" s="12">
         <f t="shared" si="1"/>
         <v>40778</v>
       </c>
-      <c r="S71" s="12">
+      <c r="T70" s="12">
         <f t="shared" si="1"/>
         <v>40779</v>
       </c>
-      <c r="T71" s="12">
+      <c r="U70" s="12">
         <f t="shared" si="1"/>
         <v>40780</v>
       </c>
-      <c r="U71" s="12">
+      <c r="V70" s="12">
         <f t="shared" si="1"/>
         <v>40781</v>
       </c>
-      <c r="V71" s="12">
+      <c r="W70" s="12">
         <f t="shared" si="1"/>
         <v>40782</v>
       </c>
-      <c r="W71" s="12">
+      <c r="X70" s="12">
         <f t="shared" si="1"/>
         <v>40783</v>
       </c>
-      <c r="X71" s="12">
+      <c r="Y70" s="12">
         <f t="shared" si="1"/>
         <v>40784</v>
       </c>
-      <c r="Y71" s="12">
+      <c r="Z70" s="12">
         <f t="shared" si="1"/>
         <v>40785</v>
       </c>
-      <c r="Z71" s="12">
+      <c r="AA70" s="12">
         <f t="shared" si="1"/>
         <v>40786</v>
       </c>
-      <c r="AA71" s="12">
+      <c r="AB70" s="12">
         <f t="shared" si="1"/>
         <v>40787</v>
       </c>
-      <c r="AB71" s="12">
+      <c r="AC70" s="12">
         <f t="shared" si="1"/>
         <v>40788</v>
       </c>
-      <c r="AC71" s="12">
+      <c r="AD70" s="12">
         <f t="shared" si="1"/>
         <v>40789</v>
       </c>
-      <c r="AD71" s="12">
+      <c r="AE70" s="12">
         <f t="shared" si="1"/>
         <v>40790</v>
       </c>
-      <c r="AE71" s="12">
+      <c r="AF70" s="12">
         <f t="shared" si="1"/>
         <v>40791</v>
       </c>
-      <c r="AF71" s="12">
+      <c r="AG70" s="12">
         <f t="shared" si="1"/>
         <v>40792</v>
       </c>
-      <c r="AG71" s="12">
+      <c r="AH70" s="12">
         <f t="shared" si="1"/>
         <v>40793</v>
       </c>
-      <c r="AH71" s="12">
+      <c r="AI70" s="12">
         <f t="shared" si="1"/>
         <v>40794</v>
       </c>
-      <c r="AI71" s="12">
+      <c r="AJ70" s="12">
         <f t="shared" si="1"/>
         <v>40795</v>
       </c>
-      <c r="AJ71" s="12">
+      <c r="AK70" s="12">
         <f t="shared" si="1"/>
         <v>40796</v>
       </c>
-      <c r="AK71" s="12">
+      <c r="AL70" s="12">
         <f t="shared" si="1"/>
         <v>40797</v>
       </c>
-      <c r="AL71" s="12">
+      <c r="AM70" s="12">
         <f t="shared" si="1"/>
         <v>40798</v>
       </c>
-      <c r="AM71" s="12">
+      <c r="AN70" s="12">
         <f t="shared" si="1"/>
         <v>40799</v>
       </c>
-      <c r="AN71" s="12">
+      <c r="AO70" s="12">
         <f t="shared" si="1"/>
         <v>40800</v>
       </c>
-      <c r="AO71" s="12">
+      <c r="AP70" s="12">
         <f t="shared" si="1"/>
         <v>40801</v>
       </c>
-      <c r="AP71" s="12">
+      <c r="AQ70" s="12">
         <f t="shared" si="1"/>
         <v>40802</v>
       </c>
-      <c r="AQ71" s="12">
+      <c r="AR70" s="12">
         <f t="shared" si="1"/>
         <v>40803</v>
       </c>
-      <c r="AR71" s="12">
+      <c r="AS70" s="12">
         <f t="shared" si="1"/>
         <v>40804</v>
       </c>
-      <c r="AS71" s="12">
+      <c r="AT70" s="12">
         <f t="shared" si="1"/>
         <v>40805</v>
       </c>
-      <c r="AT71" s="12">
+      <c r="AU70" s="12">
         <f t="shared" si="1"/>
         <v>40806</v>
       </c>
-      <c r="AU71" s="12">
+      <c r="AV70" s="12">
         <f t="shared" si="1"/>
         <v>40807</v>
       </c>
-      <c r="AV71" s="12">
+      <c r="AW70" s="12">
         <f t="shared" si="1"/>
         <v>40808</v>
       </c>
-      <c r="AW71" s="12">
+      <c r="AX70" s="12">
         <f t="shared" si="1"/>
         <v>40809</v>
       </c>
-      <c r="AX71" s="12">
+      <c r="AY70" s="12">
         <f t="shared" si="1"/>
         <v>40810</v>
       </c>
-      <c r="AY71" s="12">
+      <c r="AZ70" s="12">
         <f t="shared" si="1"/>
         <v>40811</v>
       </c>
-      <c r="AZ71" s="12">
+      <c r="BA70" s="12">
         <f t="shared" si="1"/>
         <v>40812</v>
       </c>
-      <c r="BA71" s="12">
+      <c r="BB70" s="12">
         <f t="shared" si="1"/>
         <v>40813</v>
       </c>
-      <c r="BB71" s="12">
+      <c r="BC70" s="12">
         <f t="shared" si="1"/>
         <v>40814</v>
       </c>
-      <c r="BC71" s="12">
+      <c r="BD70" s="12">
         <f t="shared" si="1"/>
         <v>40815</v>
       </c>
-      <c r="BD71" s="12">
+      <c r="BE70" s="12">
         <f t="shared" si="1"/>
         <v>40816</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A10:BD71">
+  <autoFilter ref="A10:BE70">
+    <filterColumn colId="3"/>
     <filterColumn colId="4"/>
     <filterColumn colId="7"/>
+    <filterColumn colId="9"/>
   </autoFilter>
-  <conditionalFormatting sqref="J57:BD67 J11:BD13 J29:BD38 J40:BD49 J17:BD27 J51:BD55 J57:AW68 J15:BD15">
+  <conditionalFormatting sqref="K56:BE66 K50:BE54 K56:AX67 K11:BE13 K29:BE38 K40:BE48 K17:BE27 K15:BE15">
     <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
       <formula>"-"</formula>
     </cfRule>
@@ -5807,12 +5913,12 @@
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:BD13 J29:BD38 J40:BD49 J17:BD27 J51:BD55 J57:BD67 J15:BD15">
+  <conditionalFormatting sqref="K50:BE54 K56:BE66 K11:BE13 K29:BE38 K40:BE48 K17:BE27 K15:BE15">
     <cfRule type="cellIs" dxfId="2" priority="21" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H13 H15 H17:H27 H29:H38 H40:H49 H51:H55 H57:H67">
+  <conditionalFormatting sqref="H50:H54 H56:H66 H11:H13 H15 H17:H27 H29:H38 H40:H48">
     <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>$F$4</formula>
     </cfRule>
@@ -5821,7 +5927,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:H13 H57 H51:H55 H17:H27 H29:H38 H40:H49 H15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H56 H50:H54 H15 H40:H48 H29:H38 H17:H27 H11:H13">
       <formula1>$F$2:$F$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>